<commit_message>
WIP loco consist fragments
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6710EE-4598-455D-BBFA-7ACE70B26020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C9485F-588F-4B0A-93C4-33705E92D8D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6967" yWindow="3233" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6488" yWindow="2048" windowWidth="14400" windowHeight="7484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="159">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -379,6 +379,168 @@
   </si>
   <si>
     <t>_frag 193 Groen</t>
+  </si>
+  <si>
+    <t>_frag UNIMAT</t>
+  </si>
+  <si>
+    <t>verwijst naar ander materieel</t>
+  </si>
+  <si>
+    <t>_frag Windhoff</t>
+  </si>
+  <si>
+    <t>_frag Mosi</t>
+  </si>
+  <si>
+    <t>_frag 189 MRCE</t>
+  </si>
+  <si>
+    <t>_frag Sik Kraan</t>
+  </si>
+  <si>
+    <t>_frag Sik</t>
+  </si>
+  <si>
+    <t>_frag 1100</t>
+  </si>
+  <si>
+    <t>_frag 1200 Turquoise</t>
+  </si>
+  <si>
+    <t>TODO verwijst nu naar ander materieel</t>
+  </si>
+  <si>
+    <t>_frag 1200 RoodGeel</t>
+  </si>
+  <si>
+    <t>_frag 1200 RailExperts</t>
+  </si>
+  <si>
+    <t>_frag 1200 Railpromo</t>
+  </si>
+  <si>
+    <t>_frag 1200 BruinGeel</t>
+  </si>
+  <si>
+    <t>_frag 1200 BlauwGeel</t>
+  </si>
+  <si>
+    <t>_frag 1300 Bruin</t>
+  </si>
+  <si>
+    <t>_frag 1300 Blauw</t>
+  </si>
+  <si>
+    <t>_frag 186 Grijs</t>
+  </si>
+  <si>
+    <t>_frag 186 AkiemBlauw</t>
+  </si>
+  <si>
+    <t>_frag 186 Waverider</t>
+  </si>
+  <si>
+    <t>_frag 186 AkiemRood</t>
+  </si>
+  <si>
+    <t>_frag 186 AkiemPaars</t>
+  </si>
+  <si>
+    <t>_frag 186 RailpoolVlaggen299</t>
+  </si>
+  <si>
+    <t>_frag 186 RailpoolVlaggen551</t>
+  </si>
+  <si>
+    <t>_frag 2400</t>
+  </si>
+  <si>
+    <t>_frag 6000</t>
+  </si>
+  <si>
+    <t>_frag G1206</t>
+  </si>
+  <si>
+    <t>_frag G1206 GroenWegsleepdienst</t>
+  </si>
+  <si>
+    <t>_frag G2000 Blauw</t>
+  </si>
+  <si>
+    <t>_frag HLR77</t>
+  </si>
+  <si>
+    <t>_frag HLR77 NMBS</t>
+  </si>
+  <si>
+    <t>_frag 186 ATC-edrivers</t>
+  </si>
+  <si>
+    <t>_frag 186 Wit-WeAreInThisTogether</t>
+  </si>
+  <si>
+    <t>_frag 186 RailpoolBelgie</t>
+  </si>
+  <si>
+    <t>_frag 186 RailpoolKleuren</t>
+  </si>
+  <si>
+    <t>_frag 186 RailpoolLNSneus</t>
+  </si>
+  <si>
+    <t>_frag G1206 Zwart</t>
+  </si>
+  <si>
+    <t>verwijst naar ander materieel/kleurstelling</t>
+  </si>
+  <si>
+    <t>_frag V60 BTT</t>
+  </si>
+  <si>
+    <t>_frag 1700 Railpromo</t>
+  </si>
+  <si>
+    <t>_frag 186 Railpool200</t>
+  </si>
+  <si>
+    <t>_frag 186 286</t>
+  </si>
+  <si>
+    <t>_frag 186 AttracktiveConstantService</t>
+  </si>
+  <si>
+    <t>_frag 186 AttracktiveUnitingPower</t>
+  </si>
+  <si>
+    <t>_frag 186 AttracktiveJoiningPotential</t>
+  </si>
+  <si>
+    <t>_frag 186 AttracktiveFlowingEnergy</t>
+  </si>
+  <si>
+    <t>_frag 193 ELL-C2C</t>
+  </si>
+  <si>
+    <t>_frag 193 ELLFlyingDutchman</t>
+  </si>
+  <si>
+    <t>_frag 193 ELL</t>
+  </si>
+  <si>
+    <t>_frag 193 ELLecs-eurocargo</t>
+  </si>
+  <si>
+    <t>_frag 193 ELL-111Loreley</t>
+  </si>
+  <si>
+    <t>_frag 193 ELLKommZumZug</t>
+  </si>
+  <si>
+    <t>_frag HLD62 RXP</t>
+  </si>
+  <si>
+    <t>_frag 193 emob</t>
   </si>
 </sst>
 </file>
@@ -787,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160F4763-29B2-441E-803F-0A55BDF62DFC}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -864,10 +1026,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -875,72 +1037,75 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
@@ -948,7 +1113,7 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
@@ -956,7 +1121,7 @@
         <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -964,7 +1129,10 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -972,7 +1140,10 @@
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -980,7 +1151,7 @@
         <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>69</v>
@@ -988,29 +1159,29 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
         <v>69</v>
@@ -1018,21 +1189,21 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -1040,7 +1211,7 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -1048,7 +1219,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -1056,7 +1227,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -1064,7 +1235,10 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -1072,7 +1246,7 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -1080,15 +1254,15 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -1096,7 +1270,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -1104,7 +1278,10 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -1112,10 +1289,7 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -1123,7 +1297,10 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
@@ -1131,7 +1308,10 @@
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -1150,7 +1330,7 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
         <v>69</v>
@@ -1161,10 +1341,7 @@
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -1172,7 +1349,7 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
         <v>69</v>
@@ -1183,7 +1360,7 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
         <v>69</v>
@@ -1194,7 +1371,7 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
         <v>69</v>
@@ -1205,7 +1382,7 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
         <v>69</v>
@@ -1216,7 +1393,7 @@
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
         <v>69</v>
@@ -1227,7 +1404,7 @@
         <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
         <v>69</v>
@@ -1238,7 +1415,7 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C46" t="s">
         <v>69</v>
@@ -1249,15 +1426,656 @@
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" t="s">
-        <v>69</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" t="s">
+        <v>130</v>
+      </c>
+      <c r="C72" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" t="s">
+        <v>67</v>
+      </c>
+      <c r="C73" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76" t="s">
+        <v>67</v>
+      </c>
+      <c r="C76" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77" t="s">
+        <v>133</v>
+      </c>
+      <c r="C77" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A81" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A82" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A83" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A84" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A85" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A86" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A87" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" t="s">
+        <v>140</v>
+      </c>
+      <c r="C87" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A88" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A89" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A90" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A91" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A92" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A93" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93" t="s">
+        <v>143</v>
+      </c>
+      <c r="C93" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A94" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" t="s">
+        <v>147</v>
+      </c>
+      <c r="C96" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A97" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" t="s">
+        <v>150</v>
+      </c>
+      <c r="C97" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A98" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" t="s">
+        <v>149</v>
+      </c>
+      <c r="C98" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A99" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" t="s">
+        <v>148</v>
+      </c>
+      <c r="C99" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A100" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A101" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B101" t="s">
+        <v>145</v>
+      </c>
+      <c r="C101" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A102" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A103" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B103" t="s">
+        <v>155</v>
+      </c>
+      <c r="C103" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A104" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B104" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A105" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105" t="s">
+        <v>154</v>
+      </c>
+      <c r="C105" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A106" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B106" t="s">
+        <v>152</v>
+      </c>
+      <c r="C106" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A107" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B107" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A108" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A109" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B109" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A110" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B110" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A111" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B111" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A112" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112" t="s">
+        <v>157</v>
+      </c>
+      <c r="C112" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A113" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B113" t="s">
+        <v>80</v>
+      </c>
+      <c r="C113" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A114" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B114" t="s">
+        <v>158</v>
+      </c>
+      <c r="C114" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A115" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A116" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A117" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B117" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:I3" xr:uid="{C6458945-3F93-4C1E-9CBB-8941C5921D08}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I12">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I116">
       <sortCondition ref="A3"/>
     </sortState>
   </autoFilter>
@@ -1284,7 +2102,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
WIP initial attempt at container fragments
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C9485F-588F-4B0A-93C4-33705E92D8D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64237C2-65AA-4047-AA00-BFA7DD458196}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6488" yWindow="2048" windowWidth="14400" windowHeight="7484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21540" yWindow="3615" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -59,12 +59,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="B118" authorId="0" shapeId="0" xr:uid="{68CC567B-7BD4-46AA-923D-5195801C6DD2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dubbele containers: op volgorde van alfabet, dan omdraaien wanneer nodig!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B125" authorId="0" shapeId="0" xr:uid="{C88A422F-8223-48F7-9BD6-A55F1B7AA62A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+L: 2-assig</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="187">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -541,13 +589,97 @@
   </si>
   <si>
     <t>_frag 193 emob</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Leeg</t>
+  </si>
+  <si>
+    <t>Container 2x40ft HamburgSued</t>
+  </si>
+  <si>
+    <t>Container 2x40ft PnO</t>
+  </si>
+  <si>
+    <t>Container 2x40ft PnO-Safmarine</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Maersk</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Maersk-Safmarine</t>
+  </si>
+  <si>
+    <t>Container 2x40ft CAI-Maersk</t>
+  </si>
+  <si>
+    <t>Container 40ftL Leeg</t>
+  </si>
+  <si>
+    <t>Container 40ftL CMA</t>
+  </si>
+  <si>
+    <t>Container 2x40ft CMA</t>
+  </si>
+  <si>
+    <t>Container 2x40ft CMA-Rood20</t>
+  </si>
+  <si>
+    <t>Container 40ftL Rood</t>
+  </si>
+  <si>
+    <t>Container 40ftL EvergreenWit</t>
+  </si>
+  <si>
+    <t>Container 2x40ft EvergreenWit</t>
+  </si>
+  <si>
+    <t>Container 40ftL Wit</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Cosco-Wit</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Wit</t>
+  </si>
+  <si>
+    <t>Container 40ftL Maersk</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Leeg-Maersk</t>
+  </si>
+  <si>
+    <t>Container 2x40ft HamburgSued-Maersk</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Leeg-RoodHamburgSued</t>
+  </si>
+  <si>
+    <t>Container 2x40ft HamburgSued20-Maersk</t>
+  </si>
+  <si>
+    <t>Container 2x40ft RoodMaersk-Maersk</t>
+  </si>
+  <si>
+    <t>Container 2x40ft PnoMaersk-Maersk2x20</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Rood-Maersk2x20</t>
+  </si>
+  <si>
+    <t>Container 2x40ft Leeg-Rood</t>
+  </si>
+  <si>
+    <t>Container 40ftL Triton</t>
+  </si>
+  <si>
+    <t>Container 2x40ft</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,6 +715,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -949,16 +1094,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160F4763-29B2-441E-803F-0A55BDF62DFC}">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.86328125" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="35.19921875" customWidth="1"/>
     <col min="6" max="8" width="23.59765625" customWidth="1"/>
   </cols>
@@ -2071,6 +2216,284 @@
       </c>
       <c r="B117" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A118" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B118" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A119" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B119" t="s">
+        <v>160</v>
+      </c>
+      <c r="C119" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A120" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B120" t="s">
+        <v>161</v>
+      </c>
+      <c r="C120" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A121" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B121" t="s">
+        <v>162</v>
+      </c>
+      <c r="C121" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A122" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B122" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A123" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B123" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A124" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B124" t="s">
+        <v>165</v>
+      </c>
+      <c r="C124" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A125" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B125" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A126" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B126" t="s">
+        <v>167</v>
+      </c>
+      <c r="C126" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A127" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B127" t="s">
+        <v>169</v>
+      </c>
+      <c r="C127" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A128" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B128" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A129" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B129" t="s">
+        <v>170</v>
+      </c>
+      <c r="C129" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A130" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B130" t="s">
+        <v>171</v>
+      </c>
+      <c r="C130" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A131" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B131" t="s">
+        <v>172</v>
+      </c>
+      <c r="C131" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A132" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B132" t="s">
+        <v>173</v>
+      </c>
+      <c r="C132" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A133" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B133" t="s">
+        <v>174</v>
+      </c>
+      <c r="C133" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A134" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B134" t="s">
+        <v>175</v>
+      </c>
+      <c r="C134" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A135" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B135" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A136" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B136" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A137" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B137" t="s">
+        <v>178</v>
+      </c>
+      <c r="C137" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A138" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B138" t="s">
+        <v>179</v>
+      </c>
+      <c r="C138" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A139" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B139" t="s">
+        <v>180</v>
+      </c>
+      <c r="C139" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A140" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B140" t="s">
+        <v>181</v>
+      </c>
+      <c r="C140" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A141" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B141" t="s">
+        <v>182</v>
+      </c>
+      <c r="C141" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A142" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B142" t="s">
+        <v>183</v>
+      </c>
+      <c r="C142" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A143" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B143" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A144" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B144" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A145" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B145" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cargopaden backup voor nieuwe poging
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A6D1B4-47E4-4D7F-BF9B-DE1069069841}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48ACE96-2C53-41F5-9151-F600766FC8E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8295" yWindow="1058" windowWidth="14400" windowHeight="7484" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -83,6 +83,30 @@
     Zou problemen kunnen geven door omgekeerde voorste lok!
 Beantwoorden:
     Voor nu de driving engine index aangepast...</t>
+      </text>
+    </comment>
+    <comment ref="B164" authorId="0" shapeId="0" xr:uid="{3D6D54E2-E0B8-4E05-A053-51E524B02B3D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Talns</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -302,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="683">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2336,13 +2360,28 @@
   </si>
   <si>
     <t>30400 (zo)</t>
+  </si>
+  <si>
+    <t>Freight Wood, Freight Container</t>
+  </si>
+  <si>
+    <t>Zelflosser 4assig Dak</t>
+  </si>
+  <si>
+    <t>Jemelle KalkStaaltrein</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0FhOgYRZoE4</t>
+  </si>
+  <si>
+    <t>Jemelle KalkStaaltrein - 189 MRCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2384,6 +2423,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2799,10 +2851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160F4763-29B2-441E-803F-0A55BDF62DFC}">
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="D166" sqref="D166:I166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4293,6 +4345,9 @@
       <c r="F142" t="s">
         <v>501</v>
       </c>
+      <c r="H142" t="s">
+        <v>501</v>
+      </c>
       <c r="I142" t="s">
         <v>537</v>
       </c>
@@ -4313,6 +4368,9 @@
       <c r="F143" t="s">
         <v>501</v>
       </c>
+      <c r="H143" t="s">
+        <v>501</v>
+      </c>
       <c r="I143" t="s">
         <v>537</v>
       </c>
@@ -4387,6 +4445,9 @@
       <c r="F150" t="s">
         <v>504</v>
       </c>
+      <c r="H150" t="s">
+        <v>504</v>
+      </c>
       <c r="I150" t="s">
         <v>545</v>
       </c>
@@ -4407,6 +4468,9 @@
       <c r="F151" t="s">
         <v>504</v>
       </c>
+      <c r="H151" t="s">
+        <v>504</v>
+      </c>
       <c r="I151" t="s">
         <v>545</v>
       </c>
@@ -4585,6 +4649,9 @@
       <c r="F162" t="s">
         <v>503</v>
       </c>
+      <c r="H162" t="s">
+        <v>500</v>
+      </c>
       <c r="I162" t="s">
         <v>556</v>
       </c>
@@ -4605,8 +4672,62 @@
       <c r="F163" t="s">
         <v>503</v>
       </c>
+      <c r="H163" t="s">
+        <v>500</v>
+      </c>
       <c r="I163" t="s">
         <v>556</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A164" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B164" t="s">
+        <v>679</v>
+      </c>
+      <c r="C164" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A165" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B165" t="s">
+        <v>680</v>
+      </c>
+      <c r="D165">
+        <v>2021</v>
+      </c>
+      <c r="E165">
+        <v>2021</v>
+      </c>
+      <c r="H165" t="s">
+        <v>502</v>
+      </c>
+      <c r="I165" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A166" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B166" t="s">
+        <v>682</v>
+      </c>
+      <c r="D166">
+        <v>2021</v>
+      </c>
+      <c r="E166">
+        <v>2021</v>
+      </c>
+      <c r="H166" t="s">
+        <v>502</v>
+      </c>
+      <c r="I166" t="s">
+        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -5121,7 +5242,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5293,7 +5414,7 @@
       <c r="J5" s="20" t="s">
         <v>668</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="29" t="s">
         <v>501</v>
       </c>
     </row>
@@ -5351,7 +5472,7 @@
       <c r="J7" s="20" t="s">
         <v>665</v>
       </c>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="29" t="s">
         <v>502</v>
       </c>
     </row>
@@ -5413,7 +5534,7 @@
       <c r="J9" s="20" t="s">
         <v>663</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="29" t="s">
         <v>504</v>
       </c>
     </row>
@@ -5601,7 +5722,7 @@
       <c r="J15" s="20" t="s">
         <v>671</v>
       </c>
-      <c r="K15" s="28" t="s">
+      <c r="K15" s="29" t="s">
         <v>500</v>
       </c>
     </row>
@@ -5623,6 +5744,9 @@
       </c>
       <c r="F16" s="20" t="s">
         <v>435</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>678</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>429</v>
@@ -8628,10 +8752,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9459,6 +9583,22 @@
       </c>
       <c r="B59" s="3" t="s">
         <v>620</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>568</v>
+      </c>
+      <c r="D60" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>568</v>
+      </c>
+      <c r="D61" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -9480,7 +9620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE4165F-E7AD-4ECC-A1C6-FBF961B5A770}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Verwijder cargopaden, te onregelmatig
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48ACE96-2C53-41F5-9151-F600766FC8E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603582ED-F8EB-41F5-93C9-61C4B601564B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20122" yWindow="2528" windowWidth="14401" windowHeight="7485" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ZWNL-Treinseries" sheetId="11" r:id="rId4"/>
     <sheet name="HvN-Treinseries" sheetId="10" r:id="rId5"/>
     <sheet name="Treinseries" sheetId="12" r:id="rId6"/>
+    <sheet name="Cargopaden" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
@@ -26,10 +27,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HvN-Treinseries'!$A$1:$D$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL-Treinseries'!$A$1:$F$27</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -326,7 +336,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="688">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2375,6 +2385,21 @@
   </si>
   <si>
     <t>Jemelle KalkStaaltrein - 189 MRCE</t>
+  </si>
+  <si>
+    <t>Van</t>
+  </si>
+  <si>
+    <t>Naar</t>
+  </si>
+  <si>
+    <t>Sloe</t>
+  </si>
+  <si>
+    <t>Rsd</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -2497,7 +2522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2551,6 +2576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2853,7 +2879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160F4763-29B2-441E-803F-0A55BDF62DFC}">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+    <sheetView topLeftCell="A140" workbookViewId="0">
       <selection activeCell="D166" sqref="D166:I166"/>
     </sheetView>
   </sheetViews>
@@ -10339,4 +10365,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6798E9-F79F-4543-A759-7CBB17734CEF}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.46484375" customWidth="1"/>
+    <col min="3" max="3" width="3.86328125" customWidth="1"/>
+    <col min="4" max="4" width="25.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>685</v>
+      </c>
+      <c r="B2" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D4" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New attempt at cargopaden for trains in overzicht.xml
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603582ED-F8EB-41F5-93C9-61C4B601564B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B402816-E25D-480A-BFB8-849FDB891B65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20122" yWindow="2528" windowWidth="14401" windowHeight="7485" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7110" yWindow="3630" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -18,13 +18,12 @@
     <sheet name="Goederentreinen" sheetId="9" r:id="rId3"/>
     <sheet name="ZWNL-Treinseries" sheetId="11" r:id="rId4"/>
     <sheet name="HvN-Treinseries" sheetId="10" r:id="rId5"/>
-    <sheet name="Treinseries" sheetId="12" r:id="rId6"/>
-    <sheet name="Cargopaden" sheetId="13" r:id="rId7"/>
+    <sheet name="Scenarios" sheetId="14" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HvN-Treinseries'!$A$1:$D$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HvN-Treinseries'!$A$1:$F$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL-Treinseries'!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -150,6 +149,31 @@
           </rPr>
           <t xml:space="preserve">
 Consist typen toegewezen per *traject*! Ivm meer controle bij spawnen</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{45CB35E3-0618-477F-9865-B54BB3E51548}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+gemarkeerd als goederenpaden in drgl
+geel: moet nog controleren/fixen</t>
         </r>
       </text>
     </comment>
@@ -336,7 +360,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="659">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2051,39 +2075,6 @@
     <t>ICM, VIRM</t>
   </si>
   <si>
-    <t>ZWNL</t>
-  </si>
-  <si>
-    <t>ZvNL</t>
-  </si>
-  <si>
-    <t>HvNL</t>
-  </si>
-  <si>
-    <t>Zv-Ah-Ut-Asd</t>
-  </si>
-  <si>
-    <t>Ht-Ut-Asd</t>
-  </si>
-  <si>
-    <t>Ehv-Ht-Ut-Asd</t>
-  </si>
-  <si>
-    <t>Nightjet?</t>
-  </si>
-  <si>
-    <t>Ah-Ut-Asd</t>
-  </si>
-  <si>
-    <t>Ut-Hvs</t>
-  </si>
-  <si>
-    <t>Ut-Alm</t>
-  </si>
-  <si>
-    <t>Alm-Asd</t>
-  </si>
-  <si>
     <t>Max bak</t>
   </si>
   <si>
@@ -2093,105 +2084,24 @@
     <t>ICRmh ICD</t>
   </si>
   <si>
-    <t>Bd-Rtd-Asd</t>
-  </si>
-  <si>
-    <t>Rtd-Asd</t>
-  </si>
-  <si>
     <t>ICRmh</t>
   </si>
   <si>
-    <t>Bd-Rtd-Gv</t>
-  </si>
-  <si>
-    <t>1400 NN</t>
-  </si>
-  <si>
-    <t>Ut-Asd</t>
-  </si>
-  <si>
     <t>ICM, VIRM, SGM</t>
   </si>
   <si>
-    <t>Amf-Asd</t>
-  </si>
-  <si>
-    <t>Amf-Ut-Rtd</t>
-  </si>
-  <si>
-    <t>Dv-Ut-Rtd</t>
-  </si>
-  <si>
-    <t>Asd-Alm</t>
-  </si>
-  <si>
-    <t>Ddr-Bd</t>
-  </si>
-  <si>
-    <t>Zl-Ut-Rtd</t>
-  </si>
-  <si>
-    <t>Gv-Rtd-Rsd-Vs</t>
-  </si>
-  <si>
-    <t>Ddr-Rtd-Gv</t>
-  </si>
-  <si>
-    <t>Ut-Rtd</t>
-  </si>
-  <si>
-    <t>Nm-Ah-Ut-Asd</t>
-  </si>
-  <si>
-    <t>Rsd-Bd</t>
-  </si>
-  <si>
-    <t>Tb-Ht-Nm</t>
-  </si>
-  <si>
-    <t>Ht-Nm-Ah-Zp</t>
-  </si>
-  <si>
-    <t>Asd-Ut-Ht-Ehv</t>
-  </si>
-  <si>
-    <t>Asd-Ut-Ht</t>
-  </si>
-  <si>
     <t>SLT</t>
   </si>
   <si>
-    <t>Rtd-Gd</t>
-  </si>
-  <si>
-    <t>Rtd-Wd-Bkl-Asd</t>
-  </si>
-  <si>
     <t>SNG</t>
   </si>
   <si>
-    <t>Ehv-Ht</t>
-  </si>
-  <si>
-    <t>VIRM, SNG</t>
-  </si>
-  <si>
-    <t>Ut-Hvs-Alm</t>
-  </si>
-  <si>
     <t>SNG, SGM</t>
   </si>
   <si>
     <t>SNG, SLT</t>
   </si>
   <si>
-    <t>Brn-Ut</t>
-  </si>
-  <si>
-    <t>Zl-Ut</t>
-  </si>
-  <si>
     <t>10, 6</t>
   </si>
   <si>
@@ -2282,9 +2192,6 @@
     <t>0.7, 0.3</t>
   </si>
   <si>
-    <t>Arriva GTW-D</t>
-  </si>
-  <si>
     <t>Abellio FLIRT 5</t>
   </si>
   <si>
@@ -2387,19 +2294,85 @@
     <t>Jemelle KalkStaaltrein - 189 MRCE</t>
   </si>
   <si>
-    <t>Van</t>
-  </si>
-  <si>
-    <t>Naar</t>
-  </si>
-  <si>
-    <t>Sloe</t>
-  </si>
-  <si>
-    <t>Rsd</t>
-  </si>
-  <si>
-    <t>V</t>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>HvN</t>
+  </si>
+  <si>
+    <t>Player spawn</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Opstel</t>
+  </si>
+  <si>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>Altijd-Rood</t>
+  </si>
+  <si>
+    <t>git</t>
+  </si>
+  <si>
+    <t>3001 Ut-Ah</t>
+  </si>
+  <si>
+    <t>- Ut19
+- Klp
+- Ed</t>
+  </si>
+  <si>
+    <t>Ut:
+- 420 Ut241-&gt;14
+- 1700/11700 Ut9
+- 2900 Ut7
+- 3100 Ut5
+- 3501 Ut18
+- 4900/5701 Ut1
+- 6901 Ut21
+- 7401 Ut15
+- 8800/8801 Ut12
+Ut - Ed:
+- 800 Utvr-&gt;Ut7
+- 7400 Utza-&gt;Utvr
+- 100/120/220 Utza(2)-&gt;Ut5
+- 3000 Db-&gt;Bnk
+- 7300 Mrg-Db
+- 3100 Har-Mrn
+- 420 Har-&gt;Mrn(2)
+- 7400 Har
+- 100/120/220 Klp
+- 3000 Ed-&gt;Klp
+Ed:
+- 7500/7501 Ed1b
+- 31300/31301 Ed1a
+Ed-Ah:
+- 3100 Wf
+- 420 Otb-&gt;Wf
+- 7500 Ahwa-&gt;Otb
+- 3601 Ah7
+- 6600 Ah6a
+Ah:
+- 100/120/220 Ah-&gt;10-&gt;Ut
+- 3000 Ah11
+- 30900/30901 Ah6b
+- 31100 Ah4</t>
+  </si>
+  <si>
+    <t>AI Cargo</t>
+  </si>
+  <si>
+    <t>(geen)</t>
+  </si>
+  <si>
+    <t>Arriva GTW-D 2-8</t>
+  </si>
+  <si>
+    <t>Arriva GTW-D 2-6</t>
   </si>
 </sst>
 </file>
@@ -2463,7 +2436,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2500,6 +2473,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2522,7 +2501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2576,7 +2555,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2879,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160F4763-29B2-441E-803F-0A55BDF62DFC}">
   <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166:I166"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A167" sqref="A167:B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4710,7 +4710,7 @@
         <v>84</v>
       </c>
       <c r="B164" t="s">
-        <v>679</v>
+        <v>640</v>
       </c>
       <c r="C164" t="s">
         <v>105</v>
@@ -4721,7 +4721,7 @@
         <v>425</v>
       </c>
       <c r="B165" t="s">
-        <v>680</v>
+        <v>641</v>
       </c>
       <c r="D165">
         <v>2021</v>
@@ -4733,7 +4733,7 @@
         <v>502</v>
       </c>
       <c r="I165" t="s">
-        <v>681</v>
+        <v>642</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.45">
@@ -4741,7 +4741,7 @@
         <v>13</v>
       </c>
       <c r="B166" t="s">
-        <v>682</v>
+        <v>643</v>
       </c>
       <c r="D166">
         <v>2021</v>
@@ -4753,7 +4753,7 @@
         <v>502</v>
       </c>
       <c r="I166" t="s">
-        <v>681</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -5265,10 +5265,10 @@
   <dimension ref="A1:R156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5352,233 +5352,237 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>409</v>
+        <v>362</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>363</v>
       </c>
       <c r="E3" t="s">
-        <v>164</v>
+        <v>483</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>444</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>492</v>
+        <v>429</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>492</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>664</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>492</v>
+        <v>429</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>455</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>13</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>403</v>
+        <v>353</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>354</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>497</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>429</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>448</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>668</v>
+        <v>451</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>623</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>232</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>361</v>
+        <v>403</v>
+      </c>
+      <c r="D5" t="s">
+        <v>164</v>
       </c>
       <c r="E5" t="s">
-        <v>478</v>
+        <v>164</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>431</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>501</v>
+        <v>429</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>449</v>
-      </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="20" t="s">
-        <v>668</v>
-      </c>
-      <c r="K5" s="29" t="s">
+        <v>448</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>629</v>
+      </c>
+      <c r="K5" s="28" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="D6" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="E6" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>429</v>
+        <v>431</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>501</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>451</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>662</v>
-      </c>
-      <c r="K6" s="28" t="s">
-        <v>502</v>
+        <v>449</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="38" t="s">
+        <v>629</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>356</v>
+        <v>389</v>
       </c>
       <c r="D7" t="s">
-        <v>354</v>
+        <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>498</v>
+        <v>462</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>429</v>
+        <v>428</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>504</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>450</v>
       </c>
+      <c r="I7" s="28"/>
       <c r="J7" s="20" t="s">
-        <v>665</v>
+        <v>624</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>309</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>429</v>
+        <v>445</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>512</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>450</v>
-      </c>
+        <v>453</v>
+      </c>
+      <c r="I8" s="28"/>
       <c r="J8" s="20" t="s">
-        <v>670</v>
+        <v>630</v>
       </c>
       <c r="K8" s="28" t="s">
-        <v>511</v>
+        <v>634</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="D9" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="E9" t="s">
-        <v>462</v>
+        <v>164</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>428</v>
+        <v>444</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="H9" s="20" t="s">
         <v>450</v>
       </c>
-      <c r="I9" s="28"/>
+      <c r="I9" s="29" t="s">
+        <v>492</v>
+      </c>
       <c r="J9" s="20" t="s">
-        <v>663</v>
+        <v>625</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" t="s">
-        <v>462</v>
+        <v>489</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>445</v>
@@ -5587,201 +5591,197 @@
         <v>512</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I10" s="28"/>
       <c r="J10" s="20" t="s">
-        <v>669</v>
+        <v>625</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>673</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>319</v>
+        <v>259</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>382</v>
+        <v>356</v>
+      </c>
+      <c r="D11" t="s">
+        <v>354</v>
       </c>
       <c r="E11" t="s">
-        <v>471</v>
+        <v>498</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>438</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>503</v>
+        <v>429</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>429</v>
+        <v>450</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>666</v>
-      </c>
-      <c r="K11" s="28" t="s">
-        <v>503</v>
+        <v>626</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="E12" t="s">
-        <v>164</v>
+        <v>463</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>438</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>503</v>
+        <v>429</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>429</v>
+        <v>450</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>666</v>
+        <v>631</v>
       </c>
       <c r="K12" s="28" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>362</v>
+        <v>408</v>
       </c>
       <c r="D13" t="s">
-        <v>363</v>
+        <v>181</v>
       </c>
       <c r="E13" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>429</v>
+        <v>438</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>503</v>
       </c>
       <c r="H13" s="20" t="s">
         <v>429</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>455</v>
-      </c>
-      <c r="K13" s="28" t="s">
-        <v>506</v>
+        <v>632</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>322</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>398</v>
+        <v>342</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>512</v>
+        <v>639</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>452</v>
-      </c>
-      <c r="I14" s="28"/>
+        <v>429</v>
+      </c>
       <c r="J14" s="20" t="s">
-        <v>664</v>
+        <v>633</v>
       </c>
       <c r="K14" s="28" t="s">
-        <v>492</v>
+        <v>635</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>251</v>
+        <v>319</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>408</v>
-      </c>
-      <c r="D15" t="s">
-        <v>181</v>
+        <v>382</v>
       </c>
       <c r="E15" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="F15" s="20" t="s">
         <v>438</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="28" t="s">
         <v>503</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>429</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>671</v>
-      </c>
-      <c r="K15" s="29" t="s">
-        <v>500</v>
+        <v>627</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>342</v>
+        <v>386</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E16" t="s">
-        <v>481</v>
+        <v>164</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>678</v>
+        <v>503</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>429</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>672</v>
+        <v>627</v>
       </c>
       <c r="K16" s="28" t="s">
-        <v>674</v>
+        <v>503</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
@@ -7754,7 +7754,7 @@
         <v>429</v>
       </c>
       <c r="J86" s="20" t="s">
-        <v>667</v>
+        <v>628</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.45">
@@ -8320,7 +8320,7 @@
   </sheetData>
   <autoFilter ref="A2:R156" xr:uid="{86DEC163-0F38-4216-A6F4-B629FE360FF7}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R156">
-      <sortCondition ref="K2:K156"/>
+      <sortCondition ref="J2:J156"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:D57">
@@ -8356,16 +8356,16 @@
         <v>562</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>563</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>624</v>
+        <v>586</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>626</v>
+        <v>588</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -8373,13 +8373,13 @@
         <v>900</v>
       </c>
       <c r="B2" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>629</v>
+        <v>591</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -8387,13 +8387,13 @@
         <v>1000</v>
       </c>
       <c r="B3" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="C3">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>629</v>
+        <v>591</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -8401,13 +8401,13 @@
         <v>1100</v>
       </c>
       <c r="B4" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>630</v>
+        <v>592</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -8418,10 +8418,10 @@
         <v>564</v>
       </c>
       <c r="C5" t="s">
-        <v>623</v>
+        <v>585</v>
       </c>
       <c r="D5" t="s">
-        <v>631</v>
+        <v>593</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -8432,10 +8432,10 @@
         <v>564</v>
       </c>
       <c r="C6" t="s">
-        <v>623</v>
+        <v>585</v>
       </c>
       <c r="D6" t="s">
-        <v>631</v>
+        <v>593</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -8443,13 +8443,13 @@
         <v>4000</v>
       </c>
       <c r="B7" t="s">
-        <v>607</v>
+        <v>576</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>632</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -8463,10 +8463,10 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>633</v>
+        <v>595</v>
       </c>
       <c r="F8" t="s">
-        <v>635</v>
+        <v>597</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -8477,13 +8477,13 @@
         <v>560</v>
       </c>
       <c r="C9" t="s">
-        <v>622</v>
+        <v>584</v>
       </c>
       <c r="D9" t="s">
-        <v>633</v>
+        <v>595</v>
       </c>
       <c r="F9" t="s">
-        <v>636</v>
+        <v>598</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -8497,7 +8497,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>634</v>
+        <v>596</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -8513,7 +8513,7 @@
         <v>568</v>
       </c>
       <c r="D12" t="s">
-        <v>639</v>
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -8521,16 +8521,16 @@
         <v>5000</v>
       </c>
       <c r="B13" t="s">
-        <v>614</v>
+        <v>578</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>628</v>
+        <v>590</v>
       </c>
       <c r="F13" t="s">
-        <v>637</v>
+        <v>599</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -8538,16 +8538,16 @@
         <v>5100</v>
       </c>
       <c r="B14" t="s">
-        <v>614</v>
+        <v>578</v>
       </c>
       <c r="C14">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>628</v>
+        <v>590</v>
       </c>
       <c r="F14" t="s">
-        <v>637</v>
+        <v>599</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -8558,13 +8558,13 @@
         <v>558</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>618</v>
+        <v>580</v>
       </c>
       <c r="D15" t="s">
         <v>566</v>
       </c>
       <c r="E15" t="s">
-        <v>638</v>
+        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -8637,7 +8637,7 @@
         <v>500</v>
       </c>
       <c r="B20" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -8651,7 +8651,7 @@
         <v>600</v>
       </c>
       <c r="B21" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="C21">
         <v>7</v>
@@ -8668,7 +8668,7 @@
         <v>1900</v>
       </c>
       <c r="B22" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -8685,7 +8685,7 @@
         <v>2800</v>
       </c>
       <c r="B23" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="C23">
         <v>6</v>
@@ -8702,10 +8702,10 @@
         <v>9200</v>
       </c>
       <c r="B24" t="s">
-        <v>621</v>
+        <v>583</v>
       </c>
       <c r="D24" t="s">
-        <v>625</v>
+        <v>587</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
@@ -8713,10 +8713,10 @@
         <v>9600</v>
       </c>
       <c r="B25" t="s">
-        <v>621</v>
+        <v>583</v>
       </c>
       <c r="D25" t="s">
-        <v>625</v>
+        <v>587</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -8738,19 +8738,19 @@
         <v>5900</v>
       </c>
       <c r="B27" t="s">
-        <v>619</v>
+        <v>581</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>627</v>
+        <v>589</v>
       </c>
       <c r="E27">
         <v>80</v>
       </c>
       <c r="F27" t="s">
-        <v>637</v>
+        <v>599</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -8758,7 +8758,7 @@
         <v>7700</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>620</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -8781,7 +8781,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8799,590 +8799,629 @@
         <v>562</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>563</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>624</v>
+        <v>586</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>626</v>
+        <v>588</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>100</v>
+        <v>17800</v>
       </c>
       <c r="B2" t="s">
-        <v>548</v>
+        <v>657</v>
+      </c>
+      <c r="C2" t="s">
+        <v>585</v>
       </c>
       <c r="D2" t="s">
-        <v>633</v>
+        <v>592</v>
+      </c>
+      <c r="E2">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>120</v>
+        <v>30900</v>
       </c>
       <c r="B3" t="s">
-        <v>548</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
+        <v>657</v>
+      </c>
+      <c r="C3" t="s">
+        <v>584</v>
       </c>
       <c r="D3" t="s">
-        <v>633</v>
+        <v>592</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>140</v>
+        <v>31100</v>
       </c>
       <c r="B4" t="s">
-        <v>653</v>
+        <v>658</v>
+      </c>
+      <c r="C4" t="s">
+        <v>585</v>
       </c>
       <c r="D4" t="s">
-        <v>625</v>
+        <v>592</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>220</v>
+      <c r="A5" t="s">
+        <v>638</v>
       </c>
       <c r="B5" t="s">
-        <v>548</v>
+        <v>657</v>
+      </c>
+      <c r="C5" t="s">
+        <v>585</v>
       </c>
       <c r="D5" t="s">
-        <v>633</v>
+        <v>592</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>240</v>
+        <v>20000</v>
       </c>
       <c r="B6" t="s">
-        <v>653</v>
+        <v>610</v>
+      </c>
+      <c r="C6" t="s">
+        <v>585</v>
       </c>
       <c r="D6" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>400</v>
+        <v>30700</v>
       </c>
       <c r="B7" t="s">
-        <v>675</v>
+        <v>611</v>
+      </c>
+      <c r="C7" t="s">
+        <v>585</v>
       </c>
       <c r="D7" t="s">
-        <v>633</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>583</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
+        <v>548</v>
       </c>
       <c r="D8" t="s">
-        <v>565</v>
+        <v>595</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>600</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>583</v>
+        <v>548</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>565</v>
+        <v>595</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>700</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
-        <v>583</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
+        <v>548</v>
       </c>
       <c r="D10" t="s">
-        <v>565</v>
+        <v>595</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="B11" t="s">
-        <v>558</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
+        <v>636</v>
       </c>
       <c r="D11" t="s">
-        <v>566</v>
+        <v>595</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>1500</v>
+        <v>32200</v>
       </c>
       <c r="B12" t="s">
-        <v>591</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
+        <v>612</v>
+      </c>
+      <c r="C12" t="s">
+        <v>584</v>
       </c>
       <c r="D12" t="s">
-        <v>660</v>
-      </c>
-      <c r="F12" t="s">
-        <v>640</v>
+        <v>596</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>1600</v>
+        <v>31300</v>
       </c>
       <c r="B13" t="s">
-        <v>570</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
+        <v>613</v>
       </c>
       <c r="D13" t="s">
-        <v>656</v>
-      </c>
-      <c r="F13" t="s">
-        <v>641</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>1700</v>
+        <v>31400</v>
       </c>
       <c r="B14" t="s">
-        <v>570</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
+        <v>613</v>
       </c>
       <c r="D14" t="s">
-        <v>656</v>
-      </c>
-      <c r="F14" t="s">
-        <v>641</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>1800</v>
-      </c>
-      <c r="B15" t="s">
-        <v>583</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
+      <c r="A15" t="s">
+        <v>568</v>
       </c>
       <c r="D15" t="s">
-        <v>565</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>2000</v>
-      </c>
-      <c r="B16" t="s">
-        <v>583</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
+      <c r="A16" t="s">
+        <v>568</v>
       </c>
       <c r="D16" t="s">
-        <v>565</v>
+        <v>601</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>2400</v>
+        <v>4000</v>
       </c>
       <c r="B17" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>566</v>
+        <v>615</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>2600</v>
+        <v>4300</v>
       </c>
       <c r="B18" t="s">
-        <v>591</v>
+        <v>576</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>660</v>
-      </c>
-      <c r="F18" t="s">
-        <v>640</v>
+        <v>615</v>
+      </c>
+      <c r="E18">
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>2800</v>
+        <v>4900</v>
       </c>
       <c r="B19" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>565</v>
+        <v>615</v>
+      </c>
+      <c r="E19">
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>2900</v>
+        <v>5700</v>
       </c>
       <c r="B20" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>566</v>
+        <v>615</v>
+      </c>
+      <c r="E20">
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="B21" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>566</v>
+        <v>615</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>3100</v>
+        <v>6900</v>
       </c>
       <c r="B22" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>566</v>
+        <v>615</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>3500</v>
+        <v>7300</v>
       </c>
       <c r="B23" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>566</v>
+        <v>615</v>
+      </c>
+      <c r="E23">
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>3600</v>
+        <v>7400</v>
       </c>
       <c r="B24" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>566</v>
+        <v>615</v>
+      </c>
+      <c r="E24">
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>676</v>
+      <c r="A25">
+        <v>14900</v>
       </c>
       <c r="B25" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="C25">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>566</v>
+        <v>615</v>
+      </c>
+      <c r="E25">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>3900</v>
+        <v>28300</v>
       </c>
       <c r="B26" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="C26">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>566</v>
+        <v>615</v>
+      </c>
+      <c r="E26">
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>4000</v>
+        <v>8800</v>
       </c>
       <c r="B27" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C27">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>654</v>
+        <v>616</v>
+      </c>
+      <c r="F27" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>4300</v>
+        <v>800</v>
       </c>
       <c r="B28" t="s">
-        <v>607</v>
+        <v>558</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>654</v>
+        <v>566</v>
+      </c>
+      <c r="E28">
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>4900</v>
+        <v>2400</v>
       </c>
       <c r="B29" t="s">
-        <v>607</v>
+        <v>558</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>654</v>
+        <v>566</v>
+      </c>
+      <c r="E29">
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>5500</v>
+        <v>2900</v>
       </c>
       <c r="B30" t="s">
-        <v>615</v>
+        <v>558</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>627</v>
-      </c>
-      <c r="F30" t="s">
-        <v>642</v>
+        <v>566</v>
+      </c>
+      <c r="E30">
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>5600</v>
+        <v>3000</v>
       </c>
       <c r="B31" t="s">
-        <v>610</v>
+        <v>558</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>5700</v>
+        <v>3100</v>
       </c>
       <c r="B32" t="s">
-        <v>607</v>
+        <v>558</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>654</v>
+        <v>566</v>
+      </c>
+      <c r="E32">
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>6000</v>
+        <v>3500</v>
       </c>
       <c r="B33" t="s">
-        <v>607</v>
+        <v>558</v>
       </c>
       <c r="C33">
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>654</v>
+        <v>566</v>
+      </c>
+      <c r="E33">
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>6500</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>620</v>
+        <v>3600</v>
+      </c>
+      <c r="B34" t="s">
+        <v>558</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>566</v>
+      </c>
+      <c r="E34">
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>6600</v>
+        <v>3900</v>
       </c>
       <c r="B35" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>657</v>
+        <v>566</v>
+      </c>
+      <c r="E35">
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>6900</v>
+      <c r="A36" t="s">
+        <v>637</v>
       </c>
       <c r="B36" t="s">
-        <v>607</v>
+        <v>558</v>
       </c>
       <c r="C36">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>654</v>
+        <v>566</v>
+      </c>
+      <c r="E36">
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>7000</v>
+        <v>500</v>
       </c>
       <c r="B37" t="s">
-        <v>610</v>
+        <v>572</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>7300</v>
+        <v>600</v>
       </c>
       <c r="B38" t="s">
-        <v>607</v>
+        <v>572</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>654</v>
+        <v>565</v>
+      </c>
+      <c r="E38">
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>7400</v>
+        <v>700</v>
       </c>
       <c r="B39" t="s">
-        <v>607</v>
+        <v>572</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>654</v>
+        <v>565</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>7500</v>
+        <v>1800</v>
       </c>
       <c r="B40" t="s">
-        <v>643</v>
+        <v>572</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>658</v>
-      </c>
-      <c r="F40" t="s">
-        <v>642</v>
+        <v>565</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>7600</v>
+        <v>2000</v>
       </c>
       <c r="B41" t="s">
-        <v>610</v>
+        <v>572</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>567</v>
+        <v>565</v>
+      </c>
+      <c r="E41">
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>8800</v>
+        <v>2800</v>
       </c>
       <c r="B42" t="s">
-        <v>644</v>
+        <v>572</v>
       </c>
       <c r="C42">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>655</v>
-      </c>
-      <c r="F42" t="s">
-        <v>642</v>
+        <v>565</v>
+      </c>
+      <c r="E42">
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
@@ -9390,247 +9429,304 @@
         <v>11600</v>
       </c>
       <c r="B43" t="s">
-        <v>645</v>
+        <v>607</v>
       </c>
       <c r="C43">
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>659</v>
+        <v>620</v>
+      </c>
+      <c r="E43">
+        <v>140</v>
       </c>
       <c r="F43" t="s">
-        <v>646</v>
+        <v>608</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>11700</v>
+        <v>1600</v>
       </c>
       <c r="B44" t="s">
         <v>570</v>
       </c>
       <c r="C44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>656</v>
+        <v>617</v>
+      </c>
+      <c r="E44">
+        <v>170</v>
       </c>
       <c r="F44" t="s">
-        <v>647</v>
+        <v>603</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>14600</v>
+        <v>1700</v>
       </c>
       <c r="B45" t="s">
-        <v>610</v>
+        <v>570</v>
       </c>
       <c r="C45">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>567</v>
+        <v>617</v>
+      </c>
+      <c r="E45">
+        <v>200</v>
+      </c>
+      <c r="F45" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>14900</v>
+        <v>11700</v>
       </c>
       <c r="B46" t="s">
-        <v>607</v>
+        <v>570</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>654</v>
+        <v>617</v>
+      </c>
+      <c r="E46">
+        <v>200</v>
+      </c>
+      <c r="F46" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>15600</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>620</v>
+        <v>1500</v>
+      </c>
+      <c r="B47" t="s">
+        <v>575</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>621</v>
+      </c>
+      <c r="E47">
+        <v>200</v>
+      </c>
+      <c r="F47" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
+        <v>2600</v>
+      </c>
+      <c r="B48" t="s">
+        <v>575</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>621</v>
+      </c>
+      <c r="E48">
+        <v>200</v>
+      </c>
+      <c r="F48" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>140</v>
+      </c>
+      <c r="B49" t="s">
+        <v>614</v>
+      </c>
+      <c r="D49" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>240</v>
+      </c>
+      <c r="B50" t="s">
+        <v>614</v>
+      </c>
+      <c r="D50" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>5600</v>
+      </c>
+      <c r="B51" t="s">
+        <v>577</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>567</v>
+      </c>
+      <c r="E51">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>7000</v>
+      </c>
+      <c r="B52" t="s">
+        <v>577</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>567</v>
+      </c>
+      <c r="E52">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>7600</v>
+      </c>
+      <c r="B53" t="s">
+        <v>577</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>567</v>
+      </c>
+      <c r="E53">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>14600</v>
+      </c>
+      <c r="B54" t="s">
+        <v>577</v>
+      </c>
+      <c r="C54">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55">
         <v>15800</v>
       </c>
-      <c r="B48" t="s">
-        <v>610</v>
-      </c>
-      <c r="C48">
+      <c r="B55" t="s">
+        <v>577</v>
+      </c>
+      <c r="C55">
         <v>8</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D55" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A49">
-        <v>17800</v>
-      </c>
-      <c r="B49" t="s">
-        <v>648</v>
-      </c>
-      <c r="C49" t="s">
-        <v>623</v>
-      </c>
-      <c r="D49" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50">
-        <v>20000</v>
-      </c>
-      <c r="B50" t="s">
-        <v>649</v>
-      </c>
-      <c r="C50" t="s">
-        <v>623</v>
-      </c>
-      <c r="D50" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <v>28300</v>
-      </c>
-      <c r="B51" t="s">
-        <v>607</v>
-      </c>
-      <c r="C51">
-        <v>6</v>
-      </c>
-      <c r="D51" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>677</v>
-      </c>
-      <c r="B52" t="s">
-        <v>648</v>
-      </c>
-      <c r="C52" t="s">
-        <v>623</v>
-      </c>
-      <c r="D52" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A53">
-        <v>30700</v>
-      </c>
-      <c r="B53" t="s">
-        <v>650</v>
-      </c>
-      <c r="C53" t="s">
-        <v>623</v>
-      </c>
-      <c r="D53" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A54">
-        <v>30900</v>
-      </c>
-      <c r="B54" t="s">
-        <v>648</v>
-      </c>
-      <c r="C54" t="s">
-        <v>622</v>
-      </c>
-      <c r="D54" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A55">
-        <v>31100</v>
-      </c>
-      <c r="B55" t="s">
-        <v>648</v>
-      </c>
-      <c r="C55" t="s">
-        <v>623</v>
-      </c>
-      <c r="D55" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>31300</v>
+        <v>5500</v>
       </c>
       <c r="B56" t="s">
-        <v>652</v>
+        <v>579</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+        <v>589</v>
+      </c>
+      <c r="E56">
+        <v>80</v>
+      </c>
+      <c r="F56" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>31400</v>
+        <v>6600</v>
       </c>
       <c r="B57" t="s">
-        <v>652</v>
+        <v>559</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58">
-        <v>32200</v>
+        <v>7500</v>
       </c>
       <c r="B58" t="s">
-        <v>651</v>
-      </c>
-      <c r="C58" t="s">
-        <v>622</v>
+        <v>605</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+        <v>619</v>
+      </c>
+      <c r="E58">
+        <v>80</v>
+      </c>
+      <c r="F58" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59">
+        <v>6500</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>15600</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
         <v>32300</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>568</v>
-      </c>
-      <c r="D60" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>568</v>
-      </c>
-      <c r="D61" t="s">
-        <v>492</v>
+      <c r="B61" s="3" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D59" xr:uid="{CC7F020C-C131-4AC1-A187-4250632EB997}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D59">
-      <sortCondition ref="A1:A59"/>
+  <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
+      <sortCondition ref="D1:D61"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
@@ -9643,777 +9739,72 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE4165F-E7AD-4ECC-A1C6-FBF961B5A770}">
-  <dimension ref="A1:F53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" customWidth="1"/>
-    <col min="4" max="4" width="12.9296875" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.19921875" customWidth="1"/>
+    <col min="1" max="1" width="9.06640625" style="32"/>
+    <col min="2" max="2" width="11.73046875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="9.06640625" style="32"/>
+    <col min="4" max="4" width="12.19921875" style="32" customWidth="1"/>
+    <col min="5" max="5" width="24.265625" style="32" customWidth="1"/>
+    <col min="6" max="6" width="24.1328125" style="37" customWidth="1"/>
+    <col min="7" max="16384" width="9.06640625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="31" t="s">
+        <v>644</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>549</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>582</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E2" t="s">
-        <v>578</v>
-      </c>
-      <c r="F2" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>120</v>
-      </c>
-      <c r="B3" t="s">
-        <v>548</v>
-      </c>
-      <c r="E3" t="s">
-        <v>578</v>
-      </c>
-      <c r="F3" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>150</v>
-      </c>
-      <c r="B5" t="s">
-        <v>548</v>
-      </c>
-      <c r="E5" t="s">
-        <v>576</v>
-      </c>
-      <c r="F5" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>220</v>
-      </c>
-      <c r="B6" t="s">
-        <v>548</v>
-      </c>
-      <c r="E6" t="s">
-        <v>578</v>
-      </c>
-      <c r="F6" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>250</v>
-      </c>
-      <c r="B8" t="s">
-        <v>548</v>
-      </c>
-      <c r="E8" t="s">
-        <v>576</v>
-      </c>
-      <c r="F8" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>420</v>
-      </c>
-      <c r="B10" t="s">
-        <v>577</v>
-      </c>
-      <c r="E10" t="s">
-        <v>578</v>
-      </c>
-      <c r="F10" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>500</v>
-      </c>
-      <c r="B11" t="s">
-        <v>570</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>579</v>
-      </c>
-      <c r="F11" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>600</v>
-      </c>
-      <c r="B12" t="s">
-        <v>570</v>
-      </c>
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>579</v>
-      </c>
-      <c r="F12" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>700</v>
-      </c>
-      <c r="B13" t="s">
-        <v>583</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>800</v>
-      </c>
-      <c r="B14" t="s">
-        <v>558</v>
-      </c>
-      <c r="C14">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>576</v>
-      </c>
-      <c r="F14" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>900</v>
-      </c>
-      <c r="B15" t="s">
-        <v>584</v>
-      </c>
-      <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>1000</v>
-      </c>
-      <c r="B16" t="s">
-        <v>584</v>
-      </c>
-      <c r="C16">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>1100</v>
-      </c>
-      <c r="B17" t="s">
-        <v>587</v>
-      </c>
-      <c r="C17">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>589</v>
-      </c>
-      <c r="B18" t="s">
-        <v>570</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>590</v>
-      </c>
-      <c r="F18" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>1500</v>
-      </c>
-      <c r="B19" t="s">
-        <v>591</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="F19" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>1600</v>
-      </c>
-      <c r="B20" t="s">
-        <v>570</v>
-      </c>
-      <c r="C20">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>1700</v>
-      </c>
-      <c r="B21" t="s">
-        <v>570</v>
-      </c>
-      <c r="C21">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>593</v>
-      </c>
-      <c r="F21" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>1800</v>
-      </c>
-      <c r="B22" t="s">
-        <v>570</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>1900</v>
-      </c>
-      <c r="B23" t="s">
-        <v>583</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>2000</v>
-      </c>
-      <c r="B24" t="s">
-        <v>583</v>
-      </c>
-      <c r="C24">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>593</v>
-      </c>
-      <c r="F24" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>2100</v>
-      </c>
-      <c r="B25" t="s">
-        <v>558</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>2200</v>
-      </c>
-      <c r="B26" t="s">
-        <v>558</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>2400</v>
-      </c>
-      <c r="B27" t="s">
-        <v>558</v>
-      </c>
-      <c r="C27">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>599</v>
-      </c>
-      <c r="F27" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>2600</v>
-      </c>
-      <c r="B28" t="s">
-        <v>591</v>
-      </c>
-      <c r="C28">
-        <v>7</v>
-      </c>
-      <c r="F28" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>2800</v>
-      </c>
-      <c r="B29" t="s">
-        <v>583</v>
-      </c>
-      <c r="C29">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>600</v>
-      </c>
-      <c r="F29" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30">
-        <v>2900</v>
-      </c>
-      <c r="B30" t="s">
-        <v>558</v>
-      </c>
-      <c r="C30">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>576</v>
-      </c>
-      <c r="F30" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31">
-        <v>3000</v>
-      </c>
-      <c r="B31" t="s">
-        <v>558</v>
-      </c>
-      <c r="C31">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
-        <v>578</v>
-      </c>
-      <c r="F31" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32">
-        <v>3100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>558</v>
-      </c>
-      <c r="C32">
-        <v>10</v>
-      </c>
-      <c r="E32" t="s">
-        <v>578</v>
-      </c>
-      <c r="F32" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35">
-        <v>3500</v>
-      </c>
-      <c r="B35" t="s">
-        <v>558</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-      <c r="E35" t="s">
-        <v>576</v>
-      </c>
-      <c r="F35" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>3600</v>
-      </c>
-      <c r="B36" t="s">
-        <v>558</v>
-      </c>
-      <c r="C36">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>602</v>
-      </c>
-      <c r="E36" t="s">
-        <v>603</v>
-      </c>
-      <c r="F36" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37">
-        <v>3700</v>
-      </c>
-      <c r="B37" t="s">
-        <v>558</v>
-      </c>
-      <c r="C37">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>599</v>
-      </c>
-      <c r="E37" t="s">
-        <v>605</v>
-      </c>
-      <c r="F37" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39">
-        <v>3900</v>
-      </c>
-      <c r="B39" t="s">
-        <v>558</v>
-      </c>
-      <c r="C39">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>605</v>
-      </c>
-      <c r="F39" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40">
-        <v>4000</v>
-      </c>
-      <c r="B40" t="s">
-        <v>607</v>
-      </c>
-      <c r="C40">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>608</v>
-      </c>
-      <c r="F40" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>4300</v>
-      </c>
-      <c r="B41" t="s">
-        <v>610</v>
-      </c>
-      <c r="C41">
-        <v>6</v>
-      </c>
-      <c r="F41" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42">
-        <v>4400</v>
-      </c>
-      <c r="B42" t="s">
-        <v>559</v>
-      </c>
-      <c r="C42">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>4500</v>
-      </c>
-      <c r="B43" t="s">
-        <v>612</v>
-      </c>
-      <c r="C43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>4600</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45">
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46">
-        <v>4900</v>
-      </c>
-      <c r="B46" t="s">
-        <v>607</v>
-      </c>
-      <c r="C46">
-        <v>8</v>
-      </c>
-      <c r="E46" t="s">
-        <v>579</v>
-      </c>
-      <c r="F46" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47">
-        <v>5000</v>
-      </c>
-      <c r="B47" t="s">
-        <v>614</v>
-      </c>
-      <c r="C47">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <v>5100</v>
-      </c>
-      <c r="B48" t="s">
-        <v>614</v>
-      </c>
-      <c r="C48">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49">
-        <v>5200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50">
-        <v>5300</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52">
-        <v>5500</v>
-      </c>
-      <c r="B52" t="s">
-        <v>615</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
-      </c>
-      <c r="E52" t="s">
-        <v>616</v>
-      </c>
-      <c r="F52" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53">
-        <v>5600</v>
-      </c>
-      <c r="B53" t="s">
-        <v>610</v>
-      </c>
-      <c r="C53">
-        <v>10</v>
-      </c>
-      <c r="F53" t="s">
-        <v>617</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6798E9-F79F-4543-A759-7CBB17734CEF}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="6.46484375" customWidth="1"/>
-    <col min="3" max="3" width="3.86328125" customWidth="1"/>
-    <col min="4" max="4" width="25.86328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>683</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>684</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>687</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>685</v>
-      </c>
-      <c r="B2" t="s">
-        <v>686</v>
-      </c>
-      <c r="C2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="D4" s="31"/>
+      <c r="C1" s="31" t="s">
+        <v>651</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>646</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>655</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>648</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>649</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="32" t="s">
+        <v>645</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>652</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>653</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>654</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>656</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5500] AI traffic till Ut
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF9CEDB-5C1F-4991-8486-B734B32CD21C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DB771B-ABD0-4A16-937A-1F8025C286DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5535" yWindow="4755" windowWidth="14400" windowHeight="7485" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5535" yWindow="4755" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -456,7 +456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="727">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2648,6 +2648,22 @@
   <si>
     <t>- Brn
 - St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brn - Dld:
+- 1600/11600 ri Shl
+- 5501 Stz-&gt;St
+Dld - Ut:
+- 1700/11700 Dld ri Ut
+- 1701/11701 Bhv
+- 5501 Blo
+- 5700 Uto
+- 501/601 Ut-&gt;Uto
+- 2001 Ut-&gt;Uto (2)
+- 5601 Ut
+- 14900 Ut1
+Ut:
+- </t>
   </si>
 </sst>
 </file>
@@ -2784,7 +2800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2862,6 +2878,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5753,8 +5772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10232,7 +10251,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10305,7 +10324,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="199.5" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
         <v>644</v>
       </c>
@@ -10317,6 +10336,9 @@
       </c>
       <c r="E3" s="40" t="s">
         <v>725</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[5500] Finish AI traffic
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DB771B-ABD0-4A16-937A-1F8025C286DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE2211B-F9B2-416B-B0B2-7D43F77D954E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5535" yWindow="4755" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2650,7 +2650,8 @@
 - St</t>
   </si>
   <si>
-    <t xml:space="preserve">Brn - Dld:
+    <r>
+      <t xml:space="preserve">Brn - Dld:
 - 1600/11600 ri Shl
 - 5501 Stz-&gt;St
 Dld - Ut:
@@ -2661,9 +2662,38 @@
 - 501/601 Ut-&gt;Uto
 - 2001 Ut-&gt;Uto (2)
 - 5601 Ut
-- 14900 Ut1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- 14900 Ut1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Ut:
-- </t>
+- 420 Ut14
+- 1700/11700 Ut9
+- 3100 Ut5
+- 4900 Ut1
+- 7401 Utzl
+- 8800 Ut12
+- 28300/28301 Ut2
+- 2900 Ut7</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2800,7 +2830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2878,9 +2908,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5772,8 +5799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10251,7 +10278,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10324,7 +10351,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
         <v>644</v>
       </c>
@@ -10337,7 +10364,7 @@
       <c r="E3" s="40" t="s">
         <v>725</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="38" t="s">
         <v>726</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[5500] Timers and small fixes
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE2211B-F9B2-416B-B0B2-7D43F77D954E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6A7B31-E4BE-4A84-87B6-06CE91A5179F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5535" yWindow="4755" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4755" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -456,7 +456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="727">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2686,7 +2686,28 @@
       <t xml:space="preserve">
 Ut:
 - 420 Ut14
-- 1700/11700 Ut9
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- 1700/11700 Ut9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 - 3100 Ut5
 - 4900 Ut1
 - 7401 Utzl
@@ -5800,7 +5821,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5832,920 +5853,920 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>100</v>
+        <v>17800</v>
       </c>
       <c r="B2" t="s">
-        <v>547</v>
+        <v>651</v>
+      </c>
+      <c r="C2" t="s">
+        <v>584</v>
       </c>
       <c r="D2" t="s">
-        <v>594</v>
+        <v>591</v>
+      </c>
+      <c r="E2">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>120</v>
+        <v>30900</v>
       </c>
       <c r="B3" t="s">
-        <v>547</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
+        <v>651</v>
+      </c>
+      <c r="C3" t="s">
+        <v>583</v>
       </c>
       <c r="D3" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>140</v>
+        <v>31100</v>
       </c>
       <c r="B4" t="s">
-        <v>613</v>
+        <v>652</v>
+      </c>
+      <c r="C4" t="s">
+        <v>584</v>
       </c>
       <c r="D4" t="s">
-        <v>586</v>
+        <v>591</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>220</v>
+      <c r="A5" t="s">
+        <v>637</v>
       </c>
       <c r="B5" t="s">
-        <v>547</v>
+        <v>651</v>
+      </c>
+      <c r="C5" t="s">
+        <v>584</v>
       </c>
       <c r="D5" t="s">
-        <v>594</v>
+        <v>591</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>240</v>
+        <v>20000</v>
       </c>
       <c r="B6" t="s">
-        <v>613</v>
+        <v>609</v>
+      </c>
+      <c r="C6" t="s">
+        <v>584</v>
       </c>
       <c r="D6" t="s">
-        <v>586</v>
+        <v>592</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>400</v>
+        <v>30700</v>
       </c>
       <c r="B7" t="s">
-        <v>635</v>
+        <v>610</v>
+      </c>
+      <c r="C7" t="s">
+        <v>584</v>
       </c>
       <c r="D7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>571</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
+        <v>547</v>
       </c>
       <c r="D8" t="s">
-        <v>564</v>
+        <v>594</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>600</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>571</v>
+        <v>547</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>564</v>
-      </c>
-      <c r="E9">
-        <v>250</v>
+        <v>594</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>700</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
-        <v>571</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
+        <v>547</v>
       </c>
       <c r="D10" t="s">
-        <v>564</v>
+        <v>594</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="B11" t="s">
-        <v>557</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
+        <v>635</v>
       </c>
       <c r="D11" t="s">
-        <v>565</v>
-      </c>
-      <c r="E11">
-        <v>230</v>
+        <v>594</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>1500</v>
+        <v>32200</v>
       </c>
       <c r="B12" t="s">
-        <v>574</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
+        <v>611</v>
+      </c>
+      <c r="C12" t="s">
+        <v>583</v>
       </c>
       <c r="D12" t="s">
-        <v>620</v>
-      </c>
-      <c r="E12">
-        <v>200</v>
-      </c>
-      <c r="F12" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>1600</v>
+        <v>31300</v>
       </c>
       <c r="B13" t="s">
-        <v>569</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
+        <v>612</v>
       </c>
       <c r="D13" t="s">
-        <v>616</v>
-      </c>
-      <c r="E13">
-        <v>170</v>
-      </c>
-      <c r="F13" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>1700</v>
+        <v>31400</v>
       </c>
       <c r="B14" t="s">
-        <v>569</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
+        <v>612</v>
       </c>
       <c r="D14" t="s">
-        <v>616</v>
-      </c>
-      <c r="E14">
-        <v>200</v>
-      </c>
-      <c r="F14" t="s">
-        <v>602</v>
+        <v>621</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>1800</v>
-      </c>
-      <c r="B15" t="s">
-        <v>571</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
+      <c r="A15" t="s">
+        <v>567</v>
       </c>
       <c r="D15" t="s">
-        <v>564</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>2000</v>
-      </c>
-      <c r="B16" t="s">
-        <v>571</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
+      <c r="A16" t="s">
+        <v>567</v>
       </c>
       <c r="D16" t="s">
-        <v>564</v>
-      </c>
-      <c r="E16">
-        <v>230</v>
+        <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>2400</v>
+        <v>4000</v>
       </c>
       <c r="B17" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>565</v>
-      </c>
-      <c r="E17">
-        <v>280</v>
+        <v>614</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>2600</v>
+        <v>4300</v>
       </c>
       <c r="B18" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="E18">
-        <v>200</v>
-      </c>
-      <c r="F18" t="s">
-        <v>601</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>2800</v>
+        <v>4900</v>
       </c>
       <c r="B19" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>564</v>
+        <v>614</v>
       </c>
       <c r="E19">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>2900</v>
+        <v>5700</v>
       </c>
       <c r="B20" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
       <c r="E20">
-        <v>170</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="B21" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>3100</v>
+        <v>6900</v>
       </c>
       <c r="B22" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>565</v>
-      </c>
-      <c r="E22">
-        <v>280</v>
+        <v>614</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>3500</v>
+        <v>7300</v>
       </c>
       <c r="B23" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
       <c r="E23">
-        <v>280</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>3600</v>
+        <v>7400</v>
       </c>
       <c r="B24" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
       <c r="E24">
-        <v>170</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>3900</v>
+        <v>14900</v>
       </c>
       <c r="B25" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C25">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
       <c r="E25">
-        <v>170</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>4000</v>
+        <v>28300</v>
       </c>
       <c r="B26" t="s">
         <v>575</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
         <v>614</v>
       </c>
+      <c r="E26">
+        <v>110</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>4300</v>
+        <v>8800</v>
       </c>
       <c r="B27" t="s">
-        <v>575</v>
+        <v>605</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>614</v>
-      </c>
-      <c r="E27">
-        <v>110</v>
+        <v>615</v>
+      </c>
+      <c r="F27" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>4900</v>
+        <v>800</v>
       </c>
       <c r="B28" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C28">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>614</v>
+        <v>565</v>
       </c>
       <c r="E28">
-        <v>150</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>5500</v>
+        <v>2400</v>
       </c>
       <c r="B29" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>588</v>
+        <v>565</v>
       </c>
       <c r="E29">
-        <v>80</v>
-      </c>
-      <c r="F29" t="s">
-        <v>603</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>5600</v>
+        <v>2900</v>
       </c>
       <c r="B30" t="s">
-        <v>576</v>
+        <v>557</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E30">
-        <v>80</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>5700</v>
+        <v>3000</v>
       </c>
       <c r="B31" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>614</v>
-      </c>
-      <c r="E31">
-        <v>110</v>
+        <v>565</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>6000</v>
+        <v>3100</v>
       </c>
       <c r="B32" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C32">
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>614</v>
+        <v>565</v>
+      </c>
+      <c r="E32">
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>6500</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>581</v>
+        <v>3500</v>
+      </c>
+      <c r="B33" t="s">
+        <v>557</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>565</v>
+      </c>
+      <c r="E33">
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>6600</v>
+        <v>3600</v>
       </c>
       <c r="B34" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>617</v>
+        <v>565</v>
+      </c>
+      <c r="E34">
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>6900</v>
+        <v>3900</v>
       </c>
       <c r="B35" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>614</v>
+        <v>565</v>
+      </c>
+      <c r="E35">
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>7000</v>
+      <c r="A36" t="s">
+        <v>636</v>
       </c>
       <c r="B36" t="s">
-        <v>576</v>
+        <v>557</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E36">
-        <v>80</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>7300</v>
+        <v>500</v>
       </c>
       <c r="B37" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>614</v>
-      </c>
-      <c r="E37">
-        <v>80</v>
+        <v>564</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>7400</v>
+        <v>600</v>
       </c>
       <c r="B38" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>614</v>
+        <v>564</v>
       </c>
       <c r="E38">
-        <v>110</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>7500</v>
+        <v>700</v>
       </c>
       <c r="B39" t="s">
-        <v>604</v>
+        <v>571</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>618</v>
-      </c>
-      <c r="E39">
-        <v>80</v>
-      </c>
-      <c r="F39" t="s">
-        <v>603</v>
+        <v>564</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>7600</v>
+        <v>1800</v>
       </c>
       <c r="B40" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>566</v>
-      </c>
-      <c r="E40">
-        <v>80</v>
+        <v>564</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>8800</v>
+        <v>2000</v>
       </c>
       <c r="B41" t="s">
-        <v>605</v>
+        <v>571</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>615</v>
-      </c>
-      <c r="F41" t="s">
-        <v>603</v>
+        <v>564</v>
+      </c>
+      <c r="E41">
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>11600</v>
+        <v>2800</v>
       </c>
       <c r="B42" t="s">
-        <v>606</v>
+        <v>571</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>619</v>
+        <v>564</v>
       </c>
       <c r="E42">
-        <v>140</v>
-      </c>
-      <c r="F42" t="s">
-        <v>607</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>11700</v>
+        <v>11600</v>
       </c>
       <c r="B43" t="s">
-        <v>569</v>
+        <v>606</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="E43">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="F43" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>14600</v>
+        <v>1600</v>
       </c>
       <c r="B44" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>566</v>
+        <v>616</v>
+      </c>
+      <c r="E44">
+        <v>170</v>
+      </c>
+      <c r="F44" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>14900</v>
+        <v>1700</v>
       </c>
       <c r="B45" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="E45">
-        <v>110</v>
+        <v>200</v>
+      </c>
+      <c r="F45" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>15600</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>581</v>
+        <v>11700</v>
+      </c>
+      <c r="B46" t="s">
+        <v>569</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>616</v>
+      </c>
+      <c r="E46">
+        <v>200</v>
+      </c>
+      <c r="F46" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>15800</v>
+        <v>1500</v>
       </c>
       <c r="B47" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>566</v>
+        <v>620</v>
+      </c>
+      <c r="E47">
+        <v>200</v>
+      </c>
+      <c r="F47" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>17800</v>
+        <v>2600</v>
       </c>
       <c r="B48" t="s">
-        <v>651</v>
-      </c>
-      <c r="C48" t="s">
-        <v>584</v>
+        <v>574</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>591</v>
+        <v>620</v>
       </c>
       <c r="E48">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+        <v>200</v>
+      </c>
+      <c r="F48" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>20000</v>
+        <v>140</v>
       </c>
       <c r="B49" t="s">
-        <v>609</v>
-      </c>
-      <c r="C49" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="D49" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>28300</v>
+        <v>240</v>
       </c>
       <c r="B50" t="s">
-        <v>575</v>
-      </c>
-      <c r="C50">
-        <v>6</v>
+        <v>613</v>
       </c>
       <c r="D50" t="s">
-        <v>614</v>
-      </c>
-      <c r="E50">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>30700</v>
+        <v>5600</v>
       </c>
       <c r="B51" t="s">
-        <v>610</v>
-      </c>
-      <c r="C51" t="s">
-        <v>584</v>
+        <v>576</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+        <v>566</v>
+      </c>
+      <c r="E51">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>30900</v>
+        <v>7000</v>
       </c>
       <c r="B52" t="s">
-        <v>651</v>
-      </c>
-      <c r="C52" t="s">
-        <v>583</v>
+        <v>576</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+        <v>566</v>
+      </c>
+      <c r="E52">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>31100</v>
+        <v>7600</v>
       </c>
       <c r="B53" t="s">
-        <v>652</v>
-      </c>
-      <c r="C53" t="s">
-        <v>584</v>
+        <v>576</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>591</v>
+        <v>566</v>
       </c>
       <c r="E53">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>31300</v>
+        <v>14600</v>
       </c>
       <c r="B54" t="s">
-        <v>612</v>
+        <v>576</v>
+      </c>
+      <c r="C54">
+        <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>31400</v>
+        <v>15800</v>
       </c>
       <c r="B55" t="s">
-        <v>612</v>
+        <v>576</v>
+      </c>
+      <c r="C55">
+        <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>32200</v>
+        <v>5500</v>
       </c>
       <c r="B56" t="s">
-        <v>611</v>
-      </c>
-      <c r="C56" t="s">
-        <v>583</v>
+        <v>578</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+        <v>588</v>
+      </c>
+      <c r="E56">
+        <v>80</v>
+      </c>
+      <c r="F56" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57">
+        <v>6600</v>
+      </c>
+      <c r="B57" t="s">
+        <v>558</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>7500</v>
+      </c>
+      <c r="B58" t="s">
+        <v>604</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>618</v>
+      </c>
+      <c r="E58">
+        <v>80</v>
+      </c>
+      <c r="F58" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>6500</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>15600</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61">
         <v>32300</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>581</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>637</v>
-      </c>
-      <c r="B58" t="s">
-        <v>651</v>
-      </c>
-      <c r="C58" t="s">
-        <v>584</v>
-      </c>
-      <c r="D58" t="s">
-        <v>591</v>
-      </c>
-      <c r="E58">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>636</v>
-      </c>
-      <c r="B59" t="s">
-        <v>557</v>
-      </c>
-      <c r="C59">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>565</v>
-      </c>
-      <c r="E59">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>567</v>
-      </c>
-      <c r="D60" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>567</v>
-      </c>
-      <c r="D61" t="s">
-        <v>600</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
-      <sortCondition ref="A1:A61"/>
+      <sortCondition ref="D1:D61"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
@@ -10323,13 +10344,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>644</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>717</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>716</v>
       </c>
       <c r="D2" s="33" t="s">
@@ -10361,11 +10382,20 @@
       <c r="C3" s="32" t="s">
         <v>723</v>
       </c>
+      <c r="D3" s="33" t="s">
+        <v>718</v>
+      </c>
       <c r="E3" s="40" t="s">
         <v>725</v>
       </c>
       <c r="F3" s="38" t="s">
         <v>726</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>721</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[141] Player spawn Hvs
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66D12A6-213C-423A-A379-CADF8541A898}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D3D49B-691B-41EA-B037-08D395E6152A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4755" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="729">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2858,7 +2858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2937,6 +2937,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -10310,7 +10313,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10430,8 +10433,11 @@
       <c r="B5" s="32">
         <v>140</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="42" t="s">
         <v>728</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[141] AI traffic WIP
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D3D49B-691B-41EA-B037-08D395E6152A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD71FF4-8301-4032-B00B-24C7A890DF71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4755" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="731">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2720,8 +2720,29 @@
     <t>https://www.youtube.com/watch?v=RRT-HCddLnk</t>
   </si>
   <si>
+    <t>- Hvs
+- Amf</t>
+  </si>
+  <si>
+    <t>Hvs - Amf:
+- 1600/11600 Hvs
+- G FC/FW/C8 Brn
+- 140/240/1500 Amf-Brn
+- 15800 Amf7
+Amf:
+- 501/601 Ut-Amf2-Zl
+- 31300/31301 Amf4b
+Amf - Apd:
+- 1600/1700/11600/11700 Amfa
+- 140/240 Hvl
+- 31300 Bnva
+Apd:
+- 140/240 Apd1
+- 17800/17801 Apd3</t>
+  </si>
+  <si>
     <t>Ams-Amf 2019: https://www.youtube.com/watch?v=KpwT0JuZboM
-Amf-Apd: https://www.youtube.com/watch?v=3qY8avX706c</t>
+Amf-Apd 1600: https://www.youtube.com/watch?v=3qY8avX706c</t>
   </si>
 </sst>
 </file>
@@ -2938,10 +2959,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5833,8 +5854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5866,920 +5887,920 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>17800</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>651</v>
-      </c>
-      <c r="C2" t="s">
-        <v>584</v>
+        <v>547</v>
       </c>
       <c r="D2" t="s">
-        <v>591</v>
-      </c>
-      <c r="E2">
-        <v>60</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>30900</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>651</v>
-      </c>
-      <c r="C3" t="s">
-        <v>583</v>
+        <v>547</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>31100</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>652</v>
-      </c>
-      <c r="C4" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="D4" t="s">
-        <v>591</v>
-      </c>
-      <c r="E4">
-        <v>60</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>637</v>
+      <c r="A5">
+        <v>220</v>
       </c>
       <c r="B5" t="s">
-        <v>651</v>
-      </c>
-      <c r="C5" t="s">
-        <v>584</v>
+        <v>547</v>
       </c>
       <c r="D5" t="s">
-        <v>591</v>
-      </c>
-      <c r="E5">
-        <v>60</v>
+        <v>594</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>20000</v>
+        <v>240</v>
       </c>
       <c r="B6" t="s">
-        <v>609</v>
-      </c>
-      <c r="C6" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
       <c r="D6" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>30700</v>
+        <v>400</v>
       </c>
       <c r="B7" t="s">
-        <v>610</v>
-      </c>
-      <c r="C7" t="s">
-        <v>584</v>
+        <v>635</v>
       </c>
       <c r="D7" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="B8" t="s">
-        <v>547</v>
+        <v>571</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>594</v>
+        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>120</v>
+        <v>600</v>
       </c>
       <c r="B9" t="s">
-        <v>547</v>
+        <v>571</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>594</v>
+        <v>564</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>220</v>
+        <v>700</v>
       </c>
       <c r="B10" t="s">
-        <v>547</v>
+        <v>571</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>594</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="B11" t="s">
-        <v>635</v>
+        <v>557</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>594</v>
+        <v>565</v>
+      </c>
+      <c r="E11">
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>32200</v>
+        <v>1500</v>
       </c>
       <c r="B12" t="s">
-        <v>611</v>
-      </c>
-      <c r="C12" t="s">
-        <v>583</v>
+        <v>574</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>595</v>
+        <v>620</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>31300</v>
+        <v>1600</v>
       </c>
       <c r="B13" t="s">
-        <v>612</v>
+        <v>569</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>621</v>
+        <v>616</v>
+      </c>
+      <c r="E13">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>31400</v>
+        <v>1700</v>
       </c>
       <c r="B14" t="s">
-        <v>612</v>
+        <v>569</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>621</v>
+        <v>616</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>567</v>
+      <c r="A15">
+        <v>1800</v>
+      </c>
+      <c r="B15" t="s">
+        <v>571</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>491</v>
+        <v>564</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>567</v>
+      <c r="A16">
+        <v>2000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>571</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>600</v>
+        <v>564</v>
+      </c>
+      <c r="E16">
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>4000</v>
+        <v>2400</v>
       </c>
       <c r="B17" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>614</v>
+        <v>565</v>
+      </c>
+      <c r="E17">
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>4300</v>
+        <v>2600</v>
       </c>
       <c r="B18" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>614</v>
+        <v>620</v>
       </c>
       <c r="E18">
-        <v>110</v>
+        <v>200</v>
+      </c>
+      <c r="F18" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>4900</v>
+        <v>2800</v>
       </c>
       <c r="B19" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>614</v>
+        <v>564</v>
       </c>
       <c r="E19">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>5700</v>
+        <v>2900</v>
       </c>
       <c r="B20" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>614</v>
+        <v>565</v>
       </c>
       <c r="E20">
-        <v>110</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="B21" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>614</v>
+        <v>565</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>6900</v>
+        <v>3100</v>
       </c>
       <c r="B22" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>614</v>
+        <v>565</v>
+      </c>
+      <c r="E22">
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>7300</v>
+        <v>3500</v>
       </c>
       <c r="B23" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>614</v>
+        <v>565</v>
       </c>
       <c r="E23">
-        <v>80</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>7400</v>
+        <v>3600</v>
       </c>
       <c r="B24" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>614</v>
+        <v>565</v>
       </c>
       <c r="E24">
-        <v>110</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>14900</v>
+        <v>3900</v>
       </c>
       <c r="B25" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C25">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>614</v>
+        <v>565</v>
       </c>
       <c r="E25">
-        <v>110</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>28300</v>
+        <v>4000</v>
       </c>
       <c r="B26" t="s">
         <v>575</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
         <v>614</v>
       </c>
-      <c r="E26">
-        <v>110</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>8800</v>
+        <v>4300</v>
       </c>
       <c r="B27" t="s">
-        <v>605</v>
+        <v>575</v>
       </c>
       <c r="C27">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>615</v>
-      </c>
-      <c r="F27" t="s">
-        <v>603</v>
+        <v>614</v>
+      </c>
+      <c r="E27">
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>800</v>
+        <v>4900</v>
       </c>
       <c r="B28" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C28">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>565</v>
+        <v>614</v>
       </c>
       <c r="E28">
-        <v>230</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>2400</v>
+        <v>5500</v>
       </c>
       <c r="B29" t="s">
-        <v>557</v>
+        <v>578</v>
       </c>
       <c r="C29">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>565</v>
+        <v>588</v>
       </c>
       <c r="E29">
-        <v>280</v>
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>2900</v>
+        <v>5600</v>
       </c>
       <c r="B30" t="s">
-        <v>557</v>
+        <v>576</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E30">
-        <v>170</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>3000</v>
+        <v>5700</v>
       </c>
       <c r="B31" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C31">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>565</v>
+        <v>614</v>
+      </c>
+      <c r="E31">
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>3100</v>
+        <v>6000</v>
       </c>
       <c r="B32" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C32">
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>565</v>
-      </c>
-      <c r="E32">
-        <v>280</v>
+        <v>614</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>3500</v>
-      </c>
-      <c r="B33" t="s">
-        <v>557</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
-        <v>565</v>
-      </c>
-      <c r="E33">
-        <v>280</v>
+        <v>6500</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>3600</v>
+        <v>6600</v>
       </c>
       <c r="B34" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>565</v>
-      </c>
-      <c r="E34">
-        <v>170</v>
+        <v>617</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>3900</v>
+        <v>6900</v>
       </c>
       <c r="B35" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>565</v>
-      </c>
-      <c r="E35">
-        <v>170</v>
+        <v>614</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>636</v>
+      <c r="A36">
+        <v>7000</v>
       </c>
       <c r="B36" t="s">
-        <v>557</v>
+        <v>576</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E36">
-        <v>170</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>500</v>
+        <v>7300</v>
       </c>
       <c r="B37" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>564</v>
+        <v>614</v>
+      </c>
+      <c r="E37">
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>600</v>
+        <v>7400</v>
       </c>
       <c r="B38" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="C38">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>564</v>
+        <v>614</v>
       </c>
       <c r="E38">
-        <v>250</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>700</v>
+        <v>7500</v>
       </c>
       <c r="B39" t="s">
-        <v>571</v>
+        <v>604</v>
       </c>
       <c r="C39">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>564</v>
+        <v>618</v>
+      </c>
+      <c r="E39">
+        <v>80</v>
+      </c>
+      <c r="F39" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>1800</v>
+        <v>7600</v>
       </c>
       <c r="B40" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="C40">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>564</v>
+        <v>566</v>
+      </c>
+      <c r="E40">
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>2000</v>
+        <v>8800</v>
       </c>
       <c r="B41" t="s">
-        <v>571</v>
+        <v>605</v>
       </c>
       <c r="C41">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>564</v>
-      </c>
-      <c r="E41">
-        <v>230</v>
+        <v>615</v>
+      </c>
+      <c r="F41" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>2800</v>
+        <v>11600</v>
       </c>
       <c r="B42" t="s">
-        <v>571</v>
+        <v>606</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>564</v>
+        <v>619</v>
       </c>
       <c r="E42">
-        <v>200</v>
+        <v>140</v>
+      </c>
+      <c r="F42" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>11600</v>
+        <v>11700</v>
       </c>
       <c r="B43" t="s">
-        <v>606</v>
+        <v>569</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E43">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="F43" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>1600</v>
+        <v>14600</v>
       </c>
       <c r="B44" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="C44">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>616</v>
-      </c>
-      <c r="E44">
-        <v>170</v>
-      </c>
-      <c r="F44" t="s">
-        <v>602</v>
+        <v>566</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>1700</v>
+        <v>14900</v>
       </c>
       <c r="B45" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="C45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E45">
-        <v>200</v>
-      </c>
-      <c r="F45" t="s">
-        <v>602</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
-        <v>11700</v>
-      </c>
-      <c r="B46" t="s">
-        <v>569</v>
-      </c>
-      <c r="C46">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>616</v>
-      </c>
-      <c r="E46">
-        <v>200</v>
-      </c>
-      <c r="F46" t="s">
-        <v>608</v>
+        <v>15600</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
-        <v>1500</v>
+        <v>15800</v>
       </c>
       <c r="B47" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>620</v>
-      </c>
-      <c r="E47">
-        <v>200</v>
-      </c>
-      <c r="F47" t="s">
-        <v>601</v>
+        <v>566</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
-        <v>2600</v>
+        <v>17800</v>
       </c>
       <c r="B48" t="s">
-        <v>574</v>
-      </c>
-      <c r="C48">
-        <v>7</v>
+        <v>651</v>
+      </c>
+      <c r="C48" t="s">
+        <v>584</v>
       </c>
       <c r="D48" t="s">
-        <v>620</v>
+        <v>591</v>
       </c>
       <c r="E48">
-        <v>200</v>
-      </c>
-      <c r="F48" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
-        <v>140</v>
+        <v>20000</v>
       </c>
       <c r="B49" t="s">
-        <v>613</v>
+        <v>609</v>
+      </c>
+      <c r="C49" t="s">
+        <v>584</v>
       </c>
       <c r="D49" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
-        <v>240</v>
+        <v>28300</v>
       </c>
       <c r="B50" t="s">
-        <v>613</v>
+        <v>575</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+        <v>614</v>
+      </c>
+      <c r="E50">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>5600</v>
+        <v>30700</v>
       </c>
       <c r="B51" t="s">
-        <v>576</v>
-      </c>
-      <c r="C51">
-        <v>4</v>
+        <v>610</v>
+      </c>
+      <c r="C51" t="s">
+        <v>584</v>
       </c>
       <c r="D51" t="s">
-        <v>566</v>
-      </c>
-      <c r="E51">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>7000</v>
+        <v>30900</v>
       </c>
       <c r="B52" t="s">
-        <v>576</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
+        <v>651</v>
+      </c>
+      <c r="C52" t="s">
+        <v>583</v>
       </c>
       <c r="D52" t="s">
-        <v>566</v>
-      </c>
-      <c r="E52">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
-        <v>7600</v>
+        <v>31100</v>
       </c>
       <c r="B53" t="s">
-        <v>576</v>
-      </c>
-      <c r="C53">
-        <v>4</v>
+        <v>652</v>
+      </c>
+      <c r="C53" t="s">
+        <v>584</v>
       </c>
       <c r="D53" t="s">
-        <v>566</v>
+        <v>591</v>
       </c>
       <c r="E53">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>14600</v>
+        <v>31300</v>
       </c>
       <c r="B54" t="s">
-        <v>576</v>
-      </c>
-      <c r="C54">
-        <v>8</v>
+        <v>612</v>
       </c>
       <c r="D54" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>15800</v>
+        <v>31400</v>
       </c>
       <c r="B55" t="s">
-        <v>576</v>
-      </c>
-      <c r="C55">
-        <v>8</v>
+        <v>612</v>
       </c>
       <c r="D55" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
-        <v>5500</v>
+        <v>32200</v>
       </c>
       <c r="B56" t="s">
-        <v>578</v>
-      </c>
-      <c r="C56">
-        <v>4</v>
+        <v>611</v>
+      </c>
+      <c r="C56" t="s">
+        <v>583</v>
       </c>
       <c r="D56" t="s">
-        <v>588</v>
-      </c>
-      <c r="E56">
-        <v>80</v>
-      </c>
-      <c r="F56" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>6600</v>
-      </c>
-      <c r="B57" t="s">
-        <v>558</v>
-      </c>
-      <c r="C57">
-        <v>7</v>
-      </c>
-      <c r="D57" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58">
-        <v>7500</v>
+        <v>32300</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>637</v>
       </c>
       <c r="B58" t="s">
-        <v>604</v>
-      </c>
-      <c r="C58">
-        <v>3</v>
+        <v>651</v>
+      </c>
+      <c r="C58" t="s">
+        <v>584</v>
       </c>
       <c r="D58" t="s">
-        <v>618</v>
+        <v>591</v>
       </c>
       <c r="E58">
-        <v>80</v>
-      </c>
-      <c r="F58" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59">
-        <v>6500</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A60">
-        <v>15600</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A61">
-        <v>32300</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>581</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>636</v>
+      </c>
+      <c r="B59" t="s">
+        <v>557</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>565</v>
+      </c>
+      <c r="E59">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>567</v>
+      </c>
+      <c r="D60" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>567</v>
+      </c>
+      <c r="D61" t="s">
+        <v>600</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
-      <sortCondition ref="D1:D61"/>
+      <sortCondition ref="A1:A61"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
@@ -7243,7 +7264,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J12" activeCellId="1" sqref="J7:J10 J12"/>
+      <selection pane="bottomRight" activeCell="J16" activeCellId="5" sqref="J9 J10 J13 J14 J15 J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10313,7 +10334,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10426,18 +10447,24 @@
         <v>727</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="228" x14ac:dyDescent="0.45">
       <c r="A5" s="32" t="s">
         <v>644</v>
       </c>
       <c r="B5" s="32">
         <v>140</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="41" t="s">
+        <v>730</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="E5" s="40" t="s">
         <v>728</v>
       </c>
-      <c r="E5" s="41" t="s">
-        <v>719</v>
+      <c r="F5" s="42" t="s">
+        <v>729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[141] Finish AI traffic
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD71FF4-8301-4032-B00B-24C7A890DF71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037F8C53-A270-4415-AD02-33D64C6FEEFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4755" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2724,6 +2724,10 @@
 - Amf</t>
   </si>
   <si>
+    <t>Ams-Amf 2019: https://www.youtube.com/watch?v=KpwT0JuZboM
+Amf-Apd 1600: https://www.youtube.com/watch?v=3qY8avX706c</t>
+  </si>
+  <si>
     <t>Hvs - Amf:
 - 1600/11600 Hvs
 - G FC/FW/C8 Brn
@@ -2734,15 +2738,11 @@
 - 31300/31301 Amf4b
 Amf - Apd:
 - 1600/1700/11600/11700 Amfa
-- 140/240 Hvl
+- 140/240/G-C8/FC Hvl
 - 31300 Bnva
 Apd:
 - 140/240 Apd1
 - 17800/17801 Apd3</t>
-  </si>
-  <si>
-    <t>Ams-Amf 2019: https://www.youtube.com/watch?v=KpwT0JuZboM
-Amf-Apd 1600: https://www.youtube.com/watch?v=3qY8avX706c</t>
   </si>
 </sst>
 </file>
@@ -7264,7 +7264,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J16" activeCellId="5" sqref="J9 J10 J13 J14 J15 J16"/>
+      <selection pane="bottomRight" activeCell="J14" activeCellId="3" sqref="J9 J10 J13 J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10334,7 +10334,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10455,7 +10455,7 @@
         <v>140</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>718</v>
@@ -10464,7 +10464,7 @@
         <v>728</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NS ICRmh stam fragments
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7FC02F-9E1E-4501-95FC-A0183038CCE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CE1371-8104-4E08-B750-C0C71091F80C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4755" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21533" yWindow="3420" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
-    <sheet name="HvN-Treinseries" sheetId="10" r:id="rId2"/>
-    <sheet name="ZWNL-Treinseries" sheetId="11" r:id="rId3"/>
+    <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId2"/>
+    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId3"/>
     <sheet name="Goederentreinen" sheetId="9" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="14" r:id="rId5"/>
     <sheet name="Vervoerders" sheetId="7" r:id="rId6"/>
+    <sheet name="ICRm" sheetId="17" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'HvN-Treinseries'!$A$1:$F$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL-Treinseries'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -307,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G35" authorId="0" shapeId="0" xr:uid="{C9986BBF-9545-4691-892A-183E1D4EC645}">
+    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{0E941315-59B3-40EF-882D-C9F16F01F9E7}">
       <text>
         <r>
           <rPr>
@@ -331,7 +332,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="G62" authorId="0" shapeId="0" xr:uid="{59F1FE70-1C64-4F63-A15B-1C12D9C09363}">
+    <comment ref="G56" authorId="0" shapeId="0" xr:uid="{C9986BBF-9545-4691-892A-183E1D4EC645}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Alleen spawnen Kfh-Zlw</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G57" authorId="0" shapeId="0" xr:uid="{59F1FE70-1C64-4F63-A15B-1C12D9C09363}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Alleen spawnen Kfh-Zlw</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G59" authorId="0" shapeId="0" xr:uid="{BEC6273B-35FA-45E8-A5C3-B3223C288195}">
       <text>
         <r>
           <rPr>
@@ -379,55 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G72" authorId="0" shapeId="0" xr:uid="{0E941315-59B3-40EF-882D-C9F16F01F9E7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Alleen spawnen Kfh-Zlw</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G74" authorId="0" shapeId="0" xr:uid="{BEC6273B-35FA-45E8-A5C3-B3223C288195}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Alleen spawnen Kfh-Zlw</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G77" authorId="0" shapeId="0" xr:uid="{E2216889-A549-462B-A882-FFC2A6FA641A}">
+    <comment ref="G76" authorId="0" shapeId="0" xr:uid="{E2216889-A549-462B-A882-FFC2A6FA641A}">
       <text>
         <r>
           <rPr>
@@ -456,7 +457,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="758">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2797,6 +2798,63 @@
 - 1600/11600 Brn
 Misc:
 - Blauwkapel: voor speler ivm 1701</t>
+  </si>
+  <si>
+    <t>Apmz10</t>
+  </si>
+  <si>
+    <t>Bpmbdez8</t>
+  </si>
+  <si>
+    <t>Bpmbdzf7</t>
+  </si>
+  <si>
+    <t>Bpmdz9</t>
+  </si>
+  <si>
+    <t>Bpmez10</t>
+  </si>
+  <si>
+    <t>Bpmz10</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B-eindrijtuig</t>
+  </si>
+  <si>
+    <t>Bf</t>
+  </si>
+  <si>
+    <t>BDs</t>
+  </si>
+  <si>
+    <t>Gvc-Ehv</t>
+  </si>
+  <si>
+    <t>B(f)</t>
+  </si>
+  <si>
+    <t>Amro</t>
+  </si>
+  <si>
+    <t>Asd-Bd</t>
+  </si>
+  <si>
+    <t>Bnl</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>zelfde als 16100</t>
   </si>
 </sst>
 </file>
@@ -3319,7 +3377,7 @@
   <dimension ref="A1:I219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C187" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="C209" sqref="C209"/>
@@ -5906,7 +5964,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6868,7 +6926,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7312,10 +7370,10 @@
   <dimension ref="A1:R156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J16" activeCellId="9" sqref="J3 J7 J8 J9 J10 J12 J13 J14 J15 J16"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7325,8 +7383,8 @@
     <col min="3" max="3" width="12.06640625" style="18" customWidth="1"/>
     <col min="4" max="4" width="31.796875" customWidth="1"/>
     <col min="5" max="5" width="24.19921875" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" customWidth="1"/>
+    <col min="6" max="6" width="17.53125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="22.86328125" customWidth="1"/>
     <col min="8" max="8" width="10.59765625" style="20" customWidth="1"/>
     <col min="9" max="9" width="10.59765625" customWidth="1"/>
     <col min="10" max="10" width="31.9296875" style="20" customWidth="1"/>
@@ -7399,459 +7457,442 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>361</v>
+        <v>408</v>
       </c>
       <c r="D3" t="s">
-        <v>362</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
-        <v>482</v>
+        <v>163</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>428</v>
+        <v>443</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>491</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>454</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>505</v>
+        <v>449</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>491</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>624</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>304</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>352</v>
+        <v>394</v>
       </c>
       <c r="D4" t="s">
-        <v>353</v>
+        <v>304</v>
       </c>
       <c r="E4" t="s">
-        <v>496</v>
+        <v>474</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>428</v>
+        <v>443</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>491</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="J4" s="34" t="s">
-        <v>622</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>501</v>
+        <v>428</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>20</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>461</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>428</v>
+        <v>427</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>503</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>447</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="I5" s="28"/>
       <c r="J5" s="34" t="s">
-        <v>628</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>500</v>
+        <v>623</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>280</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>360</v>
+        <v>40</v>
+      </c>
+      <c r="C6" s="18">
+        <v>44560</v>
+      </c>
+      <c r="D6" t="s">
+        <v>163</v>
       </c>
       <c r="E6" t="s">
-        <v>477</v>
+        <v>163</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>430</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>500</v>
+        <v>427</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>503</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>448</v>
-      </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="34" t="s">
-        <v>628</v>
-      </c>
-      <c r="K6" s="29" t="s">
-        <v>500</v>
+        <v>428</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>238</v>
+        <v>453</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>388</v>
-      </c>
-      <c r="D7" t="s">
-        <v>186</v>
+        <v>364</v>
       </c>
       <c r="E7" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="28" t="s">
         <v>503</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="I7" s="28"/>
-      <c r="J7" s="34" t="s">
-        <v>623</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>503</v>
+      <c r="J7" s="20" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>395</v>
-      </c>
-      <c r="D8" t="s">
-        <v>192</v>
+        <v>368</v>
       </c>
       <c r="E8" t="s">
-        <v>461</v>
+        <v>474</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="20" t="s">
-        <v>629</v>
-      </c>
-      <c r="K8" s="28" t="s">
-        <v>633</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>264</v>
+        <v>220</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="D9" t="s">
         <v>163</v>
       </c>
       <c r="E9" t="s">
-        <v>163</v>
+        <v>474</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>443</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>491</v>
+        <v>427</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>503</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>449</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>491</v>
+        <v>428</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>624</v>
-      </c>
-      <c r="K9" s="29" t="s">
-        <v>491</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>321</v>
+        <v>260</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="D10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E10" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>451</v>
-      </c>
-      <c r="I10" s="28"/>
+        <v>428</v>
+      </c>
       <c r="J10" s="20" t="s">
-        <v>624</v>
-      </c>
-      <c r="K10" s="28" t="s">
-        <v>491</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="D11" t="s">
-        <v>353</v>
+        <v>215</v>
       </c>
       <c r="E11" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>428</v>
+        <v>427</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>503</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>625</v>
-      </c>
-      <c r="K11" s="29" t="s">
-        <v>501</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>308</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>428</v>
+        <v>444</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>511</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>449</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="I12" s="28"/>
       <c r="J12" s="20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="K12" s="28" t="s">
-        <v>510</v>
+        <v>633</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>321</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="E13" t="s">
-        <v>465</v>
+        <v>488</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>502</v>
+        <v>444</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>511</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>428</v>
-      </c>
+        <v>451</v>
+      </c>
+      <c r="I13" s="28"/>
       <c r="J13" s="20" t="s">
-        <v>631</v>
-      </c>
-      <c r="K13" s="29" t="s">
-        <v>499</v>
+        <v>624</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>349</v>
       </c>
       <c r="E14" t="s">
-        <v>480</v>
+        <v>504</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>434</v>
+        <v>509</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>638</v>
+        <v>512</v>
       </c>
       <c r="H14" s="20" t="s">
         <v>428</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>632</v>
-      </c>
-      <c r="K14" s="28" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>381</v>
+        <v>374</v>
+      </c>
+      <c r="D15" t="s">
+        <v>183</v>
       </c>
       <c r="E15" t="s">
         <v>470</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>437</v>
+        <v>508</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>428</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>626</v>
-      </c>
-      <c r="K15" s="28" t="s">
-        <v>502</v>
+        <v>428</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>385</v>
+        <v>342</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>343</v>
       </c>
       <c r="E16" t="s">
-        <v>163</v>
+        <v>474</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>502</v>
+        <v>429</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>428</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>626</v>
-      </c>
-      <c r="K16" s="28" t="s">
-        <v>502</v>
+        <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>299</v>
+        <v>259</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>369</v>
+        <v>390</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="E17" t="s">
-        <v>180</v>
+        <v>469</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>492</v>
+        <v>445</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>510</v>
       </c>
       <c r="H17" s="20" t="s">
         <v>428</v>
@@ -7862,25 +7903,25 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="D18" t="s">
-        <v>347</v>
+        <v>163</v>
       </c>
       <c r="E18" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>430</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>500</v>
+        <v>432</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>501</v>
       </c>
       <c r="H18" s="20" t="s">
         <v>428</v>
@@ -7891,25 +7932,25 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>372</v>
+        <v>339</v>
       </c>
       <c r="D19" t="s">
-        <v>347</v>
+        <v>163</v>
       </c>
       <c r="E19" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H19" s="20" t="s">
         <v>428</v>
@@ -7920,25 +7961,22 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="18">
-        <v>44560</v>
-      </c>
-      <c r="D20" t="s">
-        <v>163</v>
+        <v>13</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>340</v>
       </c>
       <c r="E20" t="s">
         <v>163</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H20" s="20" t="s">
         <v>428</v>
@@ -7949,16 +7987,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>263</v>
+        <v>309</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="D21" t="s">
-        <v>163</v>
+        <v>373</v>
       </c>
       <c r="E21" t="s">
         <v>163</v>
@@ -7966,7 +8001,7 @@
       <c r="F21" s="20" t="s">
         <v>432</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="28" t="s">
         <v>501</v>
       </c>
       <c r="H21" s="20" t="s">
@@ -7978,13 +8013,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>307</v>
+        <v>249</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>339</v>
+        <v>399</v>
       </c>
       <c r="D22" t="s">
         <v>163</v>
@@ -8007,13 +8042,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>340</v>
+        <v>406</v>
+      </c>
+      <c r="D23" t="s">
+        <v>163</v>
       </c>
       <c r="E23" t="s">
         <v>163</v>
@@ -8033,13 +8071,16 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>309</v>
+        <v>222</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>373</v>
+        <v>411</v>
+      </c>
+      <c r="D24" t="s">
+        <v>163</v>
       </c>
       <c r="E24" t="s">
         <v>163</v>
@@ -8059,13 +8100,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="D25" t="s">
         <v>163</v>
@@ -8088,13 +8129,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>227</v>
+        <v>278</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="D26" t="s">
         <v>163</v>
@@ -8117,13 +8158,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>222</v>
+        <v>325</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="D27" t="s">
         <v>163</v>
@@ -8146,19 +8187,19 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="D28" t="s">
         <v>163</v>
       </c>
       <c r="E28" t="s">
-        <v>163</v>
+        <v>479</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>432</v>
@@ -8175,19 +8216,19 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>414</v>
+        <v>330</v>
       </c>
       <c r="D29" t="s">
         <v>163</v>
       </c>
       <c r="E29" t="s">
-        <v>163</v>
+        <v>474</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>432</v>
@@ -8204,19 +8245,19 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>325</v>
+        <v>272</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>416</v>
+        <v>332</v>
       </c>
       <c r="D30" t="s">
         <v>163</v>
       </c>
       <c r="E30" t="s">
-        <v>163</v>
+        <v>474</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>432</v>
@@ -8233,25 +8274,25 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="D31" t="s">
         <v>163</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>474</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="G31" s="28" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="H31" s="20" t="s">
         <v>428</v>
@@ -8262,22 +8303,25 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>359</v>
+        <v>387</v>
+      </c>
+      <c r="D32" t="s">
+        <v>163</v>
       </c>
       <c r="E32" t="s">
         <v>163</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>492</v>
+        <v>507</v>
       </c>
       <c r="H32" s="20" t="s">
         <v>428</v>
@@ -8288,25 +8332,25 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="D33" t="s">
         <v>163</v>
       </c>
       <c r="E33" t="s">
-        <v>163</v>
+        <v>474</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>492</v>
+        <v>507</v>
       </c>
       <c r="H33" s="20" t="s">
         <v>428</v>
@@ -8317,25 +8361,25 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>412</v>
+        <v>354</v>
       </c>
       <c r="D34" t="s">
         <v>163</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
+        <v>493</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>492</v>
+        <v>507</v>
       </c>
       <c r="H34" s="20" t="s">
         <v>428</v>
@@ -8346,25 +8390,25 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="E35" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="G35" s="28" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="H35" s="20" t="s">
         <v>428</v>
@@ -8375,22 +8419,22 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="D36" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="E36" t="s">
         <v>163</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>428</v>
+        <v>433</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>492</v>
       </c>
       <c r="H36" s="20" t="s">
         <v>428</v>
@@ -8401,25 +8445,25 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>282</v>
+        <v>240</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="D37" t="s">
         <v>163</v>
       </c>
       <c r="E37" t="s">
-        <v>479</v>
+        <v>163</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="H37" s="20" t="s">
         <v>428</v>
@@ -8430,19 +8474,19 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>289</v>
+        <v>242</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="D38" t="s">
         <v>163</v>
       </c>
       <c r="E38" t="s">
-        <v>479</v>
+        <v>163</v>
       </c>
       <c r="F38" s="20" t="s">
         <v>433</v>
@@ -8459,79 +8503,80 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>453</v>
+        <v>289</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>364</v>
+        <v>401</v>
+      </c>
+      <c r="D39" t="s">
+        <v>163</v>
       </c>
       <c r="E39" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>446</v>
-      </c>
-      <c r="I39" s="28"/>
+        <v>428</v>
+      </c>
       <c r="J39" s="20" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>297</v>
+        <v>268</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>368</v>
+        <v>337</v>
+      </c>
+      <c r="D40" t="s">
+        <v>163</v>
       </c>
       <c r="E40" t="s">
         <v>474</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="G40" s="28" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>446</v>
-      </c>
-      <c r="I40" s="28"/>
+        <v>428</v>
+      </c>
       <c r="J40" s="20" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>304</v>
+        <v>221</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>394</v>
-      </c>
-      <c r="D41" t="s">
-        <v>304</v>
+        <v>344</v>
       </c>
       <c r="E41" t="s">
         <v>474</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="H41" s="20" t="s">
         <v>428</v>
@@ -8542,13 +8587,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="D42" t="s">
         <v>163</v>
@@ -8557,10 +8602,10 @@
         <v>474</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="H42" s="20" t="s">
         <v>428</v>
@@ -8571,22 +8616,25 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>218</v>
+        <v>290</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>342</v>
+        <v>404</v>
       </c>
       <c r="D43" t="s">
-        <v>343</v>
+        <v>163</v>
       </c>
       <c r="E43" t="s">
         <v>474</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>429</v>
+        <v>433</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>492</v>
       </c>
       <c r="H43" s="20" t="s">
         <v>428</v>
@@ -8597,13 +8645,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>330</v>
+        <v>415</v>
       </c>
       <c r="D44" t="s">
         <v>163</v>
@@ -8612,10 +8660,10 @@
         <v>474</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G44" s="28" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="H44" s="20" t="s">
         <v>428</v>
@@ -8626,13 +8674,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>332</v>
+        <v>420</v>
       </c>
       <c r="D45" t="s">
         <v>163</v>
@@ -8641,10 +8689,10 @@
         <v>474</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="H45" s="20" t="s">
         <v>428</v>
@@ -8655,13 +8703,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>400</v>
+        <v>421</v>
       </c>
       <c r="D46" t="s">
         <v>163</v>
@@ -8670,10 +8718,10 @@
         <v>474</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G46" s="28" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="H46" s="20" t="s">
         <v>428</v>
@@ -8684,13 +8732,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>386</v>
+        <v>422</v>
       </c>
       <c r="D47" t="s">
         <v>163</v>
@@ -8699,10 +8747,10 @@
         <v>474</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="G47" s="28" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
       <c r="H47" s="20" t="s">
         <v>428</v>
@@ -8713,19 +8761,16 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>268</v>
+        <v>320</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>337</v>
-      </c>
-      <c r="D48" t="s">
-        <v>163</v>
+        <v>383</v>
       </c>
       <c r="E48" t="s">
-        <v>474</v>
+        <v>487</v>
       </c>
       <c r="F48" s="20" t="s">
         <v>433</v>
@@ -8740,18 +8785,21 @@
         <v>428</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>221</v>
+        <v>292</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>344</v>
+        <v>410</v>
+      </c>
+      <c r="D49" t="s">
+        <v>163</v>
       </c>
       <c r="E49" t="s">
-        <v>474</v>
+        <v>485</v>
       </c>
       <c r="F49" s="20" t="s">
         <v>433</v>
@@ -8766,21 +8814,18 @@
         <v>428</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>403</v>
-      </c>
-      <c r="D50" t="s">
-        <v>163</v>
+        <v>345</v>
       </c>
       <c r="E50" t="s">
-        <v>474</v>
+        <v>493</v>
       </c>
       <c r="F50" s="20" t="s">
         <v>433</v>
@@ -8795,21 +8840,21 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>290</v>
+        <v>458</v>
       </c>
       <c r="B51" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>404</v>
+        <v>419</v>
       </c>
       <c r="D51" t="s">
         <v>163</v>
       </c>
       <c r="E51" t="s">
-        <v>474</v>
+        <v>493</v>
       </c>
       <c r="F51" s="20" t="s">
         <v>433</v>
@@ -8824,21 +8869,21 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>283</v>
+        <v>323</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
       <c r="D52" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F52" s="20" t="s">
         <v>433</v>
@@ -8853,50 +8898,51 @@
         <v>428</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>420</v>
+        <v>350</v>
       </c>
       <c r="D53" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="E53" t="s">
-        <v>474</v>
+        <v>494</v>
       </c>
       <c r="F53" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="G53" s="28" t="s">
+      <c r="G53" s="29" t="s">
         <v>492</v>
       </c>
       <c r="H53" s="20" t="s">
-        <v>428</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="I53" s="28"/>
       <c r="J53" s="20" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>421</v>
+        <v>334</v>
       </c>
       <c r="D54" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="E54" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="F54" s="20" t="s">
         <v>433</v>
@@ -8911,21 +8957,21 @@
         <v>428</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>276</v>
+        <v>243</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>422</v>
+        <v>336</v>
       </c>
       <c r="D55" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="E55" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="F55" s="20" t="s">
         <v>433</v>
@@ -8940,24 +8986,27 @@
         <v>428</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>383</v>
+        <v>396</v>
+      </c>
+      <c r="D56" t="s">
+        <v>163</v>
       </c>
       <c r="E56" t="s">
-        <v>487</v>
+        <v>163</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="G56" s="28" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="H56" s="20" t="s">
         <v>428</v>
@@ -8966,27 +9015,27 @@
         <v>428</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="D57" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="E57" t="s">
-        <v>485</v>
+        <v>461</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="G57" s="28" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="H57" s="20" t="s">
         <v>428</v>
@@ -8995,53 +9044,56 @@
         <v>428</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="D58" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E58" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="G58" s="28" t="s">
-        <v>507</v>
+        <v>638</v>
       </c>
       <c r="H58" s="20" t="s">
         <v>428</v>
       </c>
       <c r="J58" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+        <v>632</v>
+      </c>
+      <c r="K58" s="28" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>225</v>
+        <v>313</v>
       </c>
       <c r="B59" t="s">
         <v>13</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>345</v>
+        <v>375</v>
       </c>
       <c r="E59" t="s">
-        <v>493</v>
+        <v>470</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>433</v>
+        <v>498</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="H59" s="20" t="s">
         <v>428</v>
@@ -9050,27 +9102,24 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>458</v>
+        <v>315</v>
       </c>
       <c r="B60" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>419</v>
-      </c>
-      <c r="D60" t="s">
-        <v>163</v>
+        <v>377</v>
       </c>
       <c r="E60" t="s">
-        <v>493</v>
+        <v>461</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="G60" s="28" t="s">
-        <v>492</v>
+        <v>505</v>
       </c>
       <c r="H60" s="20" t="s">
         <v>428</v>
@@ -9079,24 +9128,24 @@
         <v>428</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>226</v>
+        <v>316</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>335</v>
-      </c>
-      <c r="D61" t="s">
-        <v>163</v>
+        <v>378</v>
       </c>
       <c r="E61" t="s">
-        <v>495</v>
+        <v>461</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>428</v>
+        <v>436</v>
+      </c>
+      <c r="G61" s="28" t="s">
+        <v>505</v>
       </c>
       <c r="H61" s="20" t="s">
         <v>428</v>
@@ -9105,27 +9154,27 @@
         <v>428</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>296</v>
+        <v>253</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>393</v>
+        <v>431</v>
       </c>
       <c r="D62" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E62" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="G62" s="28" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="H62" s="20" t="s">
         <v>428</v>
@@ -9134,18 +9183,21 @@
         <v>428</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>377</v>
+        <v>371</v>
+      </c>
+      <c r="D63" t="s">
+        <v>202</v>
       </c>
       <c r="E63" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="F63" s="20" t="s">
         <v>436</v>
@@ -9160,24 +9212,24 @@
         <v>428</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E64" t="s">
         <v>461</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>436</v>
-      </c>
-      <c r="G64" s="28" t="s">
-        <v>505</v>
+        <v>435</v>
+      </c>
+      <c r="G64" s="29" t="s">
+        <v>506</v>
       </c>
       <c r="H64" s="20" t="s">
         <v>428</v>
@@ -9186,76 +9238,82 @@
         <v>428</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>314</v>
+        <v>250</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>376</v>
+        <v>407</v>
+      </c>
+      <c r="D65" t="s">
+        <v>180</v>
       </c>
       <c r="E65" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="G65" s="29" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="H65" s="20" t="s">
         <v>428</v>
       </c>
       <c r="J65" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+        <v>631</v>
+      </c>
+      <c r="K65" s="29" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B66" t="s">
         <v>13</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="D66" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E66" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="G66" s="29" t="s">
-        <v>499</v>
+        <v>437</v>
+      </c>
+      <c r="G66" s="28" t="s">
+        <v>502</v>
       </c>
       <c r="H66" s="20" t="s">
         <v>428</v>
       </c>
       <c r="J66" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+        <v>626</v>
+      </c>
+      <c r="K66" s="28" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>351</v>
+        <v>385</v>
       </c>
       <c r="D67" t="s">
-        <v>209</v>
+        <v>163</v>
       </c>
       <c r="E67" t="s">
-        <v>484</v>
+        <v>163</v>
       </c>
       <c r="F67" s="20" t="s">
         <v>437</v>
@@ -9267,30 +9325,33 @@
         <v>428</v>
       </c>
       <c r="J67" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+        <v>626</v>
+      </c>
+      <c r="K67" s="28" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B68" t="s">
         <v>13</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>431</v>
+        <v>351</v>
       </c>
       <c r="D68" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="E68" t="s">
-        <v>471</v>
+        <v>484</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G68" s="28" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="H68" s="20" t="s">
         <v>428</v>
@@ -9299,7 +9360,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>262</v>
       </c>
@@ -9328,24 +9389,27 @@
         <v>428</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>269</v>
+        <v>317</v>
       </c>
       <c r="B70" t="s">
         <v>13</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="D70" t="s">
-        <v>213</v>
+        <v>380</v>
       </c>
       <c r="E70" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>428</v>
+        <v>440</v>
+      </c>
+      <c r="G70" s="29" t="s">
+        <v>499</v>
       </c>
       <c r="H70" s="20" t="s">
         <v>428</v>
@@ -9354,56 +9418,57 @@
         <v>428</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>391</v>
-      </c>
-      <c r="D71" t="s">
-        <v>193</v>
+        <v>360</v>
       </c>
       <c r="E71" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>427</v>
-      </c>
-      <c r="G71" s="28" t="s">
-        <v>503</v>
+        <v>430</v>
+      </c>
+      <c r="G71" s="29" t="s">
+        <v>500</v>
       </c>
       <c r="H71" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="J71" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+        <v>448</v>
+      </c>
+      <c r="I71" s="28"/>
+      <c r="J71" s="34" t="s">
+        <v>628</v>
+      </c>
+      <c r="K71" s="29" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>312</v>
+        <v>233</v>
       </c>
       <c r="B72" t="s">
         <v>13</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
       <c r="D72" t="s">
-        <v>183</v>
+        <v>347</v>
       </c>
       <c r="E72" t="s">
-        <v>470</v>
+        <v>180</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>508</v>
+        <v>430</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="H72" s="20" t="s">
         <v>428</v>
@@ -9412,27 +9477,27 @@
         <v>428</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="B73" t="s">
         <v>13</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="D73" t="s">
-        <v>171</v>
+        <v>347</v>
       </c>
       <c r="E73" t="s">
-        <v>470</v>
+        <v>180</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G73" s="28" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="H73" s="20" t="s">
         <v>428</v>
@@ -9441,24 +9506,27 @@
         <v>428</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>313</v>
+        <v>267</v>
       </c>
       <c r="B74" t="s">
         <v>13</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>375</v>
+        <v>358</v>
+      </c>
+      <c r="D74" t="s">
+        <v>179</v>
       </c>
       <c r="E74" t="s">
         <v>470</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>498</v>
+        <v>430</v>
       </c>
       <c r="G74" s="28" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="H74" s="20" t="s">
         <v>428</v>
@@ -9467,27 +9535,27 @@
         <v>428</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="B75" t="s">
         <v>13</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="D75" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
       <c r="E75" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G75" s="28" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="H75" s="20" t="s">
         <v>428</v>
@@ -9496,27 +9564,24 @@
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>267</v>
+        <v>319</v>
       </c>
       <c r="B76" t="s">
         <v>13</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="D76" t="s">
-        <v>179</v>
+        <v>382</v>
       </c>
       <c r="E76" t="s">
         <v>470</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="G76" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H76" s="20" t="s">
         <v>428</v>
@@ -9525,164 +9590,166 @@
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>319</v>
+        <v>286</v>
       </c>
       <c r="B77" t="s">
         <v>13</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>382</v>
+        <v>361</v>
+      </c>
+      <c r="D77" t="s">
+        <v>362</v>
       </c>
       <c r="E77" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>438</v>
-      </c>
-      <c r="G77" s="28" t="s">
-        <v>499</v>
+        <v>428</v>
       </c>
       <c r="H77" s="20" t="s">
         <v>428</v>
       </c>
-      <c r="J77" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J77" s="34" t="s">
+        <v>454</v>
+      </c>
+      <c r="K77" s="28" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="B78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D78" t="s">
+        <v>353</v>
+      </c>
+      <c r="E78" t="s">
+        <v>496</v>
+      </c>
+      <c r="F78" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H78" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="J78" s="34" t="s">
+        <v>622</v>
+      </c>
+      <c r="K78" s="28" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>230</v>
+      </c>
+      <c r="B79" t="s">
+        <v>231</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="D79" t="s">
+        <v>163</v>
+      </c>
+      <c r="E79" t="s">
+        <v>163</v>
+      </c>
+      <c r="F79" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H79" s="20" t="s">
+        <v>447</v>
+      </c>
+      <c r="J79" s="34" t="s">
+        <v>628</v>
+      </c>
+      <c r="K79" s="28" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>258</v>
+      </c>
+      <c r="B80" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="D80" t="s">
+        <v>353</v>
+      </c>
+      <c r="E80" t="s">
+        <v>497</v>
+      </c>
+      <c r="F80" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H80" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="J80" s="20" t="s">
+        <v>625</v>
+      </c>
+      <c r="K80" s="29" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>196</v>
+      </c>
+      <c r="B81" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="D78" t="s">
-        <v>194</v>
-      </c>
-      <c r="E78" t="s">
-        <v>469</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>445</v>
-      </c>
-      <c r="G78" s="29" t="s">
+      <c r="C81" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="D81" t="s">
+        <v>196</v>
+      </c>
+      <c r="E81" t="s">
+        <v>462</v>
+      </c>
+      <c r="F81" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H81" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="J81" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="K81" s="28" t="s">
         <v>510</v>
       </c>
-      <c r="H78" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="J78" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>266</v>
-      </c>
-      <c r="B79" t="s">
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>295</v>
+      </c>
+      <c r="B82" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="D79" t="s">
-        <v>169</v>
-      </c>
-      <c r="E79" t="s">
-        <v>473</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>430</v>
-      </c>
-      <c r="G79" s="28" t="s">
-        <v>500</v>
-      </c>
-      <c r="H79" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="J79" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>284</v>
-      </c>
-      <c r="B80" t="s">
-        <v>40</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>333</v>
-      </c>
-      <c r="D80" t="s">
-        <v>215</v>
-      </c>
-      <c r="E80" t="s">
-        <v>480</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>427</v>
-      </c>
-      <c r="G80" s="28" t="s">
-        <v>503</v>
-      </c>
-      <c r="H80" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="J80" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>241</v>
-      </c>
-      <c r="B81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>350</v>
-      </c>
-      <c r="D81" t="s">
-        <v>174</v>
-      </c>
-      <c r="E81" t="s">
-        <v>494</v>
-      </c>
-      <c r="F81" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="G81" s="29" t="s">
-        <v>492</v>
-      </c>
-      <c r="H81" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="I81" s="28"/>
-      <c r="J81" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>273</v>
-      </c>
-      <c r="B82" t="s">
-        <v>20</v>
-      </c>
       <c r="C82" s="18" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="D82" t="s">
-        <v>168</v>
+        <v>366</v>
       </c>
       <c r="E82" t="s">
-        <v>475</v>
+        <v>163</v>
       </c>
       <c r="F82" s="20" t="s">
         <v>428</v>
@@ -9694,27 +9761,24 @@
         <v>428</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D83" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="E83" t="s">
-        <v>476</v>
+        <v>495</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="G83" s="28" t="s">
-        <v>492</v>
+        <v>428</v>
       </c>
       <c r="H83" s="20" t="s">
         <v>428</v>
@@ -9723,27 +9787,24 @@
         <v>428</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>336</v>
+        <v>367</v>
       </c>
       <c r="D84" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="E84" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="G84" s="28" t="s">
-        <v>492</v>
+        <v>428</v>
       </c>
       <c r="H84" s="20" t="s">
         <v>428</v>
@@ -9752,59 +9813,56 @@
         <v>428</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>329</v>
+        <v>273</v>
       </c>
       <c r="B85" t="s">
         <v>20</v>
       </c>
       <c r="C85" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="D85" t="s">
+        <v>168</v>
+      </c>
+      <c r="E85" t="s">
+        <v>475</v>
+      </c>
+      <c r="F85" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H85" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="J85" s="20" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>329</v>
+      </c>
+      <c r="B86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" s="18" t="s">
         <v>398</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>195</v>
       </c>
-      <c r="F85" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="H85" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="J85" s="20" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
-        <v>239</v>
-      </c>
-      <c r="B86" t="s">
-        <v>13</v>
-      </c>
-      <c r="C86" s="18" t="s">
-        <v>348</v>
-      </c>
-      <c r="D86" t="s">
-        <v>349</v>
-      </c>
-      <c r="E86" t="s">
-        <v>504</v>
-      </c>
       <c r="F86" s="20" t="s">
-        <v>509</v>
-      </c>
-      <c r="G86" s="28" t="s">
-        <v>512</v>
+        <v>428</v>
       </c>
       <c r="H86" s="20" t="s">
         <v>428</v>
       </c>
       <c r="J86" s="20" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>277</v>
       </c>
@@ -9815,7 +9873,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>286</v>
       </c>
@@ -9826,7 +9884,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>324</v>
       </c>
@@ -9837,7 +9895,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>338</v>
       </c>
@@ -9848,7 +9906,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>300</v>
       </c>
@@ -9862,7 +9920,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>327</v>
       </c>
@@ -9873,7 +9931,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>288</v>
       </c>
@@ -9884,7 +9942,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>293</v>
       </c>
@@ -9895,7 +9953,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>219</v>
       </c>
@@ -9906,7 +9964,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>255</v>
       </c>
@@ -10367,7 +10425,7 @@
   </sheetData>
   <autoFilter ref="A2:R156" xr:uid="{86DEC163-0F38-4216-A6F4-B629FE360FF7}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R156">
-      <sortCondition ref="J2:J156"/>
+      <sortCondition ref="F2:F156"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:D57">
@@ -10383,9 +10441,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11053,4 +11111,306 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8629E7C5-043E-4A29-9B03-D70DB32336F4}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>739</v>
+      </c>
+      <c r="B2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>740</v>
+      </c>
+      <c r="B3" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>741</v>
+      </c>
+      <c r="B4" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>742</v>
+      </c>
+      <c r="B5" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>743</v>
+      </c>
+      <c r="B6" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>744</v>
+      </c>
+      <c r="B7" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>16500</v>
+      </c>
+      <c r="B9" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>750</v>
+      </c>
+      <c r="B10" t="s">
+        <v>747</v>
+      </c>
+      <c r="C10" t="s">
+        <v>746</v>
+      </c>
+      <c r="D10" t="s">
+        <v>747</v>
+      </c>
+      <c r="E10" t="s">
+        <v>752</v>
+      </c>
+      <c r="F10" t="s">
+        <v>747</v>
+      </c>
+      <c r="G10" t="s">
+        <v>746</v>
+      </c>
+      <c r="H10" t="s">
+        <v>747</v>
+      </c>
+      <c r="I10" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>741</v>
+      </c>
+      <c r="B11" t="s">
+        <v>744</v>
+      </c>
+      <c r="C11" t="s">
+        <v>739</v>
+      </c>
+      <c r="D11" t="s">
+        <v>744</v>
+      </c>
+      <c r="E11" t="s">
+        <v>742</v>
+      </c>
+      <c r="F11" t="s">
+        <v>744</v>
+      </c>
+      <c r="G11" t="s">
+        <v>739</v>
+      </c>
+      <c r="H11" t="s">
+        <v>744</v>
+      </c>
+      <c r="I11" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>16100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>750</v>
+      </c>
+      <c r="B14" t="s">
+        <v>746</v>
+      </c>
+      <c r="C14" t="s">
+        <v>747</v>
+      </c>
+      <c r="D14" t="s">
+        <v>747</v>
+      </c>
+      <c r="E14" t="s">
+        <v>747</v>
+      </c>
+      <c r="F14" t="s">
+        <v>746</v>
+      </c>
+      <c r="G14" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>741</v>
+      </c>
+      <c r="B15" t="s">
+        <v>739</v>
+      </c>
+      <c r="C15" t="s">
+        <v>744</v>
+      </c>
+      <c r="D15" t="s">
+        <v>744</v>
+      </c>
+      <c r="E15" t="s">
+        <v>744</v>
+      </c>
+      <c r="F15" t="s">
+        <v>739</v>
+      </c>
+      <c r="G15" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16200</v>
+      </c>
+      <c r="B17" t="s">
+        <v>754</v>
+      </c>
+      <c r="C17" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>750</v>
+      </c>
+      <c r="B18" t="s">
+        <v>746</v>
+      </c>
+      <c r="C18" t="s">
+        <v>747</v>
+      </c>
+      <c r="D18" t="s">
+        <v>747</v>
+      </c>
+      <c r="E18" t="s">
+        <v>747</v>
+      </c>
+      <c r="F18" t="s">
+        <v>746</v>
+      </c>
+      <c r="G18" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>741</v>
+      </c>
+      <c r="B19" t="s">
+        <v>739</v>
+      </c>
+      <c r="C19" t="s">
+        <v>744</v>
+      </c>
+      <c r="D19" t="s">
+        <v>744</v>
+      </c>
+      <c r="E19" t="s">
+        <v>744</v>
+      </c>
+      <c r="F19" t="s">
+        <v>739</v>
+      </c>
+      <c r="G19" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>16400</v>
+      </c>
+      <c r="B21" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>756</v>
+      </c>
+      <c r="B22" t="s">
+        <v>747</v>
+      </c>
+      <c r="C22" t="s">
+        <v>746</v>
+      </c>
+      <c r="D22" t="s">
+        <v>749</v>
+      </c>
+      <c r="E22" t="s">
+        <v>746</v>
+      </c>
+      <c r="F22" t="s">
+        <v>747</v>
+      </c>
+      <c r="G22" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>740</v>
+      </c>
+      <c r="B23" t="s">
+        <v>744</v>
+      </c>
+      <c r="C23" t="s">
+        <v>739</v>
+      </c>
+      <c r="D23" t="s">
+        <v>742</v>
+      </c>
+      <c r="E23" t="s">
+        <v>739</v>
+      </c>
+      <c r="F23" t="s">
+        <v>744</v>
+      </c>
+      <c r="G23" t="s">
+        <v>743</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[5100] Initial scenario, LL consists
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CE1371-8104-4E08-B750-C0C71091F80C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D7568-85C7-41B3-B064-7F4C8B007DC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21533" yWindow="3420" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8355" yWindow="2948" windowWidth="14400" windowHeight="7484" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
     <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId2"/>
-    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId3"/>
-    <sheet name="Goederentreinen" sheetId="9" r:id="rId4"/>
+    <sheet name="Goederentreinen" sheetId="9" r:id="rId3"/>
+    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="14" r:id="rId5"/>
     <sheet name="Vervoerders" sheetId="7" r:id="rId6"/>
     <sheet name="ICRm" sheetId="17" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -220,40 +220,6 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Tom</author>
-  </authors>
-  <commentList>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-10 Rtd-Rsd, 6 Rsd-Vs</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tom</author>
@@ -456,8 +422,42 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+10 Rtd-Rsd, 6 Rsd-Vs</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="766">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2855,6 +2855,50 @@
   </si>
   <si>
     <t>zelfde als 16100</t>
+  </si>
+  <si>
+    <t>ZWNL</t>
+  </si>
+  <si>
+    <t>GEEN VIDEO</t>
+  </si>
+  <si>
+    <t>5100 Ddr-Rtd</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-EjJFCWNSQw&amp;t=1565s</t>
+  </si>
+  <si>
+    <t>Ddr</t>
+  </si>
+  <si>
+    <t>Losse Lok</t>
+  </si>
+  <si>
+    <t>- Kfh
+- IJsm</t>
+  </si>
+  <si>
+    <t>Ddr:
+- 1900/1901 Ddr2b
+- 5900/5901 Ddr3b
+- 6600/6601 Ddr4b
+Ddr-Rtd:
+- 5101 Zwd3, Ddr3a
+- 2401 Zwd binnenspoor
+- G Brd-Kfh aankomst
+- G Brd-Kfh aankomst 2
+- 5001 Rlb
+- 900 Rtst
+- 2200 Rtst
+- 9101/9300 Rtb
+- 1000/1001 Rtd3
+- 4000/4001 Rtd16
+Rtd:
+- 500/600 Rtd14
+- 2401 Sdm-Rtd6
+- 9100/9301 Rtd11
+- 9600 Rtd4</t>
   </si>
 </sst>
 </file>
@@ -2991,7 +3035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3072,6 +3116,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6922,458 +6972,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
-  <dimension ref="A1:F28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="20.19921875" customWidth="1"/>
-    <col min="3" max="3" width="8.1328125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>561</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>570</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>585</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>900</v>
-      </c>
-      <c r="B2" t="s">
-        <v>572</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>1000</v>
-      </c>
-      <c r="B3" t="s">
-        <v>572</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>1100</v>
-      </c>
-      <c r="B4" t="s">
-        <v>573</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>7100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>563</v>
-      </c>
-      <c r="C5" t="s">
-        <v>584</v>
-      </c>
-      <c r="D5" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>7200</v>
-      </c>
-      <c r="B6" t="s">
-        <v>563</v>
-      </c>
-      <c r="C6" t="s">
-        <v>584</v>
-      </c>
-      <c r="D6" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>4000</v>
-      </c>
-      <c r="B7" t="s">
-        <v>575</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>9100</v>
-      </c>
-      <c r="B8" t="s">
-        <v>560</v>
-      </c>
-      <c r="C8">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>594</v>
-      </c>
-      <c r="F8" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>9300</v>
-      </c>
-      <c r="B9" t="s">
-        <v>559</v>
-      </c>
-      <c r="C9" t="s">
-        <v>583</v>
-      </c>
-      <c r="D9" t="s">
-        <v>594</v>
-      </c>
-      <c r="F9" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>450</v>
-      </c>
-      <c r="B10" t="s">
-        <v>568</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>567</v>
-      </c>
-      <c r="D11" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>567</v>
-      </c>
-      <c r="D12" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>5000</v>
-      </c>
-      <c r="B13" t="s">
-        <v>577</v>
-      </c>
-      <c r="C13">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>589</v>
-      </c>
-      <c r="F13" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>5100</v>
-      </c>
-      <c r="B14" t="s">
-        <v>577</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>589</v>
-      </c>
-      <c r="F14" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>2200</v>
-      </c>
-      <c r="B15" t="s">
-        <v>557</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>579</v>
-      </c>
-      <c r="D15" t="s">
-        <v>565</v>
-      </c>
-      <c r="E15" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>2400</v>
-      </c>
-      <c r="B16" t="s">
-        <v>557</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>3600</v>
-      </c>
-      <c r="B17" t="s">
-        <v>557</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>565</v>
-      </c>
-      <c r="E17">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>3700</v>
-      </c>
-      <c r="B18" t="s">
-        <v>557</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>565</v>
-      </c>
-      <c r="E18">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>12200</v>
-      </c>
-      <c r="B19" t="s">
-        <v>557</v>
-      </c>
-      <c r="C19">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>565</v>
-      </c>
-      <c r="E19">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>500</v>
-      </c>
-      <c r="B20" t="s">
-        <v>571</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>600</v>
-      </c>
-      <c r="B21" t="s">
-        <v>571</v>
-      </c>
-      <c r="C21">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>564</v>
-      </c>
-      <c r="E21">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>1900</v>
-      </c>
-      <c r="B22" t="s">
-        <v>571</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>564</v>
-      </c>
-      <c r="E22">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>2800</v>
-      </c>
-      <c r="B23" t="s">
-        <v>571</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
-        <v>564</v>
-      </c>
-      <c r="E23">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>9200</v>
-      </c>
-      <c r="B24" t="s">
-        <v>582</v>
-      </c>
-      <c r="D24" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>9600</v>
-      </c>
-      <c r="B25" t="s">
-        <v>582</v>
-      </c>
-      <c r="D25" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>6600</v>
-      </c>
-      <c r="B26" t="s">
-        <v>558</v>
-      </c>
-      <c r="C26">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>5900</v>
-      </c>
-      <c r="B27" t="s">
-        <v>580</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>588</v>
-      </c>
-      <c r="E27">
-        <v>80</v>
-      </c>
-      <c r="F27" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>7700</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F27" xr:uid="{AA9E098D-0675-414C-8423-8DB175120546}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
-      <sortCondition ref="D1:D27"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
-    <sortCondition ref="A2:A18"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE17749-1BD2-42DC-A92D-74E793F7820B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7455,7 +7062,7 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>264</v>
       </c>
@@ -7490,7 +7097,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>304</v>
       </c>
@@ -7519,7 +7126,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>238</v>
       </c>
@@ -7552,7 +7159,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>234</v>
       </c>
@@ -7581,7 +7188,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>453</v>
       </c>
@@ -7608,7 +7215,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>297</v>
       </c>
@@ -7635,7 +7242,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>220</v>
       </c>
@@ -7664,7 +7271,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>260</v>
       </c>
@@ -7693,7 +7300,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>284</v>
       </c>
@@ -7788,7 +7395,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>239</v>
       </c>
@@ -7817,7 +7424,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>312</v>
       </c>
@@ -7846,7 +7453,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>218</v>
       </c>
@@ -7872,7 +7479,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -7901,7 +7508,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>263</v>
       </c>
@@ -7930,7 +7537,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>307</v>
       </c>
@@ -7959,7 +7566,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>216</v>
       </c>
@@ -7985,7 +7592,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>309</v>
       </c>
@@ -8011,7 +7618,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>249</v>
       </c>
@@ -8040,7 +7647,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>227</v>
       </c>
@@ -8069,7 +7676,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>222</v>
       </c>
@@ -8098,7 +7705,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>261</v>
       </c>
@@ -8127,7 +7734,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>278</v>
       </c>
@@ -8156,7 +7763,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>325</v>
       </c>
@@ -8185,7 +7792,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>282</v>
       </c>
@@ -8214,7 +7821,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>301</v>
       </c>
@@ -8243,7 +7850,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>272</v>
       </c>
@@ -8272,7 +7879,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>271</v>
       </c>
@@ -8301,7 +7908,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>279</v>
       </c>
@@ -8330,7 +7937,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>245</v>
       </c>
@@ -8359,7 +7966,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>256</v>
       </c>
@@ -8388,7 +7995,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>299</v>
       </c>
@@ -8417,7 +8024,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>270</v>
       </c>
@@ -8443,7 +8050,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>240</v>
       </c>
@@ -8472,7 +8079,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>242</v>
       </c>
@@ -8501,7 +8108,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>289</v>
       </c>
@@ -8530,7 +8137,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>268</v>
       </c>
@@ -8559,7 +8166,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>221</v>
       </c>
@@ -8585,7 +8192,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -8614,7 +8221,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>290</v>
       </c>
@@ -8643,7 +8250,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>283</v>
       </c>
@@ -8672,7 +8279,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>252</v>
       </c>
@@ -8701,7 +8308,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>254</v>
       </c>
@@ -8730,7 +8337,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>276</v>
       </c>
@@ -8759,7 +8366,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>320</v>
       </c>
@@ -8785,7 +8392,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>292</v>
       </c>
@@ -8814,7 +8421,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>225</v>
       </c>
@@ -8840,7 +8447,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>458</v>
       </c>
@@ -8869,7 +8476,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>323</v>
       </c>
@@ -8898,7 +8505,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>241</v>
       </c>
@@ -8928,7 +8535,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -8957,7 +8564,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>243</v>
       </c>
@@ -8986,7 +8593,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>311</v>
       </c>
@@ -9015,7 +8622,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>296</v>
       </c>
@@ -9076,7 +8683,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>313</v>
       </c>
@@ -9102,7 +8709,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>315</v>
       </c>
@@ -9128,7 +8735,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>316</v>
       </c>
@@ -9154,7 +8761,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>253</v>
       </c>
@@ -9183,7 +8790,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>302</v>
       </c>
@@ -9212,7 +8819,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>314</v>
       </c>
@@ -9360,7 +8967,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>262</v>
       </c>
@@ -9389,7 +8996,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>317</v>
       </c>
@@ -9418,7 +9025,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>280</v>
       </c>
@@ -9448,7 +9055,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>233</v>
       </c>
@@ -9477,7 +9084,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>306</v>
       </c>
@@ -9506,7 +9113,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>267</v>
       </c>
@@ -9535,7 +9142,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>266</v>
       </c>
@@ -9564,7 +9171,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>319</v>
       </c>
@@ -9590,7 +9197,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>286</v>
       </c>
@@ -9619,7 +9226,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>248</v>
       </c>
@@ -9648,7 +9255,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>230</v>
       </c>
@@ -9677,7 +9284,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>258</v>
       </c>
@@ -9706,7 +9313,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>196</v>
       </c>
@@ -9735,7 +9342,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>295</v>
       </c>
@@ -9761,7 +9368,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>226</v>
       </c>
@@ -9787,7 +9394,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>269</v>
       </c>
@@ -9813,7 +9420,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>273</v>
       </c>
@@ -9839,7 +9446,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>329</v>
       </c>
@@ -9862,7 +9469,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>277</v>
       </c>
@@ -9873,7 +9480,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>286</v>
       </c>
@@ -9884,7 +9491,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>324</v>
       </c>
@@ -9895,7 +9502,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>338</v>
       </c>
@@ -9906,7 +9513,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>300</v>
       </c>
@@ -9920,7 +9527,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>327</v>
       </c>
@@ -9931,7 +9538,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>288</v>
       </c>
@@ -9942,7 +9549,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>293</v>
       </c>
@@ -9953,7 +9560,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>219</v>
       </c>
@@ -9964,7 +9571,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>255</v>
       </c>
@@ -9975,7 +9582,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>255</v>
       </c>
@@ -9986,7 +9593,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>242</v>
       </c>
@@ -9997,7 +9604,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>251</v>
       </c>
@@ -10008,7 +9615,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>298</v>
       </c>
@@ -10019,7 +9626,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>237</v>
       </c>
@@ -10030,7 +9637,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>328</v>
       </c>
@@ -10041,7 +9648,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>265</v>
       </c>
@@ -10052,7 +9659,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>228</v>
       </c>
@@ -10063,7 +9670,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>244</v>
       </c>
@@ -10074,7 +9681,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>287</v>
       </c>
@@ -10088,7 +9695,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>294</v>
       </c>
@@ -10099,7 +9706,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>305</v>
       </c>
@@ -10110,7 +9717,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>303</v>
       </c>
@@ -10121,7 +9728,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>291</v>
       </c>
@@ -10132,7 +9739,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>310</v>
       </c>
@@ -10143,7 +9750,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>274</v>
       </c>
@@ -10157,7 +9764,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>247</v>
       </c>
@@ -10168,7 +9775,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>223</v>
       </c>
@@ -10179,7 +9786,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>285</v>
       </c>
@@ -10190,7 +9797,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>326</v>
       </c>
@@ -10201,7 +9808,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>322</v>
       </c>
@@ -10212,7 +9819,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>275</v>
       </c>
@@ -10223,7 +9830,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>281</v>
       </c>
@@ -10237,193 +9844,200 @@
         <v>478</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D120" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D121" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D122" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D123" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D124" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D125" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D126" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D127" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D128" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D129" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="130" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D130" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="131" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D131" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D132" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="133" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D133" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="134" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D134" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="135" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D135" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="136" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D136" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="137" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D137" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="138" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D138" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="139" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D139" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="140" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D140" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="141" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D141" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="142" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D142" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="143" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D143" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="144" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D144" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="145" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D145" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="146" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D146" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="147" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D147" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="148" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D148" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="149" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D149" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="150" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D150" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="151" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D151" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="152" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D152" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="153" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D153" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="154" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D154" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="155" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D155" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="156" spans="4:4" hidden="1" x14ac:dyDescent="0.45">
       <c r="D156" t="s">
         <v>170</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:R156" xr:uid="{86DEC163-0F38-4216-A6F4-B629FE360FF7}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Esn-Bd, Esn-Rtng"/>
+        <filter val="H-Kfh-Rtng, H-Kfh-BR"/>
+        <filter val="Kfh-Rtng"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R156">
       <sortCondition ref="F2:F156"/>
     </sortState>
@@ -10437,13 +10051,465 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="20.19921875" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>450</v>
+      </c>
+      <c r="B2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>500</v>
+      </c>
+      <c r="B3" t="s">
+        <v>571</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>600</v>
+      </c>
+      <c r="B4" t="s">
+        <v>571</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>564</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>900</v>
+      </c>
+      <c r="B5" t="s">
+        <v>572</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>572</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>1100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>573</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>1900</v>
+      </c>
+      <c r="B8" t="s">
+        <v>571</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>564</v>
+      </c>
+      <c r="E8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>2200</v>
+      </c>
+      <c r="B9" t="s">
+        <v>557</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>579</v>
+      </c>
+      <c r="D9" t="s">
+        <v>565</v>
+      </c>
+      <c r="E9" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>2400</v>
+      </c>
+      <c r="B10" t="s">
+        <v>557</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>2800</v>
+      </c>
+      <c r="B11" t="s">
+        <v>571</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>564</v>
+      </c>
+      <c r="E11">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>3600</v>
+      </c>
+      <c r="B12" t="s">
+        <v>557</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>565</v>
+      </c>
+      <c r="E12">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>3700</v>
+      </c>
+      <c r="B13" t="s">
+        <v>557</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>565</v>
+      </c>
+      <c r="E13">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>4000</v>
+      </c>
+      <c r="B14" t="s">
+        <v>575</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>5000</v>
+      </c>
+      <c r="B15" t="s">
+        <v>577</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>589</v>
+      </c>
+      <c r="F15" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>5100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>577</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>589</v>
+      </c>
+      <c r="F16" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>5900</v>
+      </c>
+      <c r="B17" t="s">
+        <v>580</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>588</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>6600</v>
+      </c>
+      <c r="B18" t="s">
+        <v>558</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>7100</v>
+      </c>
+      <c r="B19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C19" t="s">
+        <v>584</v>
+      </c>
+      <c r="D19" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>7200</v>
+      </c>
+      <c r="B20" t="s">
+        <v>563</v>
+      </c>
+      <c r="C20" t="s">
+        <v>584</v>
+      </c>
+      <c r="D20" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>7700</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>9100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>560</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>594</v>
+      </c>
+      <c r="F22" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>9200</v>
+      </c>
+      <c r="B23" t="s">
+        <v>582</v>
+      </c>
+      <c r="D23" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>9300</v>
+      </c>
+      <c r="B24" t="s">
+        <v>559</v>
+      </c>
+      <c r="C24" t="s">
+        <v>583</v>
+      </c>
+      <c r="D24" t="s">
+        <v>594</v>
+      </c>
+      <c r="F24" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>9600</v>
+      </c>
+      <c r="B25" t="s">
+        <v>582</v>
+      </c>
+      <c r="D25" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>12200</v>
+      </c>
+      <c r="B26" t="s">
+        <v>557</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>565</v>
+      </c>
+      <c r="E26">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>567</v>
+      </c>
+      <c r="D27" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>567</v>
+      </c>
+      <c r="D28" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>763</v>
+      </c>
+      <c r="D29" t="s">
+        <v>621</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F27" xr:uid="{AA9E098D-0675-414C-8423-8DB175120546}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
+      <sortCondition ref="A1:A27"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
+    <sortCondition ref="A2:A18"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10613,6 +10679,37 @@
       </c>
       <c r="C7" s="32" t="s">
         <v>727</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="32" t="s">
+        <v>758</v>
+      </c>
+      <c r="B8" s="32">
+        <v>6600</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="285" x14ac:dyDescent="0.45">
+      <c r="A9" s="32" t="s">
+        <v>758</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>760</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>761</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>762</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>765</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -11117,7 +11214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8629E7C5-043E-4A29-9B03-D70DB32336F4}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ZWNL ICD en LL consists
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D7568-85C7-41B3-B064-7F4C8B007DC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CBF339-16B1-4C2C-A314-B1BD66EB3121}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8355" yWindow="2948" windowWidth="14400" windowHeight="7484" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8355" yWindow="2948" windowWidth="14400" windowHeight="7484" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -428,7 +428,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
       <text>
         <r>
           <rPr>
@@ -10055,8 +10055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10089,207 +10089,180 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="B2" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="B3" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>564</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="B4" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>564</v>
-      </c>
-      <c r="E4">
-        <v>200</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>900</v>
+        <v>7100</v>
       </c>
       <c r="B5" t="s">
-        <v>572</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
+        <v>563</v>
+      </c>
+      <c r="C5" t="s">
+        <v>584</v>
       </c>
       <c r="D5" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>1000</v>
+        <v>7200</v>
       </c>
       <c r="B6" t="s">
-        <v>572</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
+        <v>563</v>
+      </c>
+      <c r="C6" t="s">
+        <v>584</v>
       </c>
       <c r="D6" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>1100</v>
+        <v>4000</v>
       </c>
       <c r="B7" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>1900</v>
+        <v>9100</v>
       </c>
       <c r="B8" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>564</v>
-      </c>
-      <c r="E8">
-        <v>120</v>
+        <v>594</v>
+      </c>
+      <c r="F8" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>2200</v>
+        <v>9300</v>
       </c>
       <c r="B9" t="s">
-        <v>557</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>579</v>
+        <v>559</v>
+      </c>
+      <c r="C9" t="s">
+        <v>583</v>
       </c>
       <c r="D9" t="s">
-        <v>565</v>
-      </c>
-      <c r="E9" t="s">
-        <v>599</v>
+        <v>594</v>
+      </c>
+      <c r="F9" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>2400</v>
+        <v>450</v>
       </c>
       <c r="B10" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>565</v>
+        <v>595</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>2800</v>
-      </c>
-      <c r="B11" t="s">
-        <v>571</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
+      <c r="A11" t="s">
+        <v>763</v>
       </c>
       <c r="D11" t="s">
-        <v>564</v>
-      </c>
-      <c r="E11">
-        <v>180</v>
+        <v>621</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>3600</v>
-      </c>
-      <c r="B12" t="s">
-        <v>557</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
+      <c r="A12" t="s">
+        <v>567</v>
       </c>
       <c r="D12" t="s">
-        <v>565</v>
-      </c>
-      <c r="E12">
-        <v>170</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>3700</v>
-      </c>
-      <c r="B13" t="s">
-        <v>557</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
+      <c r="A13" t="s">
+        <v>567</v>
       </c>
       <c r="D13" t="s">
-        <v>565</v>
-      </c>
-      <c r="E13">
-        <v>170</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="B14" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>593</v>
+        <v>589</v>
+      </c>
+      <c r="F14" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>5000</v>
+        <v>5100</v>
       </c>
       <c r="B15" t="s">
         <v>577</v>
@@ -10306,139 +10279,154 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>5100</v>
+        <v>2200</v>
       </c>
       <c r="B16" t="s">
-        <v>577</v>
-      </c>
-      <c r="C16">
-        <v>7</v>
+        <v>557</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>579</v>
       </c>
       <c r="D16" t="s">
-        <v>589</v>
-      </c>
-      <c r="F16" t="s">
-        <v>598</v>
+        <v>565</v>
+      </c>
+      <c r="E16" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>5900</v>
+        <v>2400</v>
       </c>
       <c r="B17" t="s">
-        <v>580</v>
+        <v>557</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>588</v>
-      </c>
-      <c r="E17">
-        <v>80</v>
-      </c>
-      <c r="F17" t="s">
-        <v>598</v>
+        <v>565</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>6600</v>
+        <v>3600</v>
       </c>
       <c r="B18" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>566</v>
+        <v>565</v>
+      </c>
+      <c r="E18">
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>7100</v>
+        <v>3700</v>
       </c>
       <c r="B19" t="s">
-        <v>563</v>
-      </c>
-      <c r="C19" t="s">
-        <v>584</v>
+        <v>557</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>592</v>
+        <v>565</v>
+      </c>
+      <c r="E19">
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>7200</v>
+        <v>12200</v>
       </c>
       <c r="B20" t="s">
-        <v>563</v>
-      </c>
-      <c r="C20" t="s">
-        <v>584</v>
+        <v>557</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>592</v>
+        <v>565</v>
+      </c>
+      <c r="E20">
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>7700</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>581</v>
+        <v>500</v>
+      </c>
+      <c r="B21" t="s">
+        <v>571</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>9100</v>
+        <v>600</v>
       </c>
       <c r="B22" t="s">
-        <v>560</v>
+        <v>571</v>
       </c>
       <c r="C22">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>594</v>
-      </c>
-      <c r="F22" t="s">
-        <v>596</v>
+        <v>564</v>
+      </c>
+      <c r="E22">
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>9200</v>
+        <v>1900</v>
       </c>
       <c r="B23" t="s">
-        <v>582</v>
+        <v>571</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>586</v>
+        <v>564</v>
+      </c>
+      <c r="E23">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>9300</v>
+        <v>2800</v>
       </c>
       <c r="B24" t="s">
-        <v>559</v>
-      </c>
-      <c r="C24" t="s">
-        <v>583</v>
+        <v>571</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>594</v>
-      </c>
-      <c r="F24" t="s">
-        <v>597</v>
+        <v>564</v>
+      </c>
+      <c r="E24">
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>9600</v>
+        <v>9200</v>
       </c>
       <c r="B25" t="s">
         <v>582</v>
@@ -10449,49 +10437,61 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>12200</v>
+        <v>9600</v>
       </c>
       <c r="B26" t="s">
-        <v>557</v>
-      </c>
-      <c r="C26">
-        <v>6</v>
+        <v>582</v>
       </c>
       <c r="D26" t="s">
-        <v>565</v>
-      </c>
-      <c r="E26">
-        <v>170</v>
+        <v>586</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>567</v>
+      <c r="A27">
+        <v>6600</v>
+      </c>
+      <c r="B27" t="s">
+        <v>558</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>491</v>
+        <v>566</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>567</v>
+      <c r="A28">
+        <v>5900</v>
+      </c>
+      <c r="B28" t="s">
+        <v>580</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>600</v>
+        <v>588</v>
+      </c>
+      <c r="E28">
+        <v>80</v>
+      </c>
+      <c r="F28" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>763</v>
-      </c>
-      <c r="D29" t="s">
-        <v>621</v>
+      <c r="A29">
+        <v>7700</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>581</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{AA9E098D-0675-414C-8423-8DB175120546}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
-      <sortCondition ref="A1:A27"/>
+      <sortCondition ref="D1:D27"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
@@ -10507,7 +10507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>

</xml_diff>

<commit_message>
[5101] Add to git, thalys and eurostar consists
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD7633B-33E7-4F40-B3B5-F763D3FE704E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4A7599-02B5-4CE8-8608-B1821898D00C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20963" yWindow="4763" windowWidth="14399" windowHeight="7484" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -428,7 +428,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
       <text>
         <r>
           <rPr>
@@ -457,7 +457,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="771">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2904,6 +2904,59 @@
 - Kfh
 - Ijsm
 - Rtd</t>
+  </si>
+  <si>
+    <t>5101 Rtd-Ddr</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=E2YkVEOnOGg</t>
+  </si>
+  <si>
+    <t>Rtd</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rtd:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">9101/9300 Rtd2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- 500/600 Rtd14
+- 1000/1001 Rtd11
+- 2400 Rtd9
+- 4000/4001 Rtd16
+- 9201/9601 Rtd12
+Rtd-Ddr:
+- 9101/9300 Wiltz buiten
+- 2201 Rtst binnen
+- 901 Rtst buiten
+- 5000 Brd binnen
+- G Kfhan ri Mvt
+- 2400 Kfhz binnen
+- 5100 Zwd binnen
+Ddr:
+- 5900/5901 Ddr3b
+- 6600/6601 Ddr4b
+- 7100 Ddr15</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -7329,7 +7382,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>308</v>
       </c>
@@ -7362,7 +7415,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>321</v>
       </c>
@@ -7508,7 +7561,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>263</v>
       </c>
@@ -7537,7 +7590,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>307</v>
       </c>
@@ -7566,7 +7619,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>216</v>
       </c>
@@ -7592,7 +7645,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>309</v>
       </c>
@@ -7618,7 +7671,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>249</v>
       </c>
@@ -7647,7 +7700,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>227</v>
       </c>
@@ -7676,7 +7729,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>222</v>
       </c>
@@ -7705,7 +7758,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>261</v>
       </c>
@@ -7734,7 +7787,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>278</v>
       </c>
@@ -7763,7 +7816,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>325</v>
       </c>
@@ -7792,7 +7845,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>282</v>
       </c>
@@ -7821,7 +7874,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>301</v>
       </c>
@@ -7850,7 +7903,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>272</v>
       </c>
@@ -7879,7 +7932,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>271</v>
       </c>
@@ -7908,7 +7961,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>279</v>
       </c>
@@ -7937,7 +7990,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>245</v>
       </c>
@@ -7966,7 +8019,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>256</v>
       </c>
@@ -7995,7 +8048,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>299</v>
       </c>
@@ -8024,7 +8077,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>270</v>
       </c>
@@ -8050,7 +8103,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>240</v>
       </c>
@@ -8079,7 +8132,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>242</v>
       </c>
@@ -8108,7 +8161,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>289</v>
       </c>
@@ -8137,7 +8190,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>268</v>
       </c>
@@ -8166,7 +8219,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>221</v>
       </c>
@@ -8192,7 +8245,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -8221,7 +8274,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>290</v>
       </c>
@@ -8250,7 +8303,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>283</v>
       </c>
@@ -8279,7 +8332,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>252</v>
       </c>
@@ -8308,7 +8361,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>254</v>
       </c>
@@ -8337,7 +8390,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>276</v>
       </c>
@@ -8366,7 +8419,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>320</v>
       </c>
@@ -8392,7 +8445,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>292</v>
       </c>
@@ -8421,7 +8474,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>225</v>
       </c>
@@ -8447,7 +8500,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>458</v>
       </c>
@@ -8476,7 +8529,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>323</v>
       </c>
@@ -8505,7 +8558,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>241</v>
       </c>
@@ -8535,7 +8588,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -8564,7 +8617,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>243</v>
       </c>
@@ -8593,7 +8646,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>311</v>
       </c>
@@ -8622,7 +8675,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>296</v>
       </c>
@@ -8845,7 +8898,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>250</v>
       </c>
@@ -8877,7 +8930,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>318</v>
       </c>
@@ -8906,7 +8959,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>232</v>
       </c>
@@ -8938,7 +8991,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>246</v>
       </c>
@@ -10033,9 +10086,11 @@
   <autoFilter ref="A2:R156" xr:uid="{86DEC163-0F38-4216-A6F4-B629FE360FF7}">
     <filterColumn colId="5">
       <filters>
-        <filter val="Esn-Bd, Esn-Rtng"/>
+        <filter val="H-Kfh-Bd"/>
+        <filter val="H-Kfh-Bd, H-Kfh-BR"/>
+        <filter val="H-Kfh-BR"/>
+        <filter val="H-Kfh-Esn"/>
         <filter val="H-Kfh-Rtng, H-Kfh-BR"/>
-        <filter val="Kfh-Rtng"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R156">
@@ -10056,7 +10111,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10089,180 +10144,207 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>900</v>
+        <v>450</v>
       </c>
       <c r="B2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="B3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>590</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>1100</v>
+        <v>600</v>
       </c>
       <c r="B4" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>591</v>
+        <v>564</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>7100</v>
+        <v>900</v>
       </c>
       <c r="B5" t="s">
-        <v>563</v>
-      </c>
-      <c r="C5" t="s">
-        <v>584</v>
+        <v>572</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>7200</v>
+        <v>1000</v>
       </c>
       <c r="B6" t="s">
-        <v>563</v>
-      </c>
-      <c r="C6" t="s">
-        <v>584</v>
+        <v>572</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>4000</v>
+        <v>1100</v>
       </c>
       <c r="B7" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>9100</v>
+        <v>1900</v>
       </c>
       <c r="B8" t="s">
-        <v>560</v>
+        <v>571</v>
       </c>
       <c r="C8">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>594</v>
-      </c>
-      <c r="F8" t="s">
-        <v>596</v>
+        <v>4</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>564</v>
+      </c>
+      <c r="E8">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>9300</v>
+        <v>2200</v>
       </c>
       <c r="B9" t="s">
-        <v>559</v>
-      </c>
-      <c r="C9" t="s">
-        <v>583</v>
-      </c>
-      <c r="D9" t="s">
-        <v>594</v>
-      </c>
-      <c r="F9" t="s">
-        <v>597</v>
+        <v>557</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>579</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>565</v>
+      </c>
+      <c r="E9" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>450</v>
+        <v>2400</v>
       </c>
       <c r="B10" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>595</v>
+        <v>565</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>763</v>
+      <c r="A11">
+        <v>2800</v>
+      </c>
+      <c r="B11" t="s">
+        <v>571</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>621</v>
+        <v>564</v>
+      </c>
+      <c r="E11">
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>567</v>
+      <c r="A12">
+        <v>3600</v>
+      </c>
+      <c r="B12" t="s">
+        <v>557</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>491</v>
+        <v>565</v>
+      </c>
+      <c r="E12">
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>567</v>
-      </c>
-      <c r="D13" t="s">
-        <v>600</v>
+      <c r="A13">
+        <v>3700</v>
+      </c>
+      <c r="B13" t="s">
+        <v>557</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>565</v>
+      </c>
+      <c r="E13">
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B14" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>589</v>
-      </c>
-      <c r="F14" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>5100</v>
+        <v>5000</v>
       </c>
       <c r="B15" t="s">
         <v>577</v>
@@ -10279,154 +10361,140 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>2200</v>
+        <v>5100</v>
       </c>
       <c r="B16" t="s">
-        <v>557</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>579</v>
+        <v>577</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>565</v>
-      </c>
-      <c r="E16" t="s">
-        <v>599</v>
+        <v>589</v>
+      </c>
+      <c r="F16" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>2400</v>
+        <v>5900</v>
       </c>
       <c r="B17" t="s">
-        <v>557</v>
+        <v>580</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>565</v>
+        <v>588</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>3600</v>
+        <v>6600</v>
       </c>
       <c r="B18" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>565</v>
-      </c>
-      <c r="E18">
-        <v>170</v>
+        <v>566</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>3700</v>
+        <v>7100</v>
       </c>
       <c r="B19" t="s">
-        <v>557</v>
-      </c>
-      <c r="C19">
-        <v>6</v>
+        <v>563</v>
+      </c>
+      <c r="C19" t="s">
+        <v>584</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>565</v>
-      </c>
-      <c r="E19">
-        <v>170</v>
+        <v>592</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>12200</v>
+        <v>7200</v>
       </c>
       <c r="B20" t="s">
-        <v>557</v>
-      </c>
-      <c r="C20">
-        <v>6</v>
+        <v>563</v>
+      </c>
+      <c r="C20" t="s">
+        <v>584</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>565</v>
-      </c>
-      <c r="E20">
-        <v>170</v>
+        <v>592</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>500</v>
-      </c>
-      <c r="B21" t="s">
-        <v>571</v>
-      </c>
-      <c r="C21">
-        <v>8</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>564</v>
-      </c>
+        <v>7700</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>600</v>
+        <v>9100</v>
       </c>
       <c r="B22" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>564</v>
-      </c>
-      <c r="E22">
-        <v>200</v>
+        <v>594</v>
+      </c>
+      <c r="F22" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>1900</v>
+        <v>9200</v>
       </c>
       <c r="B23" t="s">
-        <v>571</v>
-      </c>
-      <c r="C23">
-        <v>4</v>
+        <v>582</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>564</v>
-      </c>
-      <c r="E23">
-        <v>120</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>2800</v>
+        <v>9300</v>
       </c>
       <c r="B24" t="s">
-        <v>571</v>
-      </c>
-      <c r="C24">
-        <v>6</v>
+        <v>559</v>
+      </c>
+      <c r="C24" t="s">
+        <v>583</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>564</v>
-      </c>
-      <c r="E24">
-        <v>180</v>
+        <v>594</v>
+      </c>
+      <c r="F24" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>9200</v>
+        <v>9600</v>
       </c>
       <c r="B25" t="s">
         <v>582</v>
@@ -10437,61 +10505,49 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>9600</v>
+        <v>12200</v>
       </c>
       <c r="B26" t="s">
-        <v>582</v>
+        <v>557</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>586</v>
+        <v>565</v>
+      </c>
+      <c r="E26">
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>6600</v>
-      </c>
-      <c r="B27" t="s">
-        <v>558</v>
-      </c>
-      <c r="C27">
-        <v>7</v>
+      <c r="A27" t="s">
+        <v>567</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>566</v>
+        <v>491</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>5900</v>
-      </c>
-      <c r="B28" t="s">
-        <v>580</v>
-      </c>
-      <c r="C28">
-        <v>4</v>
+      <c r="A28" t="s">
+        <v>567</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>588</v>
-      </c>
-      <c r="E28">
-        <v>80</v>
-      </c>
-      <c r="F28" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>7700</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>581</v>
+      <c r="A29" t="s">
+        <v>763</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>621</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F27" xr:uid="{AA9E098D-0675-414C-8423-8DB175120546}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
-      <sortCondition ref="D1:D27"/>
+      <sortCondition ref="A1:A27"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
@@ -10505,11 +10561,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10702,7 +10758,9 @@
       <c r="C9" s="33" t="s">
         <v>761</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="33" t="s">
+        <v>718</v>
+      </c>
       <c r="E9" s="33" t="s">
         <v>762</v>
       </c>
@@ -10717,6 +10775,26 @@
       </c>
       <c r="I9" s="33" t="s">
         <v>722</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="270.75" x14ac:dyDescent="0.45">
+      <c r="A10" s="32" t="s">
+        <v>758</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>767</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>768</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>769</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[6600] Add scenario to git
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90865995-7AD4-4F8C-AC92-98F4DF1F0AED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52787D7B-054D-4843-901C-F88EF4C79FEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
-    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId2"/>
+    <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId2"/>
     <sheet name="Goederentreinen" sheetId="9" r:id="rId3"/>
-    <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId4"/>
+    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="14" r:id="rId5"/>
     <sheet name="Vervoerders" sheetId="7" r:id="rId6"/>
     <sheet name="ICRm" sheetId="17" r:id="rId7"/>
@@ -24,8 +24,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -220,40 +220,6 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Tom</author>
-  </authors>
-  <commentList>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-10 Rtd-Rsd, 6 Rsd-Vs</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tom</author>
@@ -456,8 +422,42 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+10 Rtd-Rsd, 6 Rsd-Vs</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2005" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="785">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2860,9 +2860,6 @@
     <t>ZWNL</t>
   </si>
   <si>
-    <t>GEEN VIDEO</t>
-  </si>
-  <si>
     <t>5100 Ddr-Rtd</t>
   </si>
   <si>
@@ -3001,6 +2998,38 @@
   </si>
   <si>
     <t>Jaartal</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=w5nanUnniCQ</t>
+  </si>
+  <si>
+    <t>6600 Ddr-Bd</t>
+  </si>
+  <si>
+    <t>- Ddr
+- Zlw</t>
+  </si>
+  <si>
+    <t>- Zlw
+- Bdpb</t>
+  </si>
+  <si>
+    <t>Ddr:
+- 7100/7101 Ddr15
+Ddr-Zlw:
+- 6601 Ddr
+- 5900 Ddzd
+- G Wld-Ddzd
+- G Wld
+- 9100/9301 v Zlw HSL
+- 9101/9300 Mdbz HSL ri brus
+Zlw-Bd:
+- 6601 Bdpb
+- 901 Bdpb
+Bd:
+- 1100 Bd7
+- 3600 Bd3
+- 9201/9601 Bd6</t>
   </si>
 </sst>
 </file>
@@ -6119,19 +6148,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="20.19921875" customWidth="1"/>
-    <col min="3" max="3" width="8.1328125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="21.53125" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="27.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -6156,418 +6184,928 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>450</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>568</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>595</v>
+        <v>547</v>
+      </c>
+      <c r="D2" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>500</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>571</v>
+        <v>547</v>
       </c>
       <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>564</v>
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>600</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>571</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>564</v>
-      </c>
-      <c r="E4">
-        <v>200</v>
+        <v>613</v>
+      </c>
+      <c r="D4" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>900</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s">
-        <v>572</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>590</v>
+        <v>547</v>
+      </c>
+      <c r="D5" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>1000</v>
+        <v>240</v>
       </c>
       <c r="B6" t="s">
-        <v>572</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>590</v>
+        <v>613</v>
+      </c>
+      <c r="D6" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>1100</v>
+        <v>400</v>
       </c>
       <c r="B7" t="s">
-        <v>573</v>
-      </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>591</v>
+        <v>635</v>
+      </c>
+      <c r="D7" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>1900</v>
+        <v>500</v>
       </c>
       <c r="B8" t="s">
         <v>571</v>
       </c>
       <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>564</v>
-      </c>
-      <c r="E8">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>2200</v>
+        <v>600</v>
       </c>
       <c r="B9" t="s">
-        <v>557</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>579</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>565</v>
-      </c>
-      <c r="E9" t="s">
-        <v>599</v>
+        <v>571</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>564</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>2400</v>
+        <v>700</v>
       </c>
       <c r="B10" t="s">
-        <v>557</v>
+        <v>571</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>565</v>
+      <c r="D10" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>2800</v>
+        <v>800</v>
       </c>
       <c r="B11" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>564</v>
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>565</v>
       </c>
       <c r="E11">
-        <v>180</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>3600</v>
+        <v>1500</v>
       </c>
       <c r="B12" t="s">
-        <v>557</v>
+        <v>574</v>
       </c>
       <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>565</v>
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>620</v>
       </c>
       <c r="E12">
-        <v>170</v>
+        <v>200</v>
+      </c>
+      <c r="F12" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>3700</v>
+        <v>1600</v>
       </c>
       <c r="B13" t="s">
-        <v>557</v>
+        <v>569</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" s="42" t="s">
-        <v>565</v>
+      <c r="D13" t="s">
+        <v>616</v>
       </c>
       <c r="E13">
         <v>170</v>
       </c>
+      <c r="F13" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>4000</v>
+        <v>1700</v>
       </c>
       <c r="B14" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>593</v>
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>616</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>5000</v>
+        <v>1800</v>
       </c>
       <c r="B15" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C15">
-        <v>7</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>589</v>
-      </c>
-      <c r="F15" t="s">
-        <v>598</v>
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>5100</v>
+        <v>2000</v>
       </c>
       <c r="B16" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C16">
-        <v>7</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>589</v>
-      </c>
-      <c r="F16" t="s">
-        <v>598</v>
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>564</v>
+      </c>
+      <c r="E16">
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>5900</v>
+        <v>2400</v>
       </c>
       <c r="B17" t="s">
-        <v>580</v>
+        <v>557</v>
       </c>
       <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>588</v>
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>565</v>
       </c>
       <c r="E17">
-        <v>80</v>
-      </c>
-      <c r="F17" t="s">
-        <v>598</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>6600</v>
+        <v>2600</v>
       </c>
       <c r="B18" t="s">
-        <v>558</v>
+        <v>574</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
-      <c r="D18" s="42" t="s">
-        <v>566</v>
+      <c r="D18" t="s">
+        <v>620</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
+      <c r="F18" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>7100</v>
+        <v>2800</v>
       </c>
       <c r="B19" t="s">
-        <v>563</v>
-      </c>
-      <c r="C19" t="s">
-        <v>584</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>592</v>
+        <v>571</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>564</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>7200</v>
+        <v>2900</v>
       </c>
       <c r="B20" t="s">
-        <v>563</v>
-      </c>
-      <c r="C20" t="s">
-        <v>584</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>592</v>
+        <v>557</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>565</v>
+      </c>
+      <c r="E20">
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>7700</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="D21" s="42"/>
+        <v>3000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>557</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>9100</v>
+        <v>3100</v>
       </c>
       <c r="B22" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C22">
-        <v>16</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>594</v>
-      </c>
-      <c r="F22" t="s">
-        <v>596</v>
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>565</v>
+      </c>
+      <c r="E22">
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>9200</v>
+        <v>3500</v>
       </c>
       <c r="B23" t="s">
-        <v>582</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>586</v>
+        <v>557</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>565</v>
+      </c>
+      <c r="E23">
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>9300</v>
+        <v>3600</v>
       </c>
       <c r="B24" t="s">
-        <v>559</v>
-      </c>
-      <c r="C24" t="s">
-        <v>583</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>594</v>
-      </c>
-      <c r="F24" t="s">
-        <v>597</v>
+        <v>557</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>565</v>
+      </c>
+      <c r="E24">
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>9600</v>
+        <v>3900</v>
       </c>
       <c r="B25" t="s">
-        <v>582</v>
-      </c>
-      <c r="D25" s="42" t="s">
-        <v>586</v>
+        <v>557</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>565</v>
+      </c>
+      <c r="E25">
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>12200</v>
+        <v>4000</v>
       </c>
       <c r="B26" t="s">
+        <v>575</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>4300</v>
+      </c>
+      <c r="B27" t="s">
+        <v>575</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>614</v>
+      </c>
+      <c r="E27">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>4900</v>
+      </c>
+      <c r="B28" t="s">
+        <v>575</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>614</v>
+      </c>
+      <c r="E28">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>5500</v>
+      </c>
+      <c r="B29" t="s">
+        <v>578</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>588</v>
+      </c>
+      <c r="E29">
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>5600</v>
+      </c>
+      <c r="B30" t="s">
+        <v>576</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>566</v>
+      </c>
+      <c r="E30">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>5700</v>
+      </c>
+      <c r="B31" t="s">
+        <v>575</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>614</v>
+      </c>
+      <c r="E31">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>6000</v>
+      </c>
+      <c r="B32" t="s">
+        <v>575</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>6500</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>6600</v>
+      </c>
+      <c r="B34" t="s">
+        <v>558</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>6900</v>
+      </c>
+      <c r="B35" t="s">
+        <v>575</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>7000</v>
+      </c>
+      <c r="B36" t="s">
+        <v>576</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>566</v>
+      </c>
+      <c r="E36">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>7300</v>
+      </c>
+      <c r="B37" t="s">
+        <v>575</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>614</v>
+      </c>
+      <c r="E37">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>7400</v>
+      </c>
+      <c r="B38" t="s">
+        <v>575</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>614</v>
+      </c>
+      <c r="E38">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>7500</v>
+      </c>
+      <c r="B39" t="s">
+        <v>604</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>618</v>
+      </c>
+      <c r="E39">
+        <v>80</v>
+      </c>
+      <c r="F39" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>7600</v>
+      </c>
+      <c r="B40" t="s">
+        <v>576</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>566</v>
+      </c>
+      <c r="E40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>8800</v>
+      </c>
+      <c r="B41" t="s">
+        <v>605</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>615</v>
+      </c>
+      <c r="F41" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>11600</v>
+      </c>
+      <c r="B42" t="s">
+        <v>606</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>619</v>
+      </c>
+      <c r="E42">
+        <v>140</v>
+      </c>
+      <c r="F42" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>11700</v>
+      </c>
+      <c r="B43" t="s">
+        <v>569</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>616</v>
+      </c>
+      <c r="E43">
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>14600</v>
+      </c>
+      <c r="B44" t="s">
+        <v>576</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>14900</v>
+      </c>
+      <c r="B45" t="s">
+        <v>575</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>614</v>
+      </c>
+      <c r="E45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>15600</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>15800</v>
+      </c>
+      <c r="B47" t="s">
+        <v>576</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>17800</v>
+      </c>
+      <c r="B48" t="s">
+        <v>651</v>
+      </c>
+      <c r="C48" t="s">
+        <v>584</v>
+      </c>
+      <c r="D48" t="s">
+        <v>591</v>
+      </c>
+      <c r="E48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>20000</v>
+      </c>
+      <c r="B49" t="s">
+        <v>609</v>
+      </c>
+      <c r="C49" t="s">
+        <v>584</v>
+      </c>
+      <c r="D49" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>28300</v>
+      </c>
+      <c r="B50" t="s">
+        <v>575</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>614</v>
+      </c>
+      <c r="E50">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>30700</v>
+      </c>
+      <c r="B51" t="s">
+        <v>610</v>
+      </c>
+      <c r="C51" t="s">
+        <v>584</v>
+      </c>
+      <c r="D51" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>30900</v>
+      </c>
+      <c r="B52" t="s">
+        <v>651</v>
+      </c>
+      <c r="C52" t="s">
+        <v>583</v>
+      </c>
+      <c r="D52" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>31100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>652</v>
+      </c>
+      <c r="C53" t="s">
+        <v>584</v>
+      </c>
+      <c r="D53" t="s">
+        <v>591</v>
+      </c>
+      <c r="E53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>31300</v>
+      </c>
+      <c r="B54" t="s">
+        <v>612</v>
+      </c>
+      <c r="D54" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>31400</v>
+      </c>
+      <c r="B55" t="s">
+        <v>612</v>
+      </c>
+      <c r="D55" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>32200</v>
+      </c>
+      <c r="B56" t="s">
+        <v>611</v>
+      </c>
+      <c r="C56" t="s">
+        <v>583</v>
+      </c>
+      <c r="D56" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>32300</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>637</v>
+      </c>
+      <c r="B58" t="s">
+        <v>651</v>
+      </c>
+      <c r="C58" t="s">
+        <v>584</v>
+      </c>
+      <c r="D58" t="s">
+        <v>591</v>
+      </c>
+      <c r="E58">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>636</v>
+      </c>
+      <c r="B59" t="s">
         <v>557</v>
       </c>
-      <c r="C26">
+      <c r="C59">
         <v>6</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D59" t="s">
         <v>565</v>
       </c>
-      <c r="E26">
+      <c r="E59">
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>567</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D60" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>567</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D61" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>763</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>621</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F27" xr:uid="{AA9E098D-0675-414C-8423-8DB175120546}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
-      <sortCondition ref="A1:A27"/>
+  <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
+      <sortCondition ref="A1:A61"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
-    <sortCondition ref="A2:A18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
+    <sortCondition ref="A3:A60"/>
   </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6577,10 +7115,10 @@
   <dimension ref="A1:R156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J176" sqref="J176"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6662,7 +7200,7 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>264</v>
       </c>
@@ -6697,7 +7235,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>304</v>
       </c>
@@ -7079,7 +7617,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -8596,7 +9134,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>317</v>
       </c>
@@ -8797,7 +9335,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>286</v>
       </c>
@@ -9631,9 +10169,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:R156" xr:uid="{86DEC163-0F38-4216-A6F4-B629FE360FF7}">
-    <filterColumn colId="9">
+    <filterColumn colId="5">
       <filters>
-        <filter val="Amf-Amfpon, Amf-Apd?"/>
+        <filter val="Bd-Zlw"/>
+        <filter val="Esn-Zlw"/>
+        <filter val="Kfh-Zlw"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:R156">
@@ -9650,18 +10190,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
-  <dimension ref="A1:F61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="21.53125" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="27.46484375" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -9686,928 +10227,418 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>100</v>
+        <v>450</v>
       </c>
       <c r="B2" t="s">
-        <v>547</v>
-      </c>
-      <c r="D2" t="s">
-        <v>594</v>
+        <v>568</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>120</v>
+        <v>500</v>
       </c>
       <c r="B3" t="s">
-        <v>547</v>
+        <v>571</v>
       </c>
       <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>594</v>
+        <v>8</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>140</v>
+        <v>600</v>
       </c>
       <c r="B4" t="s">
-        <v>613</v>
-      </c>
-      <c r="D4" t="s">
-        <v>586</v>
+        <v>571</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>564</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>220</v>
+        <v>900</v>
       </c>
       <c r="B5" t="s">
-        <v>547</v>
-      </c>
-      <c r="D5" t="s">
-        <v>594</v>
+        <v>572</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>240</v>
+        <v>1000</v>
       </c>
       <c r="B6" t="s">
-        <v>613</v>
-      </c>
-      <c r="D6" t="s">
-        <v>586</v>
+        <v>572</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>400</v>
+        <v>1100</v>
       </c>
       <c r="B7" t="s">
-        <v>635</v>
-      </c>
-      <c r="D7" t="s">
-        <v>594</v>
+        <v>573</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>500</v>
+        <v>1900</v>
       </c>
       <c r="B8" t="s">
         <v>571</v>
       </c>
       <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>564</v>
+      </c>
+      <c r="E8">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>600</v>
+        <v>2200</v>
       </c>
       <c r="B9" t="s">
-        <v>571</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>564</v>
-      </c>
-      <c r="E9">
-        <v>250</v>
+        <v>557</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>579</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>565</v>
+      </c>
+      <c r="E9" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>700</v>
+        <v>2400</v>
       </c>
       <c r="B10" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
-        <v>564</v>
+      <c r="D10" s="42" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>800</v>
+        <v>2800</v>
       </c>
       <c r="B11" t="s">
-        <v>557</v>
+        <v>571</v>
       </c>
       <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>565</v>
+        <v>6</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>564</v>
       </c>
       <c r="E11">
-        <v>230</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>1500</v>
+        <v>3600</v>
       </c>
       <c r="B12" t="s">
-        <v>574</v>
+        <v>557</v>
       </c>
       <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>620</v>
+        <v>6</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>565</v>
       </c>
       <c r="E12">
-        <v>200</v>
-      </c>
-      <c r="F12" t="s">
-        <v>601</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>1600</v>
+        <v>3700</v>
       </c>
       <c r="B13" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
-        <v>616</v>
+      <c r="D13" s="42" t="s">
+        <v>565</v>
       </c>
       <c r="E13">
         <v>170</v>
       </c>
-      <c r="F13" t="s">
-        <v>602</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>1700</v>
+        <v>4000</v>
       </c>
       <c r="B14" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>616</v>
-      </c>
-      <c r="E14">
-        <v>200</v>
-      </c>
-      <c r="F14" t="s">
-        <v>602</v>
+        <v>10</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>1800</v>
+        <v>5000</v>
       </c>
       <c r="B15" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>564</v>
+        <v>7</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>589</v>
+      </c>
+      <c r="F15" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>2000</v>
+        <v>5100</v>
       </c>
       <c r="B16" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="C16">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>564</v>
-      </c>
-      <c r="E16">
-        <v>230</v>
+        <v>7</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>589</v>
+      </c>
+      <c r="F16" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>2400</v>
+        <v>5900</v>
       </c>
       <c r="B17" t="s">
-        <v>557</v>
+        <v>580</v>
       </c>
       <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>565</v>
+        <v>4</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>588</v>
       </c>
       <c r="E17">
-        <v>280</v>
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>2600</v>
+        <v>6600</v>
       </c>
       <c r="B18" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
-      <c r="D18" t="s">
-        <v>620</v>
-      </c>
-      <c r="E18">
-        <v>200</v>
-      </c>
-      <c r="F18" t="s">
-        <v>601</v>
+      <c r="D18" s="42" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>2800</v>
+        <v>7100</v>
       </c>
       <c r="B19" t="s">
-        <v>571</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>564</v>
-      </c>
-      <c r="E19">
-        <v>200</v>
+        <v>563</v>
+      </c>
+      <c r="C19" t="s">
+        <v>584</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>2900</v>
+        <v>7200</v>
       </c>
       <c r="B20" t="s">
-        <v>557</v>
-      </c>
-      <c r="C20">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>565</v>
-      </c>
-      <c r="E20">
-        <v>170</v>
+        <v>563</v>
+      </c>
+      <c r="C20" t="s">
+        <v>584</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>3000</v>
-      </c>
-      <c r="B21" t="s">
-        <v>557</v>
-      </c>
-      <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>565</v>
-      </c>
+        <v>7700</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>3100</v>
+        <v>9100</v>
       </c>
       <c r="B22" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>565</v>
-      </c>
-      <c r="E22">
-        <v>280</v>
+        <v>16</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>594</v>
+      </c>
+      <c r="F22" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>3500</v>
+        <v>9200</v>
       </c>
       <c r="B23" t="s">
-        <v>557</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>565</v>
-      </c>
-      <c r="E23">
-        <v>280</v>
+        <v>582</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>3600</v>
+        <v>9300</v>
       </c>
       <c r="B24" t="s">
-        <v>557</v>
-      </c>
-      <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>565</v>
-      </c>
-      <c r="E24">
-        <v>170</v>
+        <v>559</v>
+      </c>
+      <c r="C24" t="s">
+        <v>583</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>594</v>
+      </c>
+      <c r="F24" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>3900</v>
+        <v>9600</v>
       </c>
       <c r="B25" t="s">
-        <v>557</v>
-      </c>
-      <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>565</v>
-      </c>
-      <c r="E25">
-        <v>170</v>
+        <v>582</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>4000</v>
+        <v>12200</v>
       </c>
       <c r="B26" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
       <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>614</v>
+        <v>6</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>565</v>
+      </c>
+      <c r="E26">
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>4300</v>
-      </c>
-      <c r="B27" t="s">
-        <v>575</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>614</v>
-      </c>
-      <c r="E27">
-        <v>110</v>
+      <c r="A27" t="s">
+        <v>567</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>4900</v>
-      </c>
-      <c r="B28" t="s">
-        <v>575</v>
-      </c>
-      <c r="C28">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>614</v>
-      </c>
-      <c r="E28">
-        <v>150</v>
+      <c r="A28" t="s">
+        <v>567</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>5500</v>
-      </c>
-      <c r="B29" t="s">
-        <v>578</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>588</v>
-      </c>
-      <c r="E29">
-        <v>80</v>
-      </c>
-      <c r="F29" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30">
-        <v>5600</v>
-      </c>
-      <c r="B30" t="s">
-        <v>576</v>
-      </c>
-      <c r="C30">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>566</v>
-      </c>
-      <c r="E30">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31">
-        <v>5700</v>
-      </c>
-      <c r="B31" t="s">
-        <v>575</v>
-      </c>
-      <c r="C31">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>614</v>
-      </c>
-      <c r="E31">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32">
-        <v>6000</v>
-      </c>
-      <c r="B32" t="s">
-        <v>575</v>
-      </c>
-      <c r="C32">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <v>6500</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <v>6600</v>
-      </c>
-      <c r="B34" t="s">
-        <v>558</v>
-      </c>
-      <c r="C34">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35">
-        <v>6900</v>
-      </c>
-      <c r="B35" t="s">
-        <v>575</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>7000</v>
-      </c>
-      <c r="B36" t="s">
-        <v>576</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>566</v>
-      </c>
-      <c r="E36">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37">
-        <v>7300</v>
-      </c>
-      <c r="B37" t="s">
-        <v>575</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>614</v>
-      </c>
-      <c r="E37">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <v>7400</v>
-      </c>
-      <c r="B38" t="s">
-        <v>575</v>
-      </c>
-      <c r="C38">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>614</v>
-      </c>
-      <c r="E38">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39">
-        <v>7500</v>
-      </c>
-      <c r="B39" t="s">
-        <v>604</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>618</v>
-      </c>
-      <c r="E39">
-        <v>80</v>
-      </c>
-      <c r="F39" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40">
-        <v>7600</v>
-      </c>
-      <c r="B40" t="s">
-        <v>576</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>566</v>
-      </c>
-      <c r="E40">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>8800</v>
-      </c>
-      <c r="B41" t="s">
-        <v>605</v>
-      </c>
-      <c r="C41">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>615</v>
-      </c>
-      <c r="F41" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42">
-        <v>11600</v>
-      </c>
-      <c r="B42" t="s">
-        <v>606</v>
-      </c>
-      <c r="C42">
-        <v>5</v>
-      </c>
-      <c r="D42" t="s">
-        <v>619</v>
-      </c>
-      <c r="E42">
-        <v>140</v>
-      </c>
-      <c r="F42" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>11700</v>
-      </c>
-      <c r="B43" t="s">
-        <v>569</v>
-      </c>
-      <c r="C43">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>616</v>
-      </c>
-      <c r="E43">
-        <v>200</v>
-      </c>
-      <c r="F43" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>14600</v>
-      </c>
-      <c r="B44" t="s">
-        <v>576</v>
-      </c>
-      <c r="C44">
-        <v>8</v>
-      </c>
-      <c r="D44" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45">
-        <v>14900</v>
-      </c>
-      <c r="B45" t="s">
-        <v>575</v>
-      </c>
-      <c r="C45">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
-        <v>614</v>
-      </c>
-      <c r="E45">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46">
-        <v>15600</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47">
-        <v>15800</v>
-      </c>
-      <c r="B47" t="s">
-        <v>576</v>
-      </c>
-      <c r="C47">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <v>17800</v>
-      </c>
-      <c r="B48" t="s">
-        <v>651</v>
-      </c>
-      <c r="C48" t="s">
-        <v>584</v>
-      </c>
-      <c r="D48" t="s">
-        <v>591</v>
-      </c>
-      <c r="E48">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A49">
-        <v>20000</v>
-      </c>
-      <c r="B49" t="s">
-        <v>609</v>
-      </c>
-      <c r="C49" t="s">
-        <v>584</v>
-      </c>
-      <c r="D49" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A50">
-        <v>28300</v>
-      </c>
-      <c r="B50" t="s">
-        <v>575</v>
-      </c>
-      <c r="C50">
-        <v>6</v>
-      </c>
-      <c r="D50" t="s">
-        <v>614</v>
-      </c>
-      <c r="E50">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <v>30700</v>
-      </c>
-      <c r="B51" t="s">
-        <v>610</v>
-      </c>
-      <c r="C51" t="s">
-        <v>584</v>
-      </c>
-      <c r="D51" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52">
-        <v>30900</v>
-      </c>
-      <c r="B52" t="s">
-        <v>651</v>
-      </c>
-      <c r="C52" t="s">
-        <v>583</v>
-      </c>
-      <c r="D52" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53">
-        <v>31100</v>
-      </c>
-      <c r="B53" t="s">
-        <v>652</v>
-      </c>
-      <c r="C53" t="s">
-        <v>584</v>
-      </c>
-      <c r="D53" t="s">
-        <v>591</v>
-      </c>
-      <c r="E53">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54">
-        <v>31300</v>
-      </c>
-      <c r="B54" t="s">
-        <v>612</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="A29" t="s">
+        <v>762</v>
+      </c>
+      <c r="D29" s="42" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A55">
-        <v>31400</v>
-      </c>
-      <c r="B55" t="s">
-        <v>612</v>
-      </c>
-      <c r="D55" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A56">
-        <v>32200</v>
-      </c>
-      <c r="B56" t="s">
-        <v>611</v>
-      </c>
-      <c r="C56" t="s">
-        <v>583</v>
-      </c>
-      <c r="D56" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A57">
-        <v>32300</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>637</v>
-      </c>
-      <c r="B58" t="s">
-        <v>651</v>
-      </c>
-      <c r="C58" t="s">
-        <v>584</v>
-      </c>
-      <c r="D58" t="s">
-        <v>591</v>
-      </c>
-      <c r="E58">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>636</v>
-      </c>
-      <c r="B59" t="s">
-        <v>557</v>
-      </c>
-      <c r="C59">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>565</v>
-      </c>
-      <c r="E59">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>567</v>
-      </c>
-      <c r="D60" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>567</v>
-      </c>
-      <c r="D61" t="s">
-        <v>600</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
-      <sortCondition ref="A1:A61"/>
+  <autoFilter ref="A1:F27" xr:uid="{AA9E098D-0675-414C-8423-8DB175120546}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
+      <sortCondition ref="A1:A27"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
-    <sortCondition ref="A3:A60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
+    <sortCondition ref="A2:A18"/>
   </sortState>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10617,7 +10648,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10650,7 +10681,7 @@
         <v>650</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>645</v>
@@ -10659,7 +10690,7 @@
         <v>646</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="I1" s="31" t="s">
         <v>647</v>
@@ -10801,26 +10832,48 @@
         <v>727</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:11" ht="285" x14ac:dyDescent="0.45">
+      <c r="A8" s="33" t="s">
         <v>758</v>
       </c>
-      <c r="B8" s="32">
-        <v>6600</v>
-      </c>
-      <c r="C8" s="32" t="s">
+      <c r="B8" s="33" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="285" x14ac:dyDescent="0.45">
-      <c r="A9" s="33" t="s">
+      <c r="C8" s="33" t="s">
+        <v>760</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="E8" s="33">
+        <v>3021</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>761</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>763</v>
+      </c>
+      <c r="H8" s="46"/>
+      <c r="I8" s="40" t="s">
+        <v>769</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>764</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
+      <c r="A9" s="32" t="s">
         <v>758</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>760</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>761</v>
+      <c r="B9" s="32" t="s">
+        <v>765</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>766</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>718</v>
@@ -10829,31 +10882,25 @@
         <v>3021</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>762</v>
-      </c>
-      <c r="G9" s="40" t="s">
-        <v>764</v>
-      </c>
-      <c r="H9" s="46"/>
+        <v>767</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>768</v>
+      </c>
+      <c r="H9" s="38"/>
       <c r="I9" s="40" t="s">
         <v>770</v>
       </c>
-      <c r="J9" s="39" t="s">
-        <v>765</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A10" s="32" t="s">
-        <v>758</v>
+        <v>644</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>718</v>
@@ -10861,47 +10908,46 @@
       <c r="E10" s="33">
         <v>3021</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>768</v>
+      <c r="F10" s="40" t="s">
+        <v>774</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>769</v>
-      </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="40" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
+        <v>776</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>775</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>777</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="242.25" x14ac:dyDescent="0.45">
       <c r="A11" s="32" t="s">
-        <v>644</v>
+        <v>758</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>773</v>
+        <v>781</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>774</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>718</v>
+        <v>780</v>
       </c>
       <c r="E11" s="33">
         <v>3021</v>
       </c>
       <c r="F11" s="40" t="s">
-        <v>775</v>
+        <v>782</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>777</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>776</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>778</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>779</v>
+        <v>784</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>782</v>
+      </c>
+      <c r="J11" s="41" t="s">
+        <v>783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exporteer bestaande consists naar ZvNL
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9F4035-46CA-4458-B46D-57756C42778B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F082D7-B6A7-49E5-8910-E5DF1B505E3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6578" yWindow="5483" windowWidth="14400" windowHeight="7484" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20955" yWindow="1590" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -7156,10 +7156,10 @@
   <dimension ref="A1:R156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7298,7 +7298,7 @@
       <c r="H4" s="20" t="s">
         <v>778</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="29" t="s">
         <v>493</v>
       </c>
       <c r="J4" s="20" t="s">
@@ -7359,7 +7359,7 @@
       <c r="H6" s="20" t="s">
         <v>785</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="29" t="s">
         <v>491</v>
       </c>
       <c r="J6" s="20" t="s">
@@ -7481,7 +7481,7 @@
       <c r="H10" s="20" t="s">
         <v>781</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="29" t="s">
         <v>788</v>
       </c>
       <c r="J10" s="34" t="s">
@@ -7551,7 +7551,7 @@
       <c r="H12" s="20" t="s">
         <v>783</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="29" t="s">
         <v>483</v>
       </c>
       <c r="J12" s="34" t="s">
@@ -7586,7 +7586,7 @@
       <c r="H13" s="20" t="s">
         <v>782</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="29" t="s">
         <v>789</v>
       </c>
       <c r="J13" s="20" t="s">
@@ -7621,7 +7621,7 @@
       <c r="H14" s="20" t="s">
         <v>786</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="29" t="s">
         <v>790</v>
       </c>
       <c r="J14" s="20" t="s">

</xml_diff>

<commit_message>
[5100] Cargo spawns van spots
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49886FA-E8BC-4125-BF84-49A2B70CB4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870978F-B6FC-4D88-9FEF-47020F3D5EF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6488" yWindow="6615" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -2906,28 +2906,6 @@
     <t>Losse Lok</t>
   </si>
   <si>
-    <t>Ddr:
-- 1900/1901 Ddr2b
-- 5900/5901 Ddr3b
-- 6600/6601 Ddr4b
-Ddr-Rtd:
-- 5101 Zwd3, Ddr3a
-- 2401 Zwd binnenspoor
-- G Brd-Kfh aankomst
-- G Brd-Kfh aankomst 2
-- 5001 Rlb
-- 900 Rtst
-- 2200 Rtst
-- 9101/9300 Rtb
-- 1000/1001 Rtd3
-- 4000/4001 Rtd16
-Rtd:
-- 500/600 Rtd14
-- 2401 Sdm-Rtd6
-- 9100/9301 Rtd11
-- 9600 Rtd4</t>
-  </si>
-  <si>
     <t>- Ddr</t>
   </si>
   <si>
@@ -3106,6 +3084,34 @@
   </si>
   <si>
     <t>C8, FN</t>
+  </si>
+  <si>
+    <t>Ddr:
+- 1900/1901 Ddr2b
+- 5900/5901 Ddr3b
+- 6600/6601 Ddr4b
+- cZwdDdr26 Grbr
+Ddr-Rtd:
+- cDdrDdzd13
+- cZwdDdr13
+- cDdrDdzd19 kfhaz
+- 5101 Zwd3, Ddr3a
+- 2401 Zwd binnenspoor
+- G Brd-Kfh aankomst
+- G Brd-Kfh aankomst 2 (cRtdRtb10?)
+- 5001 Rlb
+- 900 Rtst
+- 2200 Rtst
+- cRtdRtb25-28 Rtz
+- 9101/9300 Rtb
+- 1000/1001 Rtd3
+- 4000/4001 Rtd16
+- cRtdRtb01-04 (Rtd5)
+Rtd:
+- 500/600 Rtd14
+- 2401 Sdm-Rtd6
+- 9100/9301 Rtd11
+- 9600 Rtd4</t>
   </si>
 </sst>
 </file>
@@ -3248,7 +3254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3345,9 +3351,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7307,7 +7310,7 @@
         <v>428</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I3" s="28" t="s">
         <v>493</v>
@@ -7342,7 +7345,7 @@
         <v>484</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I4" s="29" t="s">
         <v>493</v>
@@ -7371,7 +7374,7 @@
         <v>428</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>502</v>
@@ -7403,7 +7406,7 @@
         <v>428</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="I6" s="29" t="s">
         <v>491</v>
@@ -7435,10 +7438,10 @@
         <v>495</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>428</v>
@@ -7464,10 +7467,10 @@
         <v>495</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>428</v>
@@ -7493,7 +7496,7 @@
         <v>428</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>492</v>
@@ -7525,10 +7528,10 @@
         <v>492</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="J10" s="34" t="s">
         <v>620</v>
@@ -7560,7 +7563,7 @@
         <v>483</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I11" s="29" t="s">
         <v>483</v>
@@ -7595,7 +7598,7 @@
         <v>495</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I12" s="29" t="s">
         <v>483</v>
@@ -7630,10 +7633,10 @@
         <v>503</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="J13" s="20" t="s">
         <v>621</v>
@@ -7665,10 +7668,10 @@
         <v>503</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>616</v>
@@ -7764,7 +7767,7 @@
         <v>428</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="K17" s="28" t="s">
         <v>497</v>
@@ -10753,8 +10756,8 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10787,7 +10790,7 @@
         <v>642</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>637</v>
@@ -10796,7 +10799,7 @@
         <v>638</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="I1" s="31" t="s">
         <v>639</v>
@@ -10938,7 +10941,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="285" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="384.75" x14ac:dyDescent="0.45">
       <c r="A8" s="33" t="s">
         <v>750</v>
       </c>
@@ -10957,15 +10960,15 @@
       <c r="F8" s="33" t="s">
         <v>753</v>
       </c>
-      <c r="G8" s="48" t="s">
-        <v>755</v>
+      <c r="G8" s="40" t="s">
+        <v>790</v>
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="40" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="K8" s="33" t="s">
         <v>714</v>
@@ -10976,10 +10979,10 @@
         <v>750</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>756</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>757</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>758</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>710</v>
@@ -10988,14 +10991,14 @@
         <v>3021</v>
       </c>
       <c r="F9" s="33" t="s">
+        <v>758</v>
+      </c>
+      <c r="G9" s="47" t="s">
         <v>759</v>
-      </c>
-      <c r="G9" s="47" t="s">
-        <v>760</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="40" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
@@ -11003,10 +11006,10 @@
         <v>636</v>
       </c>
       <c r="B10" s="32" t="s">
+        <v>763</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>764</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>765</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>710</v>
@@ -11015,19 +11018,19 @@
         <v>3021</v>
       </c>
       <c r="F10" s="40" t="s">
+        <v>765</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>767</v>
+      </c>
+      <c r="H10" s="39" t="s">
         <v>766</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="I10" s="39" t="s">
         <v>768</v>
       </c>
-      <c r="H10" s="39" t="s">
-        <v>767</v>
-      </c>
-      <c r="I10" s="39" t="s">
+      <c r="J10" s="40" t="s">
         <v>769</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="242.25" x14ac:dyDescent="0.45">
@@ -11035,10 +11038,10 @@
         <v>750</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>710</v>
@@ -11047,16 +11050,16 @@
         <v>3021</v>
       </c>
       <c r="F11" s="40" t="s">
+        <v>773</v>
+      </c>
+      <c r="G11" s="47" t="s">
+        <v>775</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>773</v>
+      </c>
+      <c r="J11" s="41" t="s">
         <v>774</v>
-      </c>
-      <c r="G11" s="47" t="s">
-        <v>776</v>
-      </c>
-      <c r="I11" s="40" t="s">
-        <v>774</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[6600] cargo vanuit spots
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870978F-B6FC-4D88-9FEF-47020F3D5EF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1C7DD0-FE47-4E72-AE66-E9B738B5B846}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6488" yWindow="6615" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6765" yWindow="4282" windowWidth="14400" windowHeight="7486" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -3026,24 +3026,6 @@
 - Bdpb</t>
   </si>
   <si>
-    <t>Ddr:
-- 7100/7101 Ddr15
-Ddr-Zlw:
-- 6601 Ddr
-- 5900 Ddzd
-- G Wld-Ddzd
-- G Wld
-- 9100/9301 v Zlw HSL
-- 9101/9300 Mdbz HSL ri brus
-Zlw-Bd:
-- 6601 Bdpb
-- 901 Bdpb
-Bd:
-- 1100 Bd7
-- 3600 Bd3
-- 9201/9601 Bd6</t>
-  </si>
-  <si>
     <t>Amf-Amfpon, (Amf-Apd)</t>
   </si>
   <si>
@@ -3112,6 +3094,28 @@
 - 2401 Sdm-Rtd6
 - 9100/9301 Rtd11
 - 9600 Rtd4</t>
+  </si>
+  <si>
+    <t>Ddr:
+- cDdrZwd26
+- 7100/7101 Ddr15
+Ddr-Zlw:
+- 6601 Ddr
+- 5900 Ddzd
+- G Wld-Ddzd (cDdzdDdr06?)
+- G Wld (cDdzdDdr10?)
+- cWldDdzd10-13
+- 9100/9301 v Zlw HSL
+- 9101/9300 Mdbz HSL ri brus
+Zlw-Bd:
+- cBdZlw05 Nvbro
+- 6601 Bdpb
+- 901 Bdpb
+- cBdZlw18 Bd8
+Bd:
+- 1100 Bd7
+- 3600 Bd3
+- 9201/9601 Bd6</t>
   </si>
 </sst>
 </file>
@@ -3254,7 +3258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3352,6 +3356,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7310,7 +7317,7 @@
         <v>428</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I3" s="28" t="s">
         <v>493</v>
@@ -7345,7 +7352,7 @@
         <v>484</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I4" s="29" t="s">
         <v>493</v>
@@ -7374,7 +7381,7 @@
         <v>428</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>502</v>
@@ -7406,7 +7413,7 @@
         <v>428</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I6" s="29" t="s">
         <v>491</v>
@@ -7438,10 +7445,10 @@
         <v>495</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>428</v>
@@ -7467,10 +7474,10 @@
         <v>495</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>428</v>
@@ -7496,7 +7503,7 @@
         <v>428</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>492</v>
@@ -7528,10 +7535,10 @@
         <v>492</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J10" s="34" t="s">
         <v>620</v>
@@ -7563,7 +7570,7 @@
         <v>483</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I11" s="29" t="s">
         <v>483</v>
@@ -7598,7 +7605,7 @@
         <v>495</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I12" s="29" t="s">
         <v>483</v>
@@ -7633,10 +7640,10 @@
         <v>503</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="J13" s="20" t="s">
         <v>621</v>
@@ -7668,10 +7675,10 @@
         <v>503</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>616</v>
@@ -7767,7 +7774,7 @@
         <v>428</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="K17" s="28" t="s">
         <v>497</v>
@@ -10756,8 +10763,8 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10961,7 +10968,7 @@
         <v>753</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="40" t="s">
@@ -10970,7 +10977,7 @@
       <c r="J8" s="39" t="s">
         <v>755</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="48" t="s">
         <v>714</v>
       </c>
     </row>
@@ -11033,7 +11040,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A11" s="32" t="s">
         <v>750</v>
       </c>
@@ -11053,7 +11060,7 @@
         <v>773</v>
       </c>
       <c r="G11" s="47" t="s">
-        <v>775</v>
+        <v>790</v>
       </c>
       <c r="I11" s="40" t="s">
         <v>773</v>

</xml_diff>

<commit_message>
[6600] minor scenario fixes
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1C7DD0-FE47-4E72-AE66-E9B738B5B846}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CA2E54-A7D3-470A-9517-7F2024A44267}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6765" yWindow="4282" windowWidth="14400" windowHeight="7486" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10764,7 +10764,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11059,7 +11059,7 @@
       <c r="F11" s="40" t="s">
         <v>773</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="38" t="s">
         <v>790</v>
       </c>
       <c r="I11" s="40" t="s">

</xml_diff>

<commit_message>
Update GTW-E 2-8 RNET fragment to actual RNET vehicles
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23A9151-D63D-405A-96D1-762034673F1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41EFBE6-6C96-49BE-9820-865F73643738}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="4748" windowWidth="14400" windowHeight="7485" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7088" yWindow="7628" windowWidth="14401" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="796">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3116,6 +3116,65 @@
 - 1100 Bd7
 - 3600 Bd3
 - 9201/9601 Bd6</t>
+  </si>
+  <si>
+    <t>6601 Bd-Ddr</t>
+  </si>
+  <si>
+    <t>- Bd
+- Zlw</t>
+  </si>
+  <si>
+    <t>- cBdZlw05 Bd-Zlw</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bd:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cBdZlwTb07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- 1101 Bd3
+- 9200/9600 Bd7
+- cBdTb12 Rsd-&gt;Bd4
+Bd-Zlw:
+- 900 Bdpb
+- 6600 Nvbro-Bdpb
+- cBdZlwTb28 Zha
+- cWldZlw15 Zlw
+Zlw-Ddr:
+- 9101/9300 HSL Zlw
+- cWldZlw18 Mdbz
+- cDdzdWld17 Wld
+- cDdrDdzd19 Ddzd-Wld
+- 5901 Ddzd
+- 6600 Ddr-Ddzd
+- cDdrDdzd00 Ddr6
+Ddr:
+- 2400/2401 Ddr2a</t>
+    </r>
+  </si>
+  <si>
+    <t>- Zlw
+- Ddr</t>
   </si>
 </sst>
 </file>
@@ -7211,7 +7270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE17749-1BD2-42DC-A92D-74E793F7820B}">
   <dimension ref="A1:R156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -10310,7 +10369,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10760,11 +10819,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10776,7 +10835,7 @@
     <col min="5" max="5" width="9.06640625" style="45"/>
     <col min="6" max="6" width="12.19921875" style="32" customWidth="1"/>
     <col min="7" max="7" width="24.265625" style="32" customWidth="1"/>
-    <col min="8" max="8" width="14.19921875" style="45" customWidth="1"/>
+    <col min="8" max="8" width="16.73046875" style="45" customWidth="1"/>
     <col min="9" max="9" width="15.73046875" style="32" customWidth="1"/>
     <col min="10" max="10" width="9.06640625" style="32"/>
     <col min="11" max="11" width="11.06640625" style="32" customWidth="1"/>
@@ -11067,6 +11126,29 @@
       </c>
       <c r="J11" s="41" t="s">
         <v>774</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="285" x14ac:dyDescent="0.45">
+      <c r="A12" s="32" t="s">
+        <v>750</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>791</v>
+      </c>
+      <c r="E12" s="33">
+        <v>3021</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>792</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>794</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>793</v>
+      </c>
+      <c r="I12" s="40" t="s">
+        <v>795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[6601] add scenario to version control
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41EFBE6-6C96-49BE-9820-865F73643738}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70720212-FA69-4D24-9B2E-85B14D07FCDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7088" yWindow="7628" windowWidth="14401" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7628" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -3128,30 +3128,11 @@
     <t>- cBdZlw05 Bd-Zlw</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Bd:
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cBdZlwTb07</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>- Zlw
+- Ddr</t>
+  </si>
+  <si>
+    <t>Bd:
 - 1101 Bd3
 - 9200/9600 Bd7
 - cBdTb12 Rsd-&gt;Bd4
@@ -3170,11 +3151,6 @@
 - cDdrDdzd00 Ddr6
 Ddr:
 - 2400/2401 Ddr2a</t>
-    </r>
-  </si>
-  <si>
-    <t>- Zlw
-- Ddr</t>
   </si>
 </sst>
 </file>
@@ -10823,7 +10799,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11128,7 +11104,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="285" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A12" s="32" t="s">
         <v>750</v>
       </c>
@@ -11142,13 +11118,13 @@
         <v>792</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="H12" s="39" t="s">
         <v>793</v>
       </c>
       <c r="I12" s="40" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[6601] finish scenario details
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70720212-FA69-4D24-9B2E-85B14D07FCDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA90E85D-2496-4FD9-8E6C-068C9CDEFEDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="7628" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="798">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3151,6 +3151,12 @@
 - cDdrDdzd00 Ddr6
 Ddr:
 - 2400/2401 Ddr2a</t>
+  </si>
+  <si>
+    <t>- Bd</t>
+  </si>
+  <si>
+    <t>Bd-Ddr</t>
   </si>
 </sst>
 </file>
@@ -10797,9 +10803,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11105,11 +11111,15 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="33" t="s">
         <v>750</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="33" t="s">
         <v>791</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33" t="s">
+        <v>710</v>
       </c>
       <c r="E12" s="33">
         <v>3021</v>
@@ -11125,6 +11135,12 @@
       </c>
       <c r="I12" s="40" t="s">
         <v>794</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>796</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Meer cargo spots in drgl
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA90E85D-2496-4FD9-8E6C-068C9CDEFEDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A67A66-3381-4B0F-8CBB-E742BB90ACC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7628" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7057" yWindow="1965" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="806">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3157,6 +3157,43 @@
   </si>
   <si>
     <t>Bd-Ddr</t>
+  </si>
+  <si>
+    <t>2200 Rtd-Vs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s, https://www.youtube.com/watch?v=CEayBOxq_Zo</t>
+  </si>
+  <si>
+    <t>- Ddr
+- Rsd
+- Gs</t>
+  </si>
+  <si>
+    <t>- cRbSloe25 Rsd-Bgn</t>
+  </si>
+  <si>
+    <t>Rsd:
+- cRsdgRsd02/cRsdUitEsn07
+- 450/451 Rsdg-Rsd1a
+- 3600/3601 Rsd3a
+- 5900/5901 Rsd3b
+- 2201 Rsd4b
+Rsd-Gs:
+- 2201 Bgn
+- cGsBzl25 Rb-Bgn
+- 2201 Kbd
+- cGsBzl25 Krg
+- 2201 Gs</t>
+  </si>
+  <si>
+    <t>Werktreinen</t>
+  </si>
+  <si>
+    <t>FCl*</t>
+  </si>
+  <si>
+    <t>- Rsd</t>
   </si>
 </sst>
 </file>
@@ -3299,7 +3336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3399,6 +3436,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -7253,7 +7299,7 @@
   <dimension ref="A1:R156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="G51" sqref="G51"/>
@@ -10348,10 +10394,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10782,6 +10828,14 @@
       </c>
       <c r="D29" s="42" t="s">
         <v>613</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>803</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>804</v>
       </c>
     </row>
   </sheetData>
@@ -10801,11 +10855,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11141,6 +11195,32 @@
       </c>
       <c r="K12" s="33" t="s">
         <v>797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="171" x14ac:dyDescent="0.45">
+      <c r="A13" s="32" t="s">
+        <v>750</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>798</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>799</v>
+      </c>
+      <c r="E13" s="45">
+        <v>3021</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>800</v>
+      </c>
+      <c r="G13" s="49" t="s">
+        <v>802</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>801</v>
+      </c>
+      <c r="I13" s="50" t="s">
+        <v>805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mark Hupac Novara Shuttle in overzicht
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A67A66-3381-4B0F-8CBB-E742BB90ACC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1C0BC-4332-4129-974A-BF192FE523DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7057" yWindow="1965" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6915" yWindow="7020" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -7298,11 +7298,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE17749-1BD2-42DC-A92D-74E793F7820B}">
   <dimension ref="A1:R156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="F45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G51" sqref="G51"/>
+      <selection pane="bottomRight" activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9207,7 +9207,7 @@
       <c r="F65" s="20" t="s">
         <v>441</v>
       </c>
-      <c r="G65" s="28" t="s">
+      <c r="G65" s="29" t="s">
         <v>499</v>
       </c>
       <c r="H65" s="20" t="s">
@@ -10857,9 +10857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
[2200] Delete broken scenario, have to restart :/
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1C0BC-4332-4129-974A-BF192FE523DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05713218-3561-41E4-9EF8-81FBEA86150D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6915" yWindow="7020" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="802">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3165,35 +3165,10 @@
     <t>https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s, https://www.youtube.com/watch?v=CEayBOxq_Zo</t>
   </si>
   <si>
-    <t>- Ddr
-- Rsd
-- Gs</t>
-  </si>
-  <si>
-    <t>- cRbSloe25 Rsd-Bgn</t>
-  </si>
-  <si>
-    <t>Rsd:
-- cRsdgRsd02/cRsdUitEsn07
-- 450/451 Rsdg-Rsd1a
-- 3600/3601 Rsd3a
-- 5900/5901 Rsd3b
-- 2201 Rsd4b
-Rsd-Gs:
-- 2201 Bgn
-- cGsBzl25 Rb-Bgn
-- 2201 Kbd
-- cGsBzl25 Krg
-- 2201 Gs</t>
-  </si>
-  <si>
     <t>Werktreinen</t>
   </si>
   <si>
     <t>FCl*</t>
-  </si>
-  <si>
-    <t>- Rsd</t>
   </si>
 </sst>
 </file>
@@ -7298,7 +7273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE17749-1BD2-42DC-A92D-74E793F7820B}">
   <dimension ref="A1:R156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="F45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -10832,10 +10807,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
   </sheetData>
@@ -10857,9 +10832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11197,7 +11172,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="171" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A13" s="32" t="s">
         <v>750</v>
       </c>
@@ -11207,21 +11182,10 @@
       <c r="C13" s="49" t="s">
         <v>799</v>
       </c>
-      <c r="E13" s="45">
-        <v>3021</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>800</v>
-      </c>
-      <c r="G13" s="49" t="s">
-        <v>802</v>
-      </c>
-      <c r="H13" s="51" t="s">
-        <v>801</v>
-      </c>
-      <c r="I13" s="50" t="s">
-        <v>805</v>
-      </c>
+      <c r="F13" s="41"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[2200] Create new scenario
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05713218-3561-41E4-9EF8-81FBEA86150D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35896A34-AB6A-4967-BEAB-E4CB90EFF78A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="802">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3162,13 +3162,13 @@
     <t>2200 Rtd-Vs</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s, https://www.youtube.com/watch?v=CEayBOxq_Zo</t>
-  </si>
-  <si>
     <t>Werktreinen</t>
   </si>
   <si>
     <t>FCl*</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CEayBOxq_Zo, https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s</t>
   </si>
 </sst>
 </file>
@@ -10807,10 +10807,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>799</v>
+      </c>
+      <c r="D30" s="42" t="s">
         <v>800</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>801</v>
       </c>
     </row>
   </sheetData>
@@ -10834,7 +10834,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13:I13"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11180,9 +11180,11 @@
         <v>798</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>799</v>
-      </c>
-      <c r="F13" s="41"/>
+        <v>801</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>755</v>
+      </c>
       <c r="G13" s="49"/>
       <c r="H13" s="51"/>
       <c r="I13" s="50"/>

</xml_diff>

<commit_message>
[5500] AI update, out-of-memory :/
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35896A34-AB6A-4967-BEAB-E4CB90EFF78A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59321B2-50EB-4B7B-8943-F8ED4029B1EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6652" yWindow="6675" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -2685,9 +2685,429 @@
 - St</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=RRT-HCddLnk</t>
+  </si>
+  <si>
+    <t>- Hvs
+- Amf</t>
+  </si>
+  <si>
+    <t>Ams-Amf 2019: https://www.youtube.com/watch?v=KpwT0JuZboM
+Amf-Apd 1600: https://www.youtube.com/watch?v=3qY8avX706c</t>
+  </si>
+  <si>
+    <t>Hvs - Amf:
+- 1600/11600 Hvs
+- G FC/FW/C8 Brn
+- 140/240/1500 Amf-Brn
+- 15800 Amf7
+Amf:
+- 501/601 Ut-Amf2-Zl
+- 31300/31301 Amf4b
+Amf - Apd:
+- 1600/1700/11600/11700 Amfa
+- 140/240/G-C8/FC Hvl
+- 31300 Bnva
+Apd:
+- 140/240 Apd1
+- 17800/17801 Apd3</t>
+  </si>
+  <si>
+    <t>- Bkd
+- Amfge</t>
+  </si>
+  <si>
+    <t>- Hvs - Amf
+- Amf
+- Amf - Apd
+- Apd</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aEMC3VgvYGs</t>
+  </si>
+  <si>
+    <t>5501 Ut-Brn</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tTlJvQyBbK0</t>
+  </si>
+  <si>
+    <t>31300 Ed-Amf</t>
+  </si>
+  <si>
+    <t>- Ut
+- Dld</t>
+  </si>
+  <si>
+    <t>Ut:
+- 101/121/221 Ut18
+- 1701/11701 Ut11
+- 3000 Ut5
+- 3101 Ut19
+- 3500 Ut7
+- 4901/5700 Ut1
+- 6001 Ut21
+- 6900 Ut20
+- 7400 Ut14
+- 8800/8801 Ut12
+Ut - Dld:
+- 5600/5601 Uto-Ut4
+- 2000 Uto-Ut8
+- 500/600 Uto-Ut9
+- 5701 Blw-Uto2
+- 5500 Bloa
+- 1700/11700 Bhv
+Dld - Brn:
+- 5500 St
+- 15800 Brn
+- 241 Brn
+Brn:
+- 1600/11600 Brn
+Misc:
+- Blauwkapel: voor speler ivm 1701</t>
+  </si>
+  <si>
+    <t>Apmz10</t>
+  </si>
+  <si>
+    <t>Bpmbdez8</t>
+  </si>
+  <si>
+    <t>Bpmbdzf7</t>
+  </si>
+  <si>
+    <t>Bpmdz9</t>
+  </si>
+  <si>
+    <t>Bpmez10</t>
+  </si>
+  <si>
+    <t>Bpmz10</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B-eindrijtuig</t>
+  </si>
+  <si>
+    <t>Bf</t>
+  </si>
+  <si>
+    <t>BDs</t>
+  </si>
+  <si>
+    <t>Gvc-Ehv</t>
+  </si>
+  <si>
+    <t>B(f)</t>
+  </si>
+  <si>
+    <t>Amro</t>
+  </si>
+  <si>
+    <t>Asd-Bd</t>
+  </si>
+  <si>
+    <t>Bnl</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>zelfde als 16100</t>
+  </si>
+  <si>
+    <t>ZWNL</t>
+  </si>
+  <si>
+    <t>5100 Ddr-Rtd</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-EjJFCWNSQw&amp;t=1565s</t>
+  </si>
+  <si>
+    <t>Ddr</t>
+  </si>
+  <si>
+    <t>Losse Lok</t>
+  </si>
+  <si>
+    <t>- Ddr</t>
+  </si>
+  <si>
+    <t>5101 Rtd-Ddr</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=E2YkVEOnOGg</t>
+  </si>
+  <si>
+    <t>Rtd</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rtd:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">9101/9300 Rtd2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- 500/600 Rtd14
+- 1000/1001 Rtd11
+- 2400 Rtd9
+- 4000/4001 Rtd16
+- 9201/9601 Rtd12
+Rtd-Ddr:
+- 9101/9300 Wiltz buiten
+- 2201 Rtst binnen
+- 901 Rtst buiten
+- 5000 Brd binnen
+- G Kfhan ri Mvt
+- 2400 Kfhz binnen
+- 5100 Zwd binnen
+Ddr:
+- 5900/5901 Ddr3b
+- 6600/6601 Ddr4b
+- 7100 Ddr15</t>
+    </r>
+  </si>
+  <si>
+    <t>- Ddr
+- Kfh
+- IJsm
+- Rtd</t>
+  </si>
+  <si>
+    <t>- IJsm
+- Kfh
+- Ddr</t>
+  </si>
+  <si>
+    <t>AI in front</t>
+  </si>
+  <si>
+    <t>31301 Amf-Ed</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zVWHjr8NGCw</t>
+  </si>
+  <si>
+    <t>- Amf
+- Bnc
+- Ltn</t>
+  </si>
+  <si>
+    <t>- 141/G Amf-Bnv</t>
+  </si>
+  <si>
+    <t>Amf:
+- 1500/1501 Amf5a
+- 1600/1700/11600/11700 Amf7
+- 2000/2001 Amf4a
+Amf-Ed:
+- 31300 Bnva
+- 31300 Ltn
+- 7500/7501 Ed1b</t>
+  </si>
+  <si>
+    <t>- Amf</t>
+  </si>
+  <si>
+    <t>- Amf
+- Bnc
+- Ltn
+- Edc</t>
+  </si>
+  <si>
+    <t>Jaartal</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=w5nanUnniCQ</t>
+  </si>
+  <si>
+    <t>6600 Ddr-Bd</t>
+  </si>
+  <si>
+    <t>- Ddr
+- Zlw</t>
+  </si>
+  <si>
+    <t>- Zlw
+- Bdpb</t>
+  </si>
+  <si>
+    <t>Amf-Amfpon, (Amf-Apd)</t>
+  </si>
+  <si>
+    <t>Brmet-Ut-Asd</t>
+  </si>
+  <si>
+    <t>Tb-Ht-Nm</t>
+  </si>
+  <si>
+    <t>Tb-Ht-Brmet</t>
+  </si>
+  <si>
+    <t>Tb-Ht-Nm, Tb-Ht-Ut-Amf, Tb-Ht-Brmet</t>
+  </si>
+  <si>
+    <t>Tb-Ht-Ut-Amf, Tb-Ht-Brmet</t>
+  </si>
+  <si>
+    <t>Tb-Ht-Ut-Amf</t>
+  </si>
+  <si>
+    <t>Ehv-Ht-Ut-Amf</t>
+  </si>
+  <si>
+    <t>Ehv-Ht-Ut-Asd</t>
+  </si>
+  <si>
+    <t>Tb-Ht-Ut-Amf, Tb-Ht-Nm</t>
+  </si>
+  <si>
+    <t>Freight Gravel</t>
+  </si>
+  <si>
+    <t>FN, C8, FG</t>
+  </si>
+  <si>
+    <t>C8, FG</t>
+  </si>
+  <si>
+    <t>C8, FN</t>
+  </si>
+  <si>
+    <t>Ddr:
+- 1900/1901 Ddr2b
+- 5900/5901 Ddr3b
+- 6600/6601 Ddr4b
+- cZwdDdr26 Grbr
+Ddr-Rtd:
+- cDdrDdzd13
+- cZwdDdr13
+- cDdrDdzd19 kfhaz
+- 5101 Zwd3, Ddr3a
+- 2401 Zwd binnenspoor
+- G Brd-Kfh aankomst
+- G Brd-Kfh aankomst 2 (cRtdRtb10?)
+- 5001 Rlb
+- 900 Rtst
+- 2200 Rtst
+- cRtdRtb25-28 Rtz
+- 9101/9300 Rtb
+- 1000/1001 Rtd3
+- 4000/4001 Rtd16
+- cRtdRtb01-04 (Rtd5)
+Rtd:
+- 500/600 Rtd14
+- 2401 Sdm-Rtd6
+- 9100/9301 Rtd11
+- 9600 Rtd4</t>
+  </si>
+  <si>
+    <t>Ddr:
+- cDdrZwd26
+- 7100/7101 Ddr15
+Ddr-Zlw:
+- 6601 Ddr
+- 5900 Ddzd
+- G Wld-Ddzd (cDdzdDdr06?)
+- G Wld (cDdzdDdr10?)
+- cWldDdzd10-13
+- 9100/9301 v Zlw HSL
+- 9101/9300 Mdbz HSL ri brus
+Zlw-Bd:
+- cBdZlw05 Nvbro
+- 6601 Bdpb
+- 901 Bdpb
+- cBdZlw18 Bd8
+Bd:
+- 1100 Bd7
+- 3600 Bd3
+- 9201/9601 Bd6</t>
+  </si>
+  <si>
+    <t>6601 Bd-Ddr</t>
+  </si>
+  <si>
+    <t>- Bd
+- Zlw</t>
+  </si>
+  <si>
+    <t>- cBdZlw05 Bd-Zlw</t>
+  </si>
+  <si>
+    <t>- Zlw
+- Ddr</t>
+  </si>
+  <si>
+    <t>Bd:
+- 1101 Bd3
+- 9200/9600 Bd7
+- cBdTb12 Rsd-&gt;Bd4
+Bd-Zlw:
+- 900 Bdpb
+- 6600 Nvbro-Bdpb
+- cBdZlwTb28 Zha
+- cWldZlw15 Zlw
+Zlw-Ddr:
+- 9101/9300 HSL Zlw
+- cWldZlw18 Mdbz
+- cDdzdWld17 Wld
+- cDdrDdzd19 Ddzd-Wld
+- 5901 Ddzd
+- 6600 Ddr-Ddzd
+- cDdrDdzd00 Ddr6
+Ddr:
+- 2400/2401 Ddr2a</t>
+  </si>
+  <si>
+    <t>- Bd</t>
+  </si>
+  <si>
+    <t>Bd-Ddr</t>
+  </si>
+  <si>
+    <t>2200 Rtd-Vs</t>
+  </si>
+  <si>
+    <t>Werktreinen</t>
+  </si>
+  <si>
+    <t>FCl*</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CEayBOxq_Zo, https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Brn - Dld:
 - 1600/11600 ri Shl
+- cAmfBrn14-16
 - 5501 Stz-&gt;St
 Dld - Ut:
 - 1700/11700 Dld ri Ut
@@ -2750,425 +3170,6 @@
 - 28300/28301 Ut2
 - 2900 Ut7</t>
     </r>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=RRT-HCddLnk</t>
-  </si>
-  <si>
-    <t>- Hvs
-- Amf</t>
-  </si>
-  <si>
-    <t>Ams-Amf 2019: https://www.youtube.com/watch?v=KpwT0JuZboM
-Amf-Apd 1600: https://www.youtube.com/watch?v=3qY8avX706c</t>
-  </si>
-  <si>
-    <t>Hvs - Amf:
-- 1600/11600 Hvs
-- G FC/FW/C8 Brn
-- 140/240/1500 Amf-Brn
-- 15800 Amf7
-Amf:
-- 501/601 Ut-Amf2-Zl
-- 31300/31301 Amf4b
-Amf - Apd:
-- 1600/1700/11600/11700 Amfa
-- 140/240/G-C8/FC Hvl
-- 31300 Bnva
-Apd:
-- 140/240 Apd1
-- 17800/17801 Apd3</t>
-  </si>
-  <si>
-    <t>- Bkd
-- Amfge</t>
-  </si>
-  <si>
-    <t>- Hvs - Amf
-- Amf
-- Amf - Apd
-- Apd</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=aEMC3VgvYGs</t>
-  </si>
-  <si>
-    <t>5501 Ut-Brn</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=tTlJvQyBbK0</t>
-  </si>
-  <si>
-    <t>31300 Ed-Amf</t>
-  </si>
-  <si>
-    <t>- Ut
-- Dld</t>
-  </si>
-  <si>
-    <t>Ut:
-- 101/121/221 Ut18
-- 1701/11701 Ut11
-- 3000 Ut5
-- 3101 Ut19
-- 3500 Ut7
-- 4901/5700 Ut1
-- 6001 Ut21
-- 6900 Ut20
-- 7400 Ut14
-- 8800/8801 Ut12
-Ut - Dld:
-- 5600/5601 Uto-Ut4
-- 2000 Uto-Ut8
-- 500/600 Uto-Ut9
-- 5701 Blw-Uto2
-- 5500 Bloa
-- 1700/11700 Bhv
-Dld - Brn:
-- 5500 St
-- 15800 Brn
-- 241 Brn
-Brn:
-- 1600/11600 Brn
-Misc:
-- Blauwkapel: voor speler ivm 1701</t>
-  </si>
-  <si>
-    <t>Apmz10</t>
-  </si>
-  <si>
-    <t>Bpmbdez8</t>
-  </si>
-  <si>
-    <t>Bpmbdzf7</t>
-  </si>
-  <si>
-    <t>Bpmdz9</t>
-  </si>
-  <si>
-    <t>Bpmez10</t>
-  </si>
-  <si>
-    <t>Bpmz10</t>
-  </si>
-  <si>
-    <t>Exact</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>B-eindrijtuig</t>
-  </si>
-  <si>
-    <t>Bf</t>
-  </si>
-  <si>
-    <t>BDs</t>
-  </si>
-  <si>
-    <t>Gvc-Ehv</t>
-  </si>
-  <si>
-    <t>B(f)</t>
-  </si>
-  <si>
-    <t>Amro</t>
-  </si>
-  <si>
-    <t>Asd-Bd</t>
-  </si>
-  <si>
-    <t>Bnl</t>
-  </si>
-  <si>
-    <t>BD</t>
-  </si>
-  <si>
-    <t>zelfde als 16100</t>
-  </si>
-  <si>
-    <t>ZWNL</t>
-  </si>
-  <si>
-    <t>5100 Ddr-Rtd</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=-EjJFCWNSQw&amp;t=1565s</t>
-  </si>
-  <si>
-    <t>Ddr</t>
-  </si>
-  <si>
-    <t>Losse Lok</t>
-  </si>
-  <si>
-    <t>- Ddr</t>
-  </si>
-  <si>
-    <t>5101 Rtd-Ddr</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=E2YkVEOnOGg</t>
-  </si>
-  <si>
-    <t>Rtd</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rtd:
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">9101/9300 Rtd2
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- 500/600 Rtd14
-- 1000/1001 Rtd11
-- 2400 Rtd9
-- 4000/4001 Rtd16
-- 9201/9601 Rtd12
-Rtd-Ddr:
-- 9101/9300 Wiltz buiten
-- 2201 Rtst binnen
-- 901 Rtst buiten
-- 5000 Brd binnen
-- G Kfhan ri Mvt
-- 2400 Kfhz binnen
-- 5100 Zwd binnen
-Ddr:
-- 5900/5901 Ddr3b
-- 6600/6601 Ddr4b
-- 7100 Ddr15</t>
-    </r>
-  </si>
-  <si>
-    <t>- Ddr
-- Kfh
-- IJsm
-- Rtd</t>
-  </si>
-  <si>
-    <t>- IJsm
-- Kfh
-- Ddr</t>
-  </si>
-  <si>
-    <t>AI in front</t>
-  </si>
-  <si>
-    <t>31301 Amf-Ed</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=zVWHjr8NGCw</t>
-  </si>
-  <si>
-    <t>- Amf
-- Bnc
-- Ltn</t>
-  </si>
-  <si>
-    <t>- 141/G Amf-Bnv</t>
-  </si>
-  <si>
-    <t>Amf:
-- 1500/1501 Amf5a
-- 1600/1700/11600/11700 Amf7
-- 2000/2001 Amf4a
-Amf-Ed:
-- 31300 Bnva
-- 31300 Ltn
-- 7500/7501 Ed1b</t>
-  </si>
-  <si>
-    <t>- Amf</t>
-  </si>
-  <si>
-    <t>- Amf
-- Bnc
-- Ltn
-- Edc</t>
-  </si>
-  <si>
-    <t>Jaartal</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=w5nanUnniCQ</t>
-  </si>
-  <si>
-    <t>6600 Ddr-Bd</t>
-  </si>
-  <si>
-    <t>- Ddr
-- Zlw</t>
-  </si>
-  <si>
-    <t>- Zlw
-- Bdpb</t>
-  </si>
-  <si>
-    <t>Amf-Amfpon, (Amf-Apd)</t>
-  </si>
-  <si>
-    <t>Brmet-Ut-Asd</t>
-  </si>
-  <si>
-    <t>Tb-Ht-Nm</t>
-  </si>
-  <si>
-    <t>Tb-Ht-Brmet</t>
-  </si>
-  <si>
-    <t>Tb-Ht-Nm, Tb-Ht-Ut-Amf, Tb-Ht-Brmet</t>
-  </si>
-  <si>
-    <t>Tb-Ht-Ut-Amf, Tb-Ht-Brmet</t>
-  </si>
-  <si>
-    <t>Tb-Ht-Ut-Amf</t>
-  </si>
-  <si>
-    <t>Ehv-Ht-Ut-Amf</t>
-  </si>
-  <si>
-    <t>Ehv-Ht-Ut-Asd</t>
-  </si>
-  <si>
-    <t>Tb-Ht-Ut-Amf, Tb-Ht-Nm</t>
-  </si>
-  <si>
-    <t>Freight Gravel</t>
-  </si>
-  <si>
-    <t>FN, C8, FG</t>
-  </si>
-  <si>
-    <t>C8, FG</t>
-  </si>
-  <si>
-    <t>C8, FN</t>
-  </si>
-  <si>
-    <t>Ddr:
-- 1900/1901 Ddr2b
-- 5900/5901 Ddr3b
-- 6600/6601 Ddr4b
-- cZwdDdr26 Grbr
-Ddr-Rtd:
-- cDdrDdzd13
-- cZwdDdr13
-- cDdrDdzd19 kfhaz
-- 5101 Zwd3, Ddr3a
-- 2401 Zwd binnenspoor
-- G Brd-Kfh aankomst
-- G Brd-Kfh aankomst 2 (cRtdRtb10?)
-- 5001 Rlb
-- 900 Rtst
-- 2200 Rtst
-- cRtdRtb25-28 Rtz
-- 9101/9300 Rtb
-- 1000/1001 Rtd3
-- 4000/4001 Rtd16
-- cRtdRtb01-04 (Rtd5)
-Rtd:
-- 500/600 Rtd14
-- 2401 Sdm-Rtd6
-- 9100/9301 Rtd11
-- 9600 Rtd4</t>
-  </si>
-  <si>
-    <t>Ddr:
-- cDdrZwd26
-- 7100/7101 Ddr15
-Ddr-Zlw:
-- 6601 Ddr
-- 5900 Ddzd
-- G Wld-Ddzd (cDdzdDdr06?)
-- G Wld (cDdzdDdr10?)
-- cWldDdzd10-13
-- 9100/9301 v Zlw HSL
-- 9101/9300 Mdbz HSL ri brus
-Zlw-Bd:
-- cBdZlw05 Nvbro
-- 6601 Bdpb
-- 901 Bdpb
-- cBdZlw18 Bd8
-Bd:
-- 1100 Bd7
-- 3600 Bd3
-- 9201/9601 Bd6</t>
-  </si>
-  <si>
-    <t>6601 Bd-Ddr</t>
-  </si>
-  <si>
-    <t>- Bd
-- Zlw</t>
-  </si>
-  <si>
-    <t>- cBdZlw05 Bd-Zlw</t>
-  </si>
-  <si>
-    <t>- Zlw
-- Ddr</t>
-  </si>
-  <si>
-    <t>Bd:
-- 1101 Bd3
-- 9200/9600 Bd7
-- cBdTb12 Rsd-&gt;Bd4
-Bd-Zlw:
-- 900 Bdpb
-- 6600 Nvbro-Bdpb
-- cBdZlwTb28 Zha
-- cWldZlw15 Zlw
-Zlw-Ddr:
-- 9101/9300 HSL Zlw
-- cWldZlw18 Mdbz
-- cDdzdWld17 Wld
-- cDdrDdzd19 Ddzd-Wld
-- 5901 Ddzd
-- 6600 Ddr-Ddzd
-- cDdrDdzd00 Ddr6
-Ddr:
-- 2400/2401 Ddr2a</t>
-  </si>
-  <si>
-    <t>- Bd</t>
-  </si>
-  <si>
-    <t>Bd-Ddr</t>
-  </si>
-  <si>
-    <t>2200 Rtd-Vs</t>
-  </si>
-  <si>
-    <t>Werktreinen</t>
-  </si>
-  <si>
-    <t>FCl*</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=CEayBOxq_Zo, https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s</t>
   </si>
 </sst>
 </file>
@@ -7382,7 +7383,7 @@
         <v>483</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>483</v>
@@ -7672,7 +7673,7 @@
         <v>484</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="I13" s="29" t="s">
         <v>493</v>
@@ -8298,10 +8299,10 @@
         <v>492</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I35" s="29" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>620</v>
@@ -8446,10 +8447,10 @@
         <v>495</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I40" s="28" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="J40" s="20" t="s">
         <v>428</v>
@@ -8475,10 +8476,10 @@
         <v>495</v>
       </c>
       <c r="H41" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="J41" s="20" t="s">
         <v>428</v>
@@ -8507,7 +8508,7 @@
         <v>495</v>
       </c>
       <c r="H42" s="20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I42" s="29" t="s">
         <v>483</v>
@@ -8658,10 +8659,10 @@
         <v>503</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J47" s="20" t="s">
         <v>621</v>
@@ -8693,10 +8694,10 @@
         <v>503</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I48" s="29" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="J48" s="20" t="s">
         <v>616</v>
@@ -9502,7 +9503,7 @@
         <v>428</v>
       </c>
       <c r="H76" s="20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="I76" s="28" t="s">
         <v>493</v>
@@ -9534,7 +9535,7 @@
         <v>428</v>
       </c>
       <c r="H77" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I77" s="28" t="s">
         <v>502</v>
@@ -9566,7 +9567,7 @@
         <v>428</v>
       </c>
       <c r="H78" s="20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I78" s="29" t="s">
         <v>491</v>
@@ -9598,7 +9599,7 @@
         <v>428</v>
       </c>
       <c r="H79" s="20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I79" s="28" t="s">
         <v>492</v>
@@ -9633,7 +9634,7 @@
         <v>428</v>
       </c>
       <c r="J80" s="34" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="K80" s="28" t="s">
         <v>497</v>
@@ -10799,7 +10800,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D29" s="42" t="s">
         <v>613</v>
@@ -10807,10 +10808,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>798</v>
+      </c>
+      <c r="D30" s="42" t="s">
         <v>799</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>800</v>
       </c>
     </row>
   </sheetData>
@@ -10832,9 +10833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10867,7 +10868,7 @@
         <v>642</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>637</v>
@@ -10876,7 +10877,7 @@
         <v>638</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="I1" s="31" t="s">
         <v>639</v>
@@ -10918,7 +10919,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="313.5" x14ac:dyDescent="0.45">
       <c r="A3" s="33" t="s">
         <v>636</v>
       </c>
@@ -10931,11 +10932,14 @@
       <c r="D3" s="33" t="s">
         <v>710</v>
       </c>
+      <c r="E3" s="33">
+        <v>3021</v>
+      </c>
       <c r="F3" s="40" t="s">
         <v>717</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>718</v>
+        <v>801</v>
       </c>
       <c r="H3" s="44"/>
       <c r="I3" s="39" t="s">
@@ -10956,26 +10960,26 @@
         <v>140</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>710</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="H4" s="44"/>
       <c r="I4" s="40" t="s">
+        <v>722</v>
+      </c>
+      <c r="J4" s="40" t="s">
+        <v>719</v>
+      </c>
+      <c r="K4" s="40" t="s">
         <v>723</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>720</v>
-      </c>
-      <c r="K4" s="40" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="384.75" x14ac:dyDescent="0.45">
@@ -10983,16 +10987,16 @@
         <v>636</v>
       </c>
       <c r="B5" s="32" t="s">
+        <v>725</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>726</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>727</v>
-      </c>
       <c r="F5" s="41" t="s">
+        <v>728</v>
+      </c>
+      <c r="G5" s="47" t="s">
         <v>729</v>
-      </c>
-      <c r="G5" s="47" t="s">
-        <v>730</v>
       </c>
       <c r="H5" s="44"/>
     </row>
@@ -11001,10 +11005,10 @@
         <v>636</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -11015,18 +11019,18 @@
         <v>5600</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="384.75" x14ac:dyDescent="0.45">
       <c r="A8" s="33" t="s">
+        <v>749</v>
+      </c>
+      <c r="B8" s="33" t="s">
         <v>750</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="C8" s="33" t="s">
         <v>751</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>752</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>710</v>
@@ -11035,17 +11039,17 @@
         <v>3021</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="40" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="K8" s="48" t="s">
         <v>714</v>
@@ -11053,13 +11057,13 @@
     </row>
     <row r="9" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A9" s="32" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>755</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>756</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>757</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>710</v>
@@ -11068,14 +11072,14 @@
         <v>3021</v>
       </c>
       <c r="F9" s="33" t="s">
+        <v>757</v>
+      </c>
+      <c r="G9" s="47" t="s">
         <v>758</v>
-      </c>
-      <c r="G9" s="47" t="s">
-        <v>759</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="40" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
@@ -11083,10 +11087,10 @@
         <v>636</v>
       </c>
       <c r="B10" s="32" t="s">
+        <v>762</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>763</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>764</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>710</v>
@@ -11095,30 +11099,30 @@
         <v>3021</v>
       </c>
       <c r="F10" s="40" t="s">
+        <v>764</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>766</v>
+      </c>
+      <c r="H10" s="39" t="s">
         <v>765</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="I10" s="39" t="s">
         <v>767</v>
       </c>
-      <c r="H10" s="39" t="s">
-        <v>766</v>
-      </c>
-      <c r="I10" s="39" t="s">
+      <c r="J10" s="40" t="s">
         <v>768</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A11" s="32" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>710</v>
@@ -11127,24 +11131,24 @@
         <v>3021</v>
       </c>
       <c r="F11" s="40" t="s">
+        <v>772</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>789</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>772</v>
+      </c>
+      <c r="J11" s="41" t="s">
         <v>773</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>790</v>
-      </c>
-      <c r="I11" s="40" t="s">
-        <v>773</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A12" s="33" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="33" t="s">
@@ -11154,36 +11158,36 @@
         <v>3021</v>
       </c>
       <c r="F12" s="40" t="s">
+        <v>791</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>794</v>
+      </c>
+      <c r="H12" s="39" t="s">
         <v>792</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="I12" s="40" t="s">
+        <v>793</v>
+      </c>
+      <c r="J12" s="39" t="s">
         <v>795</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>793</v>
-      </c>
-      <c r="I12" s="40" t="s">
-        <v>794</v>
-      </c>
-      <c r="J12" s="39" t="s">
+      <c r="K12" s="33" t="s">
         <v>796</v>
-      </c>
-      <c r="K12" s="33" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A13" s="32" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G13" s="49"/>
       <c r="H13" s="51"/>
@@ -11700,7 +11704,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -11708,50 +11712,50 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B3" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B6" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B7" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -11759,65 +11763,65 @@
         <v>16500</v>
       </c>
       <c r="B9" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B10" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C10" t="s">
+        <v>737</v>
+      </c>
+      <c r="D10" t="s">
         <v>738</v>
       </c>
-      <c r="D10" t="s">
-        <v>739</v>
-      </c>
       <c r="E10" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F10" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G10" t="s">
+        <v>737</v>
+      </c>
+      <c r="H10" t="s">
         <v>738</v>
       </c>
-      <c r="H10" t="s">
-        <v>739</v>
-      </c>
       <c r="I10" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>732</v>
+      </c>
+      <c r="B11" t="s">
+        <v>735</v>
+      </c>
+      <c r="C11" t="s">
+        <v>730</v>
+      </c>
+      <c r="D11" t="s">
+        <v>735</v>
+      </c>
+      <c r="E11" t="s">
         <v>733</v>
       </c>
-      <c r="B11" t="s">
-        <v>736</v>
-      </c>
-      <c r="C11" t="s">
-        <v>731</v>
-      </c>
-      <c r="D11" t="s">
-        <v>736</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>735</v>
+      </c>
+      <c r="G11" t="s">
+        <v>730</v>
+      </c>
+      <c r="H11" t="s">
+        <v>735</v>
+      </c>
+      <c r="I11" t="s">
         <v>734</v>
-      </c>
-      <c r="F11" t="s">
-        <v>736</v>
-      </c>
-      <c r="G11" t="s">
-        <v>731</v>
-      </c>
-      <c r="H11" t="s">
-        <v>736</v>
-      </c>
-      <c r="I11" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -11825,53 +11829,53 @@
         <v>16100</v>
       </c>
       <c r="B13" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B14" t="s">
+        <v>737</v>
+      </c>
+      <c r="C14" t="s">
         <v>738</v>
       </c>
-      <c r="C14" t="s">
-        <v>739</v>
-      </c>
       <c r="D14" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E14" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F14" t="s">
+        <v>737</v>
+      </c>
+      <c r="G14" t="s">
         <v>738</v>
-      </c>
-      <c r="G14" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B15" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C15" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D15" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E15" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F15" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -11879,56 +11883,56 @@
         <v>16200</v>
       </c>
       <c r="B17" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C17" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B18" t="s">
+        <v>737</v>
+      </c>
+      <c r="C18" t="s">
         <v>738</v>
       </c>
-      <c r="C18" t="s">
-        <v>739</v>
-      </c>
       <c r="D18" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E18" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F18" t="s">
+        <v>737</v>
+      </c>
+      <c r="G18" t="s">
         <v>738</v>
-      </c>
-      <c r="G18" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C19" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D19" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E19" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -11936,53 +11940,53 @@
         <v>16400</v>
       </c>
       <c r="B21" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B22" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C22" t="s">
+        <v>737</v>
+      </c>
+      <c r="D22" t="s">
+        <v>740</v>
+      </c>
+      <c r="E22" t="s">
+        <v>737</v>
+      </c>
+      <c r="F22" t="s">
         <v>738</v>
       </c>
-      <c r="D22" t="s">
-        <v>741</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>738</v>
-      </c>
-      <c r="F22" t="s">
-        <v>739</v>
-      </c>
-      <c r="G22" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B23" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C23" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D23" t="s">
+        <v>733</v>
+      </c>
+      <c r="E23" t="s">
+        <v>730</v>
+      </c>
+      <c r="F23" t="s">
+        <v>735</v>
+      </c>
+      <c r="G23" t="s">
         <v>734</v>
-      </c>
-      <c r="E23" t="s">
-        <v>731</v>
-      </c>
-      <c r="F23" t="s">
-        <v>736</v>
-      </c>
-      <c r="G23" t="s">
-        <v>735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[5500] Add cargo AI
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59321B2-50EB-4B7B-8943-F8ED4029B1EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF2491C-5FCB-4666-9054-081BAC773577}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6652" yWindow="6675" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6652" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="803">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3104,18 +3104,22 @@
     <t>https://www.youtube.com/watch?v=CEayBOxq_Zo, https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s</t>
   </si>
   <si>
+    <t>- cUtoUt15 Dld-Ut</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Brn - Dld:
 - 1600/11600 ri Shl
 - cAmfBrn14-16
 - 5501 Stz-&gt;St
 Dld - Ut:
-- 1700/11700 Dld ri Ut
 - 1701/11701 Bhv
 - 5501 Blo
+- cUtoBlw13
 - 5700 Uto
 - 501/601 Ut-&gt;Uto
 - 2001 Ut-&gt;Uto (2)
+- cUtUto
 - 5601 Ut
 </t>
     </r>
@@ -10835,7 +10839,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10919,7 +10923,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="327.75" x14ac:dyDescent="0.45">
       <c r="A3" s="33" t="s">
         <v>636</v>
       </c>
@@ -10938,10 +10942,12 @@
       <c r="F3" s="40" t="s">
         <v>717</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="38" t="s">
+        <v>802</v>
+      </c>
+      <c r="H3" s="40" t="s">
         <v>801</v>
       </c>
-      <c r="H3" s="44"/>
       <c r="I3" s="39" t="s">
         <v>713</v>
       </c>

</xml_diff>

<commit_message>
[5501] Finish and add to git
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF2491C-5FCB-4666-9054-081BAC773577}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4C8CE8-AF14-43B9-A9D7-799EDE9C612A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6652" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6540" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
-    <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId2"/>
-    <sheet name="Goederentreinen" sheetId="9" r:id="rId3"/>
-    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId4"/>
+    <sheet name="Goederentreinen" sheetId="9" r:id="rId2"/>
+    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId3"/>
+    <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId4"/>
     <sheet name="Scenarios" sheetId="14" r:id="rId5"/>
     <sheet name="Vervoerders" sheetId="7" r:id="rId6"/>
     <sheet name="ICRm" sheetId="17" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="803">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2737,34 +2737,6 @@
   <si>
     <t>- Ut
 - Dld</t>
-  </si>
-  <si>
-    <t>Ut:
-- 101/121/221 Ut18
-- 1701/11701 Ut11
-- 3000 Ut5
-- 3101 Ut19
-- 3500 Ut7
-- 4901/5700 Ut1
-- 6001 Ut21
-- 6900 Ut20
-- 7400 Ut14
-- 8800/8801 Ut12
-Ut - Dld:
-- 5600/5601 Uto-Ut4
-- 2000 Uto-Ut8
-- 500/600 Uto-Ut9
-- 5701 Blw-Uto2
-- 5500 Bloa
-- 1700/11700 Bhv
-Dld - Brn:
-- 5500 St
-- 15800 Brn
-- 241 Brn
-Brn:
-- 1600/11600 Brn
-Misc:
-- Blauwkapel: voor speler ivm 1701</t>
   </si>
   <si>
     <t>Apmz10</t>
@@ -3175,12 +3147,43 @@
 - 2900 Ut7</t>
     </r>
   </si>
+  <si>
+    <t>Ut:
+- 101/121/221 Ut18
+- 1701/11701 Ut11
+- 3000 Ut5
+- 3101 Ut19
+- 3500 Ut7
+- 4901/5700 Ut1
+- 6001 Ut21
+- 6900 Ut20
+- 7400 Ut14
+- 8800/8801 Ut12
+Ut - Dld:
+- cUtUtvr06 via Ut9
+- 5600/5601 Uto-Ut4
+- 2000 Uto-Ut8
+- 500/600 Uto-Ut9
+- 5701 Blw-Uto2
+- cUtoUt15 Bloa
+- 5500 Bloa
+- 1700/11700 Bhv
+- cUtoUt25 Dld
+Dld - Brn:
+- 5500 St
+- 15800 Brn
+- 241 Brn
+Brn:
+- 1600/11600 Brn
+Misc:
+- Blauwkapel: voor speler ivm 1701</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3240,6 +3243,14 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3313,10 +3324,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3427,8 +3439,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6313,968 +6329,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
-  <dimension ref="A1:F61"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="21.53125" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="27.46484375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>553</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>539</v>
-      </c>
-      <c r="D2" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>120</v>
-      </c>
-      <c r="B3" t="s">
-        <v>539</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>140</v>
-      </c>
-      <c r="B4" t="s">
-        <v>605</v>
-      </c>
-      <c r="D4" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>220</v>
-      </c>
-      <c r="B5" t="s">
-        <v>539</v>
-      </c>
-      <c r="D5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>240</v>
-      </c>
-      <c r="B6" t="s">
-        <v>605</v>
-      </c>
-      <c r="D6" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>400</v>
-      </c>
-      <c r="B7" t="s">
-        <v>627</v>
-      </c>
-      <c r="D7" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>500</v>
-      </c>
-      <c r="B8" t="s">
-        <v>563</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>600</v>
-      </c>
-      <c r="B9" t="s">
-        <v>563</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>556</v>
-      </c>
-      <c r="E9">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>700</v>
-      </c>
-      <c r="B10" t="s">
-        <v>563</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>800</v>
-      </c>
-      <c r="B11" t="s">
-        <v>549</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>557</v>
-      </c>
-      <c r="E11">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>1500</v>
-      </c>
-      <c r="B12" t="s">
-        <v>566</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>612</v>
-      </c>
-      <c r="E12">
-        <v>200</v>
-      </c>
-      <c r="F12" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>1600</v>
-      </c>
-      <c r="B13" t="s">
-        <v>561</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>608</v>
-      </c>
-      <c r="E13">
-        <v>170</v>
-      </c>
-      <c r="F13" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>1700</v>
-      </c>
-      <c r="B14" t="s">
-        <v>561</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>608</v>
-      </c>
-      <c r="E14">
-        <v>200</v>
-      </c>
-      <c r="F14" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>1800</v>
-      </c>
-      <c r="B15" t="s">
-        <v>563</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>2000</v>
-      </c>
-      <c r="B16" t="s">
-        <v>563</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>556</v>
-      </c>
-      <c r="E16">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>2400</v>
-      </c>
-      <c r="B17" t="s">
-        <v>549</v>
-      </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>557</v>
-      </c>
-      <c r="E17">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>2600</v>
-      </c>
-      <c r="B18" t="s">
-        <v>566</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>612</v>
-      </c>
-      <c r="E18">
-        <v>200</v>
-      </c>
-      <c r="F18" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>2800</v>
-      </c>
-      <c r="B19" t="s">
-        <v>563</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>556</v>
-      </c>
-      <c r="E19">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>2900</v>
-      </c>
-      <c r="B20" t="s">
-        <v>549</v>
-      </c>
-      <c r="C20">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>557</v>
-      </c>
-      <c r="E20">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>3000</v>
-      </c>
-      <c r="B21" t="s">
-        <v>549</v>
-      </c>
-      <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>3100</v>
-      </c>
-      <c r="B22" t="s">
-        <v>549</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>557</v>
-      </c>
-      <c r="E22">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>3500</v>
-      </c>
-      <c r="B23" t="s">
-        <v>549</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>557</v>
-      </c>
-      <c r="E23">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>3600</v>
-      </c>
-      <c r="B24" t="s">
-        <v>549</v>
-      </c>
-      <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>557</v>
-      </c>
-      <c r="E24">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>3900</v>
-      </c>
-      <c r="B25" t="s">
-        <v>549</v>
-      </c>
-      <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>557</v>
-      </c>
-      <c r="E25">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>4000</v>
-      </c>
-      <c r="B26" t="s">
-        <v>567</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>4300</v>
-      </c>
-      <c r="B27" t="s">
-        <v>567</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>606</v>
-      </c>
-      <c r="E27">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>4900</v>
-      </c>
-      <c r="B28" t="s">
-        <v>567</v>
-      </c>
-      <c r="C28">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>606</v>
-      </c>
-      <c r="E28">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>5500</v>
-      </c>
-      <c r="B29" t="s">
-        <v>570</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>580</v>
-      </c>
-      <c r="E29">
-        <v>80</v>
-      </c>
-      <c r="F29" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30">
-        <v>5600</v>
-      </c>
-      <c r="B30" t="s">
-        <v>568</v>
-      </c>
-      <c r="C30">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>558</v>
-      </c>
-      <c r="E30">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31">
-        <v>5700</v>
-      </c>
-      <c r="B31" t="s">
-        <v>567</v>
-      </c>
-      <c r="C31">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>606</v>
-      </c>
-      <c r="E31">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32">
-        <v>6000</v>
-      </c>
-      <c r="B32" t="s">
-        <v>567</v>
-      </c>
-      <c r="C32">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <v>6500</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <v>6600</v>
-      </c>
-      <c r="B34" t="s">
-        <v>550</v>
-      </c>
-      <c r="C34">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35">
-        <v>6900</v>
-      </c>
-      <c r="B35" t="s">
-        <v>567</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>7000</v>
-      </c>
-      <c r="B36" t="s">
-        <v>568</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>558</v>
-      </c>
-      <c r="E36">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37">
-        <v>7300</v>
-      </c>
-      <c r="B37" t="s">
-        <v>567</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>606</v>
-      </c>
-      <c r="E37">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <v>7400</v>
-      </c>
-      <c r="B38" t="s">
-        <v>567</v>
-      </c>
-      <c r="C38">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>606</v>
-      </c>
-      <c r="E38">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39">
-        <v>7500</v>
-      </c>
-      <c r="B39" t="s">
-        <v>596</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>610</v>
-      </c>
-      <c r="E39">
-        <v>80</v>
-      </c>
-      <c r="F39" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40">
-        <v>7600</v>
-      </c>
-      <c r="B40" t="s">
-        <v>568</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>558</v>
-      </c>
-      <c r="E40">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>8800</v>
-      </c>
-      <c r="B41" t="s">
-        <v>597</v>
-      </c>
-      <c r="C41">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>607</v>
-      </c>
-      <c r="F41" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42">
-        <v>11600</v>
-      </c>
-      <c r="B42" t="s">
-        <v>598</v>
-      </c>
-      <c r="C42">
-        <v>5</v>
-      </c>
-      <c r="D42" t="s">
-        <v>611</v>
-      </c>
-      <c r="E42">
-        <v>140</v>
-      </c>
-      <c r="F42" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>11700</v>
-      </c>
-      <c r="B43" t="s">
-        <v>561</v>
-      </c>
-      <c r="C43">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>608</v>
-      </c>
-      <c r="E43">
-        <v>200</v>
-      </c>
-      <c r="F43" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>14600</v>
-      </c>
-      <c r="B44" t="s">
-        <v>568</v>
-      </c>
-      <c r="C44">
-        <v>8</v>
-      </c>
-      <c r="D44" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45">
-        <v>14900</v>
-      </c>
-      <c r="B45" t="s">
-        <v>567</v>
-      </c>
-      <c r="C45">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
-        <v>606</v>
-      </c>
-      <c r="E45">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46">
-        <v>15600</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47">
-        <v>15800</v>
-      </c>
-      <c r="B47" t="s">
-        <v>568</v>
-      </c>
-      <c r="C47">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <v>17800</v>
-      </c>
-      <c r="B48" t="s">
-        <v>643</v>
-      </c>
-      <c r="C48" t="s">
-        <v>576</v>
-      </c>
-      <c r="D48" t="s">
-        <v>583</v>
-      </c>
-      <c r="E48">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A49">
-        <v>20000</v>
-      </c>
-      <c r="B49" t="s">
-        <v>601</v>
-      </c>
-      <c r="C49" t="s">
-        <v>576</v>
-      </c>
-      <c r="D49" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A50">
-        <v>28300</v>
-      </c>
-      <c r="B50" t="s">
-        <v>567</v>
-      </c>
-      <c r="C50">
-        <v>6</v>
-      </c>
-      <c r="D50" t="s">
-        <v>606</v>
-      </c>
-      <c r="E50">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <v>30700</v>
-      </c>
-      <c r="B51" t="s">
-        <v>602</v>
-      </c>
-      <c r="C51" t="s">
-        <v>576</v>
-      </c>
-      <c r="D51" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52">
-        <v>30900</v>
-      </c>
-      <c r="B52" t="s">
-        <v>643</v>
-      </c>
-      <c r="C52" t="s">
-        <v>575</v>
-      </c>
-      <c r="D52" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53">
-        <v>31100</v>
-      </c>
-      <c r="B53" t="s">
-        <v>644</v>
-      </c>
-      <c r="C53" t="s">
-        <v>576</v>
-      </c>
-      <c r="D53" t="s">
-        <v>583</v>
-      </c>
-      <c r="E53">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54">
-        <v>31300</v>
-      </c>
-      <c r="B54" t="s">
-        <v>604</v>
-      </c>
-      <c r="D54" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A55">
-        <v>31400</v>
-      </c>
-      <c r="B55" t="s">
-        <v>604</v>
-      </c>
-      <c r="D55" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A56">
-        <v>32200</v>
-      </c>
-      <c r="B56" t="s">
-        <v>603</v>
-      </c>
-      <c r="C56" t="s">
-        <v>575</v>
-      </c>
-      <c r="D56" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A57">
-        <v>32300</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>629</v>
-      </c>
-      <c r="B58" t="s">
-        <v>643</v>
-      </c>
-      <c r="C58" t="s">
-        <v>576</v>
-      </c>
-      <c r="D58" t="s">
-        <v>583</v>
-      </c>
-      <c r="E58">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>628</v>
-      </c>
-      <c r="B59" t="s">
-        <v>549</v>
-      </c>
-      <c r="C59">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>557</v>
-      </c>
-      <c r="E59">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>559</v>
-      </c>
-      <c r="D60" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>559</v>
-      </c>
-      <c r="D61" t="s">
-        <v>592</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
-      <sortCondition ref="A1:A61"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
-    <sortCondition ref="A3:A60"/>
-  </sortState>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE17749-1BD2-42DC-A92D-74E793F7820B}">
   <dimension ref="A1:R156"/>
   <sheetViews>
@@ -7387,7 +6441,7 @@
         <v>483</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>483</v>
@@ -7677,7 +6731,7 @@
         <v>484</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I13" s="29" t="s">
         <v>493</v>
@@ -8303,10 +7357,10 @@
         <v>492</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I35" s="29" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>620</v>
@@ -8451,10 +7505,10 @@
         <v>495</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I40" s="28" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J40" s="20" t="s">
         <v>428</v>
@@ -8480,10 +7534,10 @@
         <v>495</v>
       </c>
       <c r="H41" s="20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J41" s="20" t="s">
         <v>428</v>
@@ -8512,7 +7566,7 @@
         <v>495</v>
       </c>
       <c r="H42" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I42" s="29" t="s">
         <v>483</v>
@@ -8663,10 +7717,10 @@
         <v>503</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J47" s="20" t="s">
         <v>621</v>
@@ -8698,10 +7752,10 @@
         <v>503</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I48" s="29" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J48" s="20" t="s">
         <v>616</v>
@@ -9507,7 +8561,7 @@
         <v>428</v>
       </c>
       <c r="H76" s="20" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I76" s="28" t="s">
         <v>493</v>
@@ -9539,7 +8593,7 @@
         <v>428</v>
       </c>
       <c r="H77" s="20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I77" s="28" t="s">
         <v>502</v>
@@ -9571,7 +8625,7 @@
         <v>428</v>
       </c>
       <c r="H78" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I78" s="29" t="s">
         <v>491</v>
@@ -9603,7 +8657,7 @@
         <v>428</v>
       </c>
       <c r="H79" s="20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="I79" s="28" t="s">
         <v>492</v>
@@ -9638,7 +8692,7 @@
         <v>428</v>
       </c>
       <c r="J80" s="34" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="K80" s="28" t="s">
         <v>497</v>
@@ -10372,7 +9426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -10804,7 +9858,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D29" s="42" t="s">
         <v>613</v>
@@ -10812,10 +9866,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>797</v>
+      </c>
+      <c r="D30" s="42" t="s">
         <v>798</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>799</v>
       </c>
     </row>
   </sheetData>
@@ -10833,13 +9887,975 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
+  <dimension ref="A1:F61"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="21.53125" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="27.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>605</v>
+      </c>
+      <c r="D4" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>220</v>
+      </c>
+      <c r="B5" t="s">
+        <v>539</v>
+      </c>
+      <c r="D5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>605</v>
+      </c>
+      <c r="D6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>400</v>
+      </c>
+      <c r="B7" t="s">
+        <v>627</v>
+      </c>
+      <c r="D7" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>500</v>
+      </c>
+      <c r="B8" t="s">
+        <v>563</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>600</v>
+      </c>
+      <c r="B9" t="s">
+        <v>563</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>556</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>700</v>
+      </c>
+      <c r="B10" t="s">
+        <v>563</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>800</v>
+      </c>
+      <c r="B11" t="s">
+        <v>549</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>557</v>
+      </c>
+      <c r="E11">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>1500</v>
+      </c>
+      <c r="B12" t="s">
+        <v>566</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>612</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>1600</v>
+      </c>
+      <c r="B13" t="s">
+        <v>561</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>608</v>
+      </c>
+      <c r="E13">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>1700</v>
+      </c>
+      <c r="B14" t="s">
+        <v>561</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>608</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>1800</v>
+      </c>
+      <c r="B15" t="s">
+        <v>563</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>2000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>563</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>556</v>
+      </c>
+      <c r="E16">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>2400</v>
+      </c>
+      <c r="B17" t="s">
+        <v>549</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>557</v>
+      </c>
+      <c r="E17">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>2600</v>
+      </c>
+      <c r="B18" t="s">
+        <v>566</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>612</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
+      <c r="F18" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2800</v>
+      </c>
+      <c r="B19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>556</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2900</v>
+      </c>
+      <c r="B20" t="s">
+        <v>549</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>557</v>
+      </c>
+      <c r="E20">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>3000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>549</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>3100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>549</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>557</v>
+      </c>
+      <c r="E22">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>3500</v>
+      </c>
+      <c r="B23" t="s">
+        <v>549</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>557</v>
+      </c>
+      <c r="E23">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>3600</v>
+      </c>
+      <c r="B24" t="s">
+        <v>549</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>557</v>
+      </c>
+      <c r="E24">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>3900</v>
+      </c>
+      <c r="B25" t="s">
+        <v>549</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>557</v>
+      </c>
+      <c r="E25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>4000</v>
+      </c>
+      <c r="B26" t="s">
+        <v>567</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>4300</v>
+      </c>
+      <c r="B27" t="s">
+        <v>567</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>606</v>
+      </c>
+      <c r="E27">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>4900</v>
+      </c>
+      <c r="B28" t="s">
+        <v>567</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>606</v>
+      </c>
+      <c r="E28">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>5500</v>
+      </c>
+      <c r="B29" t="s">
+        <v>570</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>580</v>
+      </c>
+      <c r="E29">
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>5600</v>
+      </c>
+      <c r="B30" t="s">
+        <v>568</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>558</v>
+      </c>
+      <c r="E30">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>5700</v>
+      </c>
+      <c r="B31" t="s">
+        <v>567</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>606</v>
+      </c>
+      <c r="E31">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>6000</v>
+      </c>
+      <c r="B32" t="s">
+        <v>567</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>6500</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>6600</v>
+      </c>
+      <c r="B34" t="s">
+        <v>550</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>6900</v>
+      </c>
+      <c r="B35" t="s">
+        <v>567</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>7000</v>
+      </c>
+      <c r="B36" t="s">
+        <v>568</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>558</v>
+      </c>
+      <c r="E36">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>7300</v>
+      </c>
+      <c r="B37" t="s">
+        <v>567</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>606</v>
+      </c>
+      <c r="E37">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>7400</v>
+      </c>
+      <c r="B38" t="s">
+        <v>567</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>606</v>
+      </c>
+      <c r="E38">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>7500</v>
+      </c>
+      <c r="B39" t="s">
+        <v>596</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>610</v>
+      </c>
+      <c r="E39">
+        <v>80</v>
+      </c>
+      <c r="F39" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>7600</v>
+      </c>
+      <c r="B40" t="s">
+        <v>568</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>558</v>
+      </c>
+      <c r="E40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>8800</v>
+      </c>
+      <c r="B41" t="s">
+        <v>597</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>607</v>
+      </c>
+      <c r="F41" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>11600</v>
+      </c>
+      <c r="B42" t="s">
+        <v>598</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>611</v>
+      </c>
+      <c r="E42">
+        <v>140</v>
+      </c>
+      <c r="F42" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>11700</v>
+      </c>
+      <c r="B43" t="s">
+        <v>561</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>608</v>
+      </c>
+      <c r="E43">
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>14600</v>
+      </c>
+      <c r="B44" t="s">
+        <v>568</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>14900</v>
+      </c>
+      <c r="B45" t="s">
+        <v>567</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>606</v>
+      </c>
+      <c r="E45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>15600</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>15800</v>
+      </c>
+      <c r="B47" t="s">
+        <v>568</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>17800</v>
+      </c>
+      <c r="B48" t="s">
+        <v>643</v>
+      </c>
+      <c r="C48" t="s">
+        <v>576</v>
+      </c>
+      <c r="D48" t="s">
+        <v>583</v>
+      </c>
+      <c r="E48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>20000</v>
+      </c>
+      <c r="B49" t="s">
+        <v>601</v>
+      </c>
+      <c r="C49" t="s">
+        <v>576</v>
+      </c>
+      <c r="D49" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>28300</v>
+      </c>
+      <c r="B50" t="s">
+        <v>567</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>606</v>
+      </c>
+      <c r="E50">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>30700</v>
+      </c>
+      <c r="B51" t="s">
+        <v>602</v>
+      </c>
+      <c r="C51" t="s">
+        <v>576</v>
+      </c>
+      <c r="D51" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>30900</v>
+      </c>
+      <c r="B52" t="s">
+        <v>643</v>
+      </c>
+      <c r="C52" t="s">
+        <v>575</v>
+      </c>
+      <c r="D52" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>31100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>644</v>
+      </c>
+      <c r="C53" t="s">
+        <v>576</v>
+      </c>
+      <c r="D53" t="s">
+        <v>583</v>
+      </c>
+      <c r="E53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>31300</v>
+      </c>
+      <c r="B54" t="s">
+        <v>604</v>
+      </c>
+      <c r="D54" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>31400</v>
+      </c>
+      <c r="B55" t="s">
+        <v>604</v>
+      </c>
+      <c r="D55" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>32200</v>
+      </c>
+      <c r="B56" t="s">
+        <v>603</v>
+      </c>
+      <c r="C56" t="s">
+        <v>575</v>
+      </c>
+      <c r="D56" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>32300</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>629</v>
+      </c>
+      <c r="B58" t="s">
+        <v>643</v>
+      </c>
+      <c r="C58" t="s">
+        <v>576</v>
+      </c>
+      <c r="D58" t="s">
+        <v>583</v>
+      </c>
+      <c r="E58">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>628</v>
+      </c>
+      <c r="B59" t="s">
+        <v>549</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>557</v>
+      </c>
+      <c r="E59">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>559</v>
+      </c>
+      <c r="D60" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>559</v>
+      </c>
+      <c r="D61" t="s">
+        <v>592</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
+      <sortCondition ref="A1:A61"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
+    <sortCondition ref="A3:A60"/>
+  </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10872,7 +10888,7 @@
         <v>642</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>637</v>
@@ -10881,7 +10897,7 @@
         <v>638</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I1" s="31" t="s">
         <v>639</v>
@@ -10943,10 +10959,10 @@
         <v>717</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="I3" s="39" t="s">
         <v>713</v>
@@ -10988,23 +11004,40 @@
         <v>723</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="384.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:11" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="33" t="s">
         <v>636</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="33" t="s">
         <v>725</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="52" t="s">
         <v>726</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="D5" s="33" t="s">
+        <v>710</v>
+      </c>
+      <c r="E5" s="33">
+        <v>3021</v>
+      </c>
+      <c r="F5" s="40" t="s">
         <v>728</v>
       </c>
-      <c r="G5" s="47" t="s">
-        <v>729</v>
-      </c>
-      <c r="H5" s="44"/>
+      <c r="G5" s="38" t="s">
+        <v>802</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>713</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>714</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="32" t="s">
@@ -11030,13 +11063,13 @@
     </row>
     <row r="8" spans="1:11" ht="384.75" x14ac:dyDescent="0.45">
       <c r="A8" s="33" t="s">
+        <v>748</v>
+      </c>
+      <c r="B8" s="33" t="s">
         <v>749</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="C8" s="33" t="s">
         <v>750</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>751</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>710</v>
@@ -11045,17 +11078,17 @@
         <v>3021</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="40" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="K8" s="48" t="s">
         <v>714</v>
@@ -11063,13 +11096,13 @@
     </row>
     <row r="9" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A9" s="32" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>754</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>755</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>756</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>710</v>
@@ -11078,14 +11111,14 @@
         <v>3021</v>
       </c>
       <c r="F9" s="33" t="s">
+        <v>756</v>
+      </c>
+      <c r="G9" s="47" t="s">
         <v>757</v>
-      </c>
-      <c r="G9" s="47" t="s">
-        <v>758</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="40" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
@@ -11093,10 +11126,10 @@
         <v>636</v>
       </c>
       <c r="B10" s="32" t="s">
+        <v>761</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>762</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>763</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>710</v>
@@ -11105,30 +11138,30 @@
         <v>3021</v>
       </c>
       <c r="F10" s="40" t="s">
+        <v>763</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>765</v>
+      </c>
+      <c r="H10" s="39" t="s">
         <v>764</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="I10" s="39" t="s">
         <v>766</v>
       </c>
-      <c r="H10" s="39" t="s">
-        <v>765</v>
-      </c>
-      <c r="I10" s="39" t="s">
+      <c r="J10" s="40" t="s">
         <v>767</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A11" s="32" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>710</v>
@@ -11137,24 +11170,24 @@
         <v>3021</v>
       </c>
       <c r="F11" s="40" t="s">
+        <v>771</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>788</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>771</v>
+      </c>
+      <c r="J11" s="41" t="s">
         <v>772</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>789</v>
-      </c>
-      <c r="I11" s="40" t="s">
-        <v>772</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A12" s="33" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="33" t="s">
@@ -11164,45 +11197,48 @@
         <v>3021</v>
       </c>
       <c r="F12" s="40" t="s">
+        <v>790</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>793</v>
+      </c>
+      <c r="H12" s="39" t="s">
         <v>791</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="I12" s="40" t="s">
+        <v>792</v>
+      </c>
+      <c r="J12" s="39" t="s">
         <v>794</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>792</v>
-      </c>
-      <c r="I12" s="40" t="s">
-        <v>793</v>
-      </c>
-      <c r="J12" s="39" t="s">
+      <c r="K12" s="33" t="s">
         <v>795</v>
-      </c>
-      <c r="K12" s="33" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A13" s="32" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G13" s="49"/>
       <c r="H13" s="51"/>
       <c r="I13" s="50"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{943F34A2-1BA5-4D1C-81A8-62EE384FF261}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -11710,7 +11746,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -11718,50 +11754,50 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B3" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B6" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -11769,65 +11805,65 @@
         <v>16500</v>
       </c>
       <c r="B9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B10" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C10" t="s">
+        <v>736</v>
+      </c>
+      <c r="D10" t="s">
         <v>737</v>
       </c>
-      <c r="D10" t="s">
-        <v>738</v>
-      </c>
       <c r="E10" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F10" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G10" t="s">
+        <v>736</v>
+      </c>
+      <c r="H10" t="s">
         <v>737</v>
       </c>
-      <c r="H10" t="s">
-        <v>738</v>
-      </c>
       <c r="I10" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>731</v>
+      </c>
+      <c r="B11" t="s">
+        <v>734</v>
+      </c>
+      <c r="C11" t="s">
+        <v>729</v>
+      </c>
+      <c r="D11" t="s">
+        <v>734</v>
+      </c>
+      <c r="E11" t="s">
         <v>732</v>
       </c>
-      <c r="B11" t="s">
-        <v>735</v>
-      </c>
-      <c r="C11" t="s">
-        <v>730</v>
-      </c>
-      <c r="D11" t="s">
-        <v>735</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>734</v>
+      </c>
+      <c r="G11" t="s">
+        <v>729</v>
+      </c>
+      <c r="H11" t="s">
+        <v>734</v>
+      </c>
+      <c r="I11" t="s">
         <v>733</v>
-      </c>
-      <c r="F11" t="s">
-        <v>735</v>
-      </c>
-      <c r="G11" t="s">
-        <v>730</v>
-      </c>
-      <c r="H11" t="s">
-        <v>735</v>
-      </c>
-      <c r="I11" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -11835,53 +11871,53 @@
         <v>16100</v>
       </c>
       <c r="B13" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B14" t="s">
+        <v>736</v>
+      </c>
+      <c r="C14" t="s">
         <v>737</v>
       </c>
-      <c r="C14" t="s">
-        <v>738</v>
-      </c>
       <c r="D14" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E14" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F14" t="s">
+        <v>736</v>
+      </c>
+      <c r="G14" t="s">
         <v>737</v>
-      </c>
-      <c r="G14" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B15" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F15" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G15" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -11889,56 +11925,56 @@
         <v>16200</v>
       </c>
       <c r="B17" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C17" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B18" t="s">
+        <v>736</v>
+      </c>
+      <c r="C18" t="s">
         <v>737</v>
       </c>
-      <c r="C18" t="s">
-        <v>738</v>
-      </c>
       <c r="D18" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E18" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F18" t="s">
+        <v>736</v>
+      </c>
+      <c r="G18" t="s">
         <v>737</v>
-      </c>
-      <c r="G18" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F19" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G19" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -11946,53 +11982,53 @@
         <v>16400</v>
       </c>
       <c r="B21" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B22" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C22" t="s">
+        <v>736</v>
+      </c>
+      <c r="D22" t="s">
+        <v>739</v>
+      </c>
+      <c r="E22" t="s">
+        <v>736</v>
+      </c>
+      <c r="F22" t="s">
         <v>737</v>
       </c>
-      <c r="D22" t="s">
-        <v>740</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>737</v>
-      </c>
-      <c r="F22" t="s">
-        <v>738</v>
-      </c>
-      <c r="G22" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B23" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D23" t="s">
+        <v>732</v>
+      </c>
+      <c r="E23" t="s">
+        <v>729</v>
+      </c>
+      <c r="F23" t="s">
+        <v>734</v>
+      </c>
+      <c r="G23" t="s">
         <v>733</v>
-      </c>
-      <c r="E23" t="s">
-        <v>730</v>
-      </c>
-      <c r="F23" t="s">
-        <v>735</v>
-      </c>
-      <c r="G23" t="s">
-        <v>734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[2200] restore original scenario, now works again...
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CFF201-C4E1-49D5-A7A6-FE16B36D5A05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883A6F03-0F66-43D7-B3ED-F6564F1897A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6495" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="807">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3071,9 +3071,6 @@
   </si>
   <si>
     <t>FCl*</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=CEayBOxq_Zo, https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s</t>
   </si>
   <si>
     <t>- cUtoUt15 Dld-Ut</t>
@@ -3200,6 +3197,34 @@
 Misc:
 - Blauwkapel: voor speler ivm 1701</t>
     </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s, https://www.youtube.com/watch?v=CEayBOxq_Zo</t>
+  </si>
+  <si>
+    <t>Rsd:
+- cRsdgRsd02/cRsdUitEsn07
+- 450/451 Rsdg-Rsd1a
+- 3600/3601 Rsd3a
+- 5900/5901 Rsd3b
+- 2201 Rsd4b
+Rsd-Gs:
+- 2201 Bgn
+- cGsBzl25 Rb-Bgn
+- 2201 Kbd
+- cGsBzl25 Krg
+- 2201 Gs</t>
+  </si>
+  <si>
+    <t>- Ddr
+- Rsd
+- Gs</t>
+  </si>
+  <si>
+    <t>- cRbSloe25 Rsd-Bgn</t>
+  </si>
+  <si>
+    <t>- Rsd</t>
   </si>
 </sst>
 </file>
@@ -3351,7 +3376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3451,12 +3476,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
@@ -10877,8 +10896,8 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10982,10 +11001,10 @@
         <v>717</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I3" s="39" t="s">
         <v>713</v>
@@ -11034,7 +11053,7 @@
       <c r="B5" s="33" t="s">
         <v>725</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="50" t="s">
         <v>726</v>
       </c>
       <c r="D5" s="33" t="s">
@@ -11047,7 +11066,7 @@
         <v>728</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H5" s="38" t="s">
         <v>42</v>
@@ -11238,22 +11257,34 @@
         <v>795</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="171" x14ac:dyDescent="0.45">
       <c r="A13" s="32" t="s">
         <v>748</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>796</v>
       </c>
-      <c r="C13" s="49" t="s">
-        <v>799</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>753</v>
-      </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="50"/>
+      <c r="C13" s="33" t="s">
+        <v>802</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>710</v>
+      </c>
+      <c r="E13" s="33">
+        <v>3021</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>804</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>803</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>805</v>
+      </c>
+      <c r="I13" s="49" t="s">
+        <v>806</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
[2200] Rtd player spawn
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883A6F03-0F66-43D7-B3ED-F6564F1897A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1DCF7C-8247-4B26-80CE-F4E116874809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="338" yWindow="6832" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -3199,9 +3199,6 @@
     </r>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s, https://www.youtube.com/watch?v=CEayBOxq_Zo</t>
-  </si>
-  <si>
     <t>Rsd:
 - cRsdgRsd02/cRsdUitEsn07
 - 450/451 Rsdg-Rsd1a
@@ -3216,15 +3213,19 @@
 - 2201 Gs</t>
   </si>
   <si>
-    <t>- Ddr
+    <t>- cRbSloe25 Rsd-Bgn</t>
+  </si>
+  <si>
+    <t>- Rsd</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CEayBOxq_Zo, https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s</t>
+  </si>
+  <si>
+    <t>- Rtd
+- Ddr
 - Rsd
 - Gs</t>
-  </si>
-  <si>
-    <t>- cRbSloe25 Rsd-Bgn</t>
-  </si>
-  <si>
-    <t>- Rsd</t>
   </si>
 </sst>
 </file>
@@ -10897,7 +10898,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11265,7 +11266,7 @@
         <v>796</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>710</v>
@@ -11273,17 +11274,17 @@
       <c r="E13" s="33">
         <v>3021</v>
       </c>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="40" t="s">
+        <v>806</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>802</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>803</v>
+      </c>
+      <c r="I13" s="49" t="s">
         <v>804</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>803</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>805</v>
-      </c>
-      <c r="I13" s="49" t="s">
-        <v>806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[2200] AI traffic Rtd-Ddr incl
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4C1573-4CA1-44DC-B1F0-53DBB7B7666E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217591D0-B593-42DD-A8F2-4A56D4C8C605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="338" yWindow="6832" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="808">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3199,29 +3199,7 @@
     </r>
   </si>
   <si>
-    <t>- cRbSloe25 Rsd-Bgn</t>
-  </si>
-  <si>
-    <t>- Rsd</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=CEayBOxq_Zo, https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s</t>
-  </si>
-  <si>
-    <t>- Rtd
-- Ddr
-- Rsd
-- Gs</t>
-  </si>
-  <si>
-    <t>Rtd:
-- 900 Rtd3 -&gt; hsl
-- 1000/1001 Rtd11
-- 2800/2801 Rtd13
-- 4000/4001 Rtd16
-- 5000 Rtd8
-- 9201/9601 Rtd12
-Rsd:
+    <t>Rsd:
 - cRsdgRsd02/cRsdUitEsn07
 - 450/451 Rsdg-Rsd1a
 - 3600/3601 Rsd3a
@@ -3233,6 +3211,44 @@
 - 2201 Kbd
 - cGsBzl25 Krg
 - 2201 Gs</t>
+  </si>
+  <si>
+    <t>- Rsd</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CEayBOxq_Zo, https://www.youtube.com/watch?v=9RR7UUSssjQ&amp;t=2555s</t>
+  </si>
+  <si>
+    <t>- cDdrDdzd06 Zwd-Ddr
+- cRbSloe25 Rsd-Bgn</t>
+  </si>
+  <si>
+    <t>- Rtd (Zwd niet geheel vastgelegd)
+- Ddr
+- Rsd
+- Gs</t>
+  </si>
+  <si>
+    <t>Rtd:
+- 900 Rtd3 -&gt; hsl
+- 1000/1001 Rtd11
+- 2800/2801 Rtd13
+- 4000/4001 Rtd16
+- 5000 Rtd8
+- 9201/9601 Rtd12
+Rtd-Ddr:
+- 2400 Rtb-Rtd9
+- cRtdSdm28-29 ea Rtz
+- 5100 Rtst
+- 9100/9301 Rlb
+- 2201 Kfh
+- 5000 Zwd
+Ddr:
+- 2400/2401 Ddr2
+- 5001/5100 Ddr3a
+- 5900 Ddr3b
+- 6600/6601 Ddr4b
+- 7200/7201 Ddr15</t>
   </si>
 </sst>
 </file>
@@ -10443,7 +10459,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10901,11 +10917,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11265,7 +11281,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="285" x14ac:dyDescent="0.45">
       <c r="A13" s="32" t="s">
         <v>748</v>
       </c>
@@ -11282,16 +11298,25 @@
         <v>3021</v>
       </c>
       <c r="F13" s="40" t="s">
+        <v>806</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>807</v>
+      </c>
+      <c r="H13" s="41" t="s">
         <v>805</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>806</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>802</v>
       </c>
       <c r="I13" s="49" t="s">
         <v>803</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="171" x14ac:dyDescent="0.45">
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="41" t="s">
+        <v>802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[4900] scenario updates (cargo)
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217591D0-B593-42DD-A8F2-4A56D4C8C605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44832D8-2AB2-46FA-B67C-00E8C09B53BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="338" yWindow="6832" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="808">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -2651,22 +2651,6 @@
   </si>
   <si>
     <t>- Hvs</t>
-  </si>
-  <si>
-    <t>Hvs - Ut:
-- 5700 Hor-Hvs
-- FO/FL/C8 Amf-Uto-Ut9-Ht
-- 4900 Uto
-- 28301 Ut-Uto
-Ut:
-- 101/121/221 Ut18
-- 1701/11701 Ut11
-- 3101 Ut19
-- 3500 Ht-Ut7
-- 5500/5501 Ut3
-- 7400 Ut14
-- 8800/8801 Wd-Ut12
-- 2800/2801 Ut20-Wd</t>
   </si>
   <si>
     <t>- Ut</t>
@@ -3249,6 +3233,24 @@
 - 5900 Ddr3b
 - 6600/6601 Ddr4b
 - 7200/7201 Ddr15</t>
+  </si>
+  <si>
+    <t>Hvs - Ut:
+- 5700 Hor-Hvs
+- cUtoUt01, Blw
+- cUtUto25, Uto
+- 4900 Uto
+- cUtUto00
+- 28301 Ut-Uto
+Ut:
+- 101/121/221 Ut18
+- 1701/11701 Ut11
+- 3101 Ut19
+- 3500 Ht-Ut7
+- 5500/5501 Ut3
+- 7400 Ut14
+- 8800/8801 Wd-Ut12
+- 2800/2801 Ut20-Wd</t>
   </si>
 </sst>
 </file>
@@ -6507,7 +6509,7 @@
         <v>483</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>483</v>
@@ -6797,7 +6799,7 @@
         <v>484</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I13" s="29" t="s">
         <v>493</v>
@@ -7423,10 +7425,10 @@
         <v>492</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I35" s="29" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>620</v>
@@ -7571,10 +7573,10 @@
         <v>495</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="I40" s="28" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="J40" s="20" t="s">
         <v>428</v>
@@ -7600,10 +7602,10 @@
         <v>495</v>
       </c>
       <c r="H41" s="20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="J41" s="20" t="s">
         <v>428</v>
@@ -7632,7 +7634,7 @@
         <v>495</v>
       </c>
       <c r="H42" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I42" s="29" t="s">
         <v>483</v>
@@ -7783,10 +7785,10 @@
         <v>503</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="J47" s="20" t="s">
         <v>621</v>
@@ -7818,10 +7820,10 @@
         <v>503</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I48" s="29" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J48" s="20" t="s">
         <v>616</v>
@@ -8627,7 +8629,7 @@
         <v>428</v>
       </c>
       <c r="H76" s="20" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I76" s="28" t="s">
         <v>493</v>
@@ -8659,7 +8661,7 @@
         <v>428</v>
       </c>
       <c r="H77" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I77" s="28" t="s">
         <v>502</v>
@@ -8691,7 +8693,7 @@
         <v>428</v>
       </c>
       <c r="H78" s="20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I78" s="29" t="s">
         <v>491</v>
@@ -8723,7 +8725,7 @@
         <v>428</v>
       </c>
       <c r="H79" s="20" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I79" s="28" t="s">
         <v>492</v>
@@ -8758,7 +8760,7 @@
         <v>428</v>
       </c>
       <c r="J80" s="34" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="K80" s="28" t="s">
         <v>497</v>
@@ -10886,7 +10888,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D29" s="42" t="s">
         <v>613</v>
@@ -10894,10 +10896,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>796</v>
+      </c>
+      <c r="D30" s="42" t="s">
         <v>797</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>798</v>
       </c>
     </row>
   </sheetData>
@@ -10919,9 +10921,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10954,7 +10956,7 @@
         <v>642</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>637</v>
@@ -10963,7 +10965,7 @@
         <v>638</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="I1" s="31" t="s">
         <v>639</v>
@@ -10975,7 +10977,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="228" x14ac:dyDescent="0.45">
       <c r="A2" s="33" t="s">
         <v>636</v>
       </c>
@@ -10988,21 +10990,26 @@
       <c r="D2" s="33" t="s">
         <v>710</v>
       </c>
+      <c r="E2" s="33">
+        <v>3021</v>
+      </c>
       <c r="F2" s="39" t="s">
         <v>711</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="38" t="s">
+        <v>807</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="39" t="s">
         <v>712</v>
-      </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="39" t="s">
-        <v>713</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>711</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="327.75" x14ac:dyDescent="0.45">
@@ -11010,10 +11017,10 @@
         <v>636</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D3" s="33" t="s">
         <v>710</v>
@@ -11022,22 +11029,22 @@
         <v>3021</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="I3" s="39" t="s">
+        <v>712</v>
+      </c>
+      <c r="J3" s="33" t="s">
         <v>713</v>
       </c>
-      <c r="J3" s="33" t="s">
-        <v>714</v>
-      </c>
       <c r="K3" s="33" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="228" x14ac:dyDescent="0.45">
@@ -11048,26 +11055,26 @@
         <v>140</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>710</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="H4" s="44"/>
       <c r="I4" s="40" t="s">
+        <v>721</v>
+      </c>
+      <c r="J4" s="40" t="s">
+        <v>718</v>
+      </c>
+      <c r="K4" s="40" t="s">
         <v>722</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>719</v>
-      </c>
-      <c r="K4" s="40" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="409.5" x14ac:dyDescent="0.45">
@@ -11075,10 +11082,10 @@
         <v>636</v>
       </c>
       <c r="B5" s="33" t="s">
+        <v>724</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>725</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>726</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>710</v>
@@ -11087,22 +11094,22 @@
         <v>3021</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="H5" s="38" t="s">
         <v>42</v>
       </c>
       <c r="I5" s="39" t="s">
+        <v>712</v>
+      </c>
+      <c r="J5" s="33" t="s">
         <v>713</v>
       </c>
-      <c r="J5" s="33" t="s">
-        <v>714</v>
-      </c>
       <c r="K5" s="33" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -11110,10 +11117,10 @@
         <v>636</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -11124,18 +11131,18 @@
         <v>5600</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="384.75" x14ac:dyDescent="0.45">
       <c r="A8" s="33" t="s">
+        <v>747</v>
+      </c>
+      <c r="B8" s="33" t="s">
         <v>748</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="C8" s="33" t="s">
         <v>749</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>750</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>710</v>
@@ -11144,31 +11151,31 @@
         <v>3021</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="40" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K8" s="48" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A9" s="32" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>753</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>754</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>755</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>710</v>
@@ -11177,14 +11184,14 @@
         <v>3021</v>
       </c>
       <c r="F9" s="33" t="s">
+        <v>755</v>
+      </c>
+      <c r="G9" s="47" t="s">
         <v>756</v>
-      </c>
-      <c r="G9" s="47" t="s">
-        <v>757</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="40" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
@@ -11192,10 +11199,10 @@
         <v>636</v>
       </c>
       <c r="B10" s="32" t="s">
+        <v>760</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>761</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>762</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>710</v>
@@ -11204,30 +11211,30 @@
         <v>3021</v>
       </c>
       <c r="F10" s="40" t="s">
+        <v>762</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>764</v>
+      </c>
+      <c r="H10" s="39" t="s">
         <v>763</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="I10" s="39" t="s">
         <v>765</v>
       </c>
-      <c r="H10" s="39" t="s">
-        <v>764</v>
-      </c>
-      <c r="I10" s="39" t="s">
+      <c r="J10" s="40" t="s">
         <v>766</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A11" s="32" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>710</v>
@@ -11236,24 +11243,24 @@
         <v>3021</v>
       </c>
       <c r="F11" s="40" t="s">
+        <v>770</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>787</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>770</v>
+      </c>
+      <c r="J11" s="41" t="s">
         <v>771</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>788</v>
-      </c>
-      <c r="I11" s="40" t="s">
-        <v>771</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="270.75" x14ac:dyDescent="0.45">
       <c r="A12" s="33" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="33" t="s">
@@ -11263,33 +11270,33 @@
         <v>3021</v>
       </c>
       <c r="F12" s="40" t="s">
+        <v>789</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>792</v>
+      </c>
+      <c r="H12" s="39" t="s">
         <v>790</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="I12" s="40" t="s">
+        <v>791</v>
+      </c>
+      <c r="J12" s="39" t="s">
         <v>793</v>
       </c>
-      <c r="H12" s="39" t="s">
-        <v>791</v>
-      </c>
-      <c r="I12" s="40" t="s">
-        <v>792</v>
-      </c>
-      <c r="J12" s="39" t="s">
+      <c r="K12" s="33" t="s">
         <v>794</v>
-      </c>
-      <c r="K12" s="33" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="285" x14ac:dyDescent="0.45">
       <c r="A13" s="32" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>710</v>
@@ -11298,16 +11305,16 @@
         <v>3021</v>
       </c>
       <c r="F13" s="40" t="s">
+        <v>805</v>
+      </c>
+      <c r="G13" s="41" t="s">
         <v>806</v>
       </c>
-      <c r="G13" s="41" t="s">
-        <v>807</v>
-      </c>
       <c r="H13" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I13" s="49" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="171" x14ac:dyDescent="0.45">
@@ -11316,7 +11323,7 @@
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
       <c r="G14" s="41" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
   </sheetData>
@@ -11833,7 +11840,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -11841,50 +11848,50 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B6" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B7" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -11892,65 +11899,65 @@
         <v>16500</v>
       </c>
       <c r="B9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B10" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C10" t="s">
+        <v>735</v>
+      </c>
+      <c r="D10" t="s">
         <v>736</v>
       </c>
-      <c r="D10" t="s">
-        <v>737</v>
-      </c>
       <c r="E10" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F10" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G10" t="s">
+        <v>735</v>
+      </c>
+      <c r="H10" t="s">
         <v>736</v>
       </c>
-      <c r="H10" t="s">
-        <v>737</v>
-      </c>
       <c r="I10" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>730</v>
+      </c>
+      <c r="B11" t="s">
+        <v>733</v>
+      </c>
+      <c r="C11" t="s">
+        <v>728</v>
+      </c>
+      <c r="D11" t="s">
+        <v>733</v>
+      </c>
+      <c r="E11" t="s">
         <v>731</v>
       </c>
-      <c r="B11" t="s">
-        <v>734</v>
-      </c>
-      <c r="C11" t="s">
-        <v>729</v>
-      </c>
-      <c r="D11" t="s">
-        <v>734</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>733</v>
+      </c>
+      <c r="G11" t="s">
+        <v>728</v>
+      </c>
+      <c r="H11" t="s">
+        <v>733</v>
+      </c>
+      <c r="I11" t="s">
         <v>732</v>
-      </c>
-      <c r="F11" t="s">
-        <v>734</v>
-      </c>
-      <c r="G11" t="s">
-        <v>729</v>
-      </c>
-      <c r="H11" t="s">
-        <v>734</v>
-      </c>
-      <c r="I11" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -11958,53 +11965,53 @@
         <v>16100</v>
       </c>
       <c r="B13" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B14" t="s">
+        <v>735</v>
+      </c>
+      <c r="C14" t="s">
         <v>736</v>
       </c>
-      <c r="C14" t="s">
-        <v>737</v>
-      </c>
       <c r="D14" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E14" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F14" t="s">
+        <v>735</v>
+      </c>
+      <c r="G14" t="s">
         <v>736</v>
-      </c>
-      <c r="G14" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B15" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C15" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D15" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E15" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F15" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G15" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -12012,56 +12019,56 @@
         <v>16200</v>
       </c>
       <c r="B17" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C17" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B18" t="s">
+        <v>735</v>
+      </c>
+      <c r="C18" t="s">
         <v>736</v>
       </c>
-      <c r="C18" t="s">
-        <v>737</v>
-      </c>
       <c r="D18" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E18" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F18" t="s">
+        <v>735</v>
+      </c>
+      <c r="G18" t="s">
         <v>736</v>
-      </c>
-      <c r="G18" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C19" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D19" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E19" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G19" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -12069,53 +12076,53 @@
         <v>16400</v>
       </c>
       <c r="B21" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B22" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C22" t="s">
+        <v>735</v>
+      </c>
+      <c r="D22" t="s">
+        <v>738</v>
+      </c>
+      <c r="E22" t="s">
+        <v>735</v>
+      </c>
+      <c r="F22" t="s">
         <v>736</v>
       </c>
-      <c r="D22" t="s">
-        <v>739</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>736</v>
-      </c>
-      <c r="F22" t="s">
-        <v>737</v>
-      </c>
-      <c r="G22" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B23" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C23" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D23" t="s">
+        <v>731</v>
+      </c>
+      <c r="E23" t="s">
+        <v>728</v>
+      </c>
+      <c r="F23" t="s">
+        <v>733</v>
+      </c>
+      <c r="G23" t="s">
         <v>732</v>
-      </c>
-      <c r="E23" t="s">
-        <v>729</v>
-      </c>
-      <c r="F23" t="s">
-        <v>734</v>
-      </c>
-      <c r="G23" t="s">
-        <v>733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Research: drgl 2022 voor HvN
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,24 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44832D8-2AB2-46FA-B67C-00E8C09B53BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90700BF-149F-4FD3-9DCD-09E5A64158A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="338" yWindow="6832" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6742" yWindow="5783" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
     <sheet name="Goederentreinen" sheetId="9" r:id="rId2"/>
     <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId3"/>
-    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId4"/>
-    <sheet name="Scenarios" sheetId="14" r:id="rId5"/>
-    <sheet name="Vervoerders" sheetId="7" r:id="rId6"/>
-    <sheet name="ICRm" sheetId="17" r:id="rId7"/>
+    <sheet name="HvN-Treinseries 2022" sheetId="18" r:id="rId4"/>
+    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId5"/>
+    <sheet name="Scenarios" sheetId="14" r:id="rId6"/>
+    <sheet name="Vervoerders" sheetId="7" r:id="rId7"/>
+    <sheet name="ICRm" sheetId="17" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'HvN-Treinseries 2022'!$A$1:$F$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -452,6 +454,113 @@
     <author>Tom</author>
   </authors>
   <commentList>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{428C447F-3560-4B7D-B002-B0A3F8A1BE88}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DDZ alleen 1x6 bakken</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{6BECAE74-5D00-4BB6-B0D6-6D39894B72B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+geen somda drgl?
+Nu uit 3000, 3700</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{77AFD862-B4EA-429F-BB66-A98C2B8B3480}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+weggelaten, alleen zondag</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A50" authorId="0" shapeId="0" xr:uid="{DD718A40-EB37-4C6E-BA23-E511F95E1997}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+zazo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
     <comment ref="C9" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
       <text>
         <r>
@@ -480,7 +589,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tom</author>
@@ -515,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="827">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3251,6 +3360,63 @@
 - 7400 Ut14
 - 8800/8801 Wd-Ut12
 - 2800/2801 Ut20-Wd</t>
+  </si>
+  <si>
+    <t>IC Berlijn</t>
+  </si>
+  <si>
+    <t>Nightjet</t>
+  </si>
+  <si>
+    <t>9, 6</t>
+  </si>
+  <si>
+    <t>0.3, 0.7</t>
+  </si>
+  <si>
+    <t>11, 6</t>
+  </si>
+  <si>
+    <t>0.1, 0.9</t>
+  </si>
+  <si>
+    <t>VIRM, DDZ, ICM</t>
+  </si>
+  <si>
+    <t>0.4, 0.4, 0.2</t>
+  </si>
+  <si>
+    <t>0.9, 0.1</t>
+  </si>
+  <si>
+    <t>8, 4</t>
+  </si>
+  <si>
+    <t>SLT, SNG</t>
+  </si>
+  <si>
+    <t>SNG, FLIRT</t>
+  </si>
+  <si>
+    <t>Valleilijn FLIRT</t>
+  </si>
+  <si>
+    <t>Passenger Scrap, Regional</t>
+  </si>
+  <si>
+    <t>Passenger Commuter, Regional</t>
+  </si>
+  <si>
+    <t>Passenger Regional, Scrap</t>
+  </si>
+  <si>
+    <t>Passenger Fast, Custom 1, Intercity</t>
+  </si>
+  <si>
+    <t>ICM, DDZ*</t>
+  </si>
+  <si>
+    <t>rijdt niet ivm corona?</t>
   </si>
 </sst>
 </file>
@@ -3402,7 +3568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3510,6 +3676,8 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9498,8 +9666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10457,6 +10625,943 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D33F517-9C34-403A-A4F3-107C3F8D830D}">
+  <dimension ref="A1:F57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.53125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.9296875" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" customWidth="1"/>
+    <col min="6" max="6" width="16.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="42">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="42">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="42">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>808</v>
+      </c>
+      <c r="D4" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="42">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="42">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>808</v>
+      </c>
+      <c r="D6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="42">
+        <v>250</v>
+      </c>
+      <c r="B7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="42">
+        <v>400</v>
+      </c>
+      <c r="B8" t="s">
+        <v>809</v>
+      </c>
+      <c r="D8" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="42">
+        <v>420</v>
+      </c>
+      <c r="B9" t="s">
+        <v>809</v>
+      </c>
+      <c r="D9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="42">
+        <v>500</v>
+      </c>
+      <c r="B10" t="s">
+        <v>563</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>556</v>
+      </c>
+      <c r="E10">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="42">
+        <v>600</v>
+      </c>
+      <c r="B11" t="s">
+        <v>563</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>556</v>
+      </c>
+      <c r="E11">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="42">
+        <v>700</v>
+      </c>
+      <c r="B12" t="s">
+        <v>563</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>556</v>
+      </c>
+      <c r="E12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="42">
+        <v>800</v>
+      </c>
+      <c r="B13" t="s">
+        <v>549</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>557</v>
+      </c>
+      <c r="E13">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="42">
+        <v>1500</v>
+      </c>
+      <c r="B14" t="s">
+        <v>563</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>556</v>
+      </c>
+      <c r="E14">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="42">
+        <v>1600</v>
+      </c>
+      <c r="B15" t="s">
+        <v>825</v>
+      </c>
+      <c r="C15" t="s">
+        <v>810</v>
+      </c>
+      <c r="D15" t="s">
+        <v>611</v>
+      </c>
+      <c r="E15">
+        <v>250</v>
+      </c>
+      <c r="F15" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="42">
+        <v>1700</v>
+      </c>
+      <c r="B16" t="s">
+        <v>825</v>
+      </c>
+      <c r="C16" t="s">
+        <v>812</v>
+      </c>
+      <c r="D16" t="s">
+        <v>611</v>
+      </c>
+      <c r="F16" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="42">
+        <v>2000</v>
+      </c>
+      <c r="B17" t="s">
+        <v>563</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="42">
+        <v>2800</v>
+      </c>
+      <c r="B18" t="s">
+        <v>563</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>556</v>
+      </c>
+      <c r="E18">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="42">
+        <v>2900</v>
+      </c>
+      <c r="B19" t="s">
+        <v>549</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>557</v>
+      </c>
+      <c r="E19">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="42">
+        <v>3000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>549</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>557</v>
+      </c>
+      <c r="E20">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="42">
+        <v>3100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>549</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>557</v>
+      </c>
+      <c r="E21">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="51">
+        <v>3200</v>
+      </c>
+      <c r="B22" t="s">
+        <v>549</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="42">
+        <v>3500</v>
+      </c>
+      <c r="B23" t="s">
+        <v>549</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="42">
+        <v>3600</v>
+      </c>
+      <c r="B24" t="s">
+        <v>814</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>824</v>
+      </c>
+      <c r="E24">
+        <v>170</v>
+      </c>
+      <c r="F24" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="52">
+        <v>3700</v>
+      </c>
+      <c r="B25" t="s">
+        <v>549</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>557</v>
+      </c>
+      <c r="E25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="42">
+        <v>3900</v>
+      </c>
+      <c r="B26" t="s">
+        <v>549</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>557</v>
+      </c>
+      <c r="E26">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="42">
+        <v>4000</v>
+      </c>
+      <c r="B27" t="s">
+        <v>567</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="42">
+        <v>4900</v>
+      </c>
+      <c r="B28" t="s">
+        <v>550</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>609</v>
+      </c>
+      <c r="E28">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="42">
+        <v>5500</v>
+      </c>
+      <c r="B29" t="s">
+        <v>567</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>606</v>
+      </c>
+      <c r="E29">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="42">
+        <v>5600</v>
+      </c>
+      <c r="B30" t="s">
+        <v>568</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>558</v>
+      </c>
+      <c r="E30">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="42">
+        <v>5700</v>
+      </c>
+      <c r="B31" t="s">
+        <v>567</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>606</v>
+      </c>
+      <c r="E31">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="42">
+        <v>6000</v>
+      </c>
+      <c r="B32" t="s">
+        <v>567</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>606</v>
+      </c>
+      <c r="E32">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="42">
+        <v>6600</v>
+      </c>
+      <c r="B33" t="s">
+        <v>572</v>
+      </c>
+      <c r="C33" t="s">
+        <v>817</v>
+      </c>
+      <c r="D33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F33" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="42">
+        <v>6900</v>
+      </c>
+      <c r="B34" t="s">
+        <v>567</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="42">
+        <v>7000</v>
+      </c>
+      <c r="B35" t="s">
+        <v>568</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>558</v>
+      </c>
+      <c r="E35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="42">
+        <v>7300</v>
+      </c>
+      <c r="B36" t="s">
+        <v>818</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>822</v>
+      </c>
+      <c r="E36">
+        <v>110</v>
+      </c>
+      <c r="F36" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="42">
+        <v>7400</v>
+      </c>
+      <c r="B37" t="s">
+        <v>818</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>822</v>
+      </c>
+      <c r="F37" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="42">
+        <v>7500</v>
+      </c>
+      <c r="B38" t="s">
+        <v>819</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>823</v>
+      </c>
+      <c r="E38">
+        <v>80</v>
+      </c>
+      <c r="F38" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="42">
+        <v>7600</v>
+      </c>
+      <c r="B39" t="s">
+        <v>550</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>609</v>
+      </c>
+      <c r="E39">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="42">
+        <v>8800</v>
+      </c>
+      <c r="B40" t="s">
+        <v>567</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>606</v>
+      </c>
+      <c r="E40">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="42">
+        <v>8900</v>
+      </c>
+      <c r="B41" t="s">
+        <v>567</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>606</v>
+      </c>
+      <c r="E41">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="42">
+        <v>11600</v>
+      </c>
+      <c r="B42" t="s">
+        <v>825</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>611</v>
+      </c>
+      <c r="E42">
+        <v>170</v>
+      </c>
+      <c r="F42" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="42">
+        <v>11700</v>
+      </c>
+      <c r="B43" t="s">
+        <v>825</v>
+      </c>
+      <c r="C43" t="s">
+        <v>571</v>
+      </c>
+      <c r="D43" t="s">
+        <v>611</v>
+      </c>
+      <c r="E43">
+        <v>290</v>
+      </c>
+      <c r="F43" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="42">
+        <v>14900</v>
+      </c>
+      <c r="B44" t="s">
+        <v>567</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>606</v>
+      </c>
+      <c r="E44">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="42">
+        <v>15600</v>
+      </c>
+      <c r="B45" t="s">
+        <v>567</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>606</v>
+      </c>
+      <c r="E45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="42">
+        <v>15800</v>
+      </c>
+      <c r="B46" t="s">
+        <v>568</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>558</v>
+      </c>
+      <c r="E46">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="42">
+        <v>17800</v>
+      </c>
+      <c r="B47" t="s">
+        <v>643</v>
+      </c>
+      <c r="C47" t="s">
+        <v>575</v>
+      </c>
+      <c r="D47" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="42">
+        <v>20000</v>
+      </c>
+      <c r="B48" t="s">
+        <v>601</v>
+      </c>
+      <c r="C48" t="s">
+        <v>575</v>
+      </c>
+      <c r="D48" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49" s="42">
+        <v>28300</v>
+      </c>
+      <c r="B49" t="s">
+        <v>567</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>606</v>
+      </c>
+      <c r="E49">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>30400</v>
+      </c>
+      <c r="B50" t="s">
+        <v>644</v>
+      </c>
+      <c r="C50" t="s">
+        <v>576</v>
+      </c>
+      <c r="D50" t="s">
+        <v>583</v>
+      </c>
+      <c r="E50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" s="42">
+        <v>30700</v>
+      </c>
+      <c r="B51" t="s">
+        <v>602</v>
+      </c>
+      <c r="C51" t="s">
+        <v>575</v>
+      </c>
+      <c r="D51" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" s="42">
+        <v>30900</v>
+      </c>
+      <c r="B52" t="s">
+        <v>643</v>
+      </c>
+      <c r="C52" t="s">
+        <v>575</v>
+      </c>
+      <c r="D52" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53" s="42">
+        <v>31100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>644</v>
+      </c>
+      <c r="C53" t="s">
+        <v>576</v>
+      </c>
+      <c r="D53" t="s">
+        <v>583</v>
+      </c>
+      <c r="E53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" s="42">
+        <v>31300</v>
+      </c>
+      <c r="B54" t="s">
+        <v>820</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" s="42">
+        <v>31400</v>
+      </c>
+      <c r="B55" t="s">
+        <v>820</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" s="42">
+        <v>32200</v>
+      </c>
+      <c r="B56" t="s">
+        <v>603</v>
+      </c>
+      <c r="C56" t="s">
+        <v>575</v>
+      </c>
+      <c r="D56" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57" s="42">
+        <v>32300</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>826</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F122" xr:uid="{4CD7727A-D3C7-4DD7-AD54-8F6EE120CBB6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F57">
+      <sortCondition ref="A1:A122"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A29">
+    <sortCondition ref="A2:A29"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -10917,11 +12022,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
@@ -11336,7 +12441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FB34A4-CC11-43B7-A0E1-7E36604CB0F9}">
   <dimension ref="A1:D36"/>
   <sheetViews>
@@ -11828,7 +12933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8629E7C5-043E-4A29-9B03-D70DB32336F4}">
   <dimension ref="A1:I23"/>
   <sheetViews>

</xml_diff>

<commit_message>
Passagier consists HvN 2022
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90700BF-149F-4FD3-9DCD-09E5A64158A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C52A98-6381-4EA3-9622-08EDD26F464D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6742" yWindow="5783" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{428C447F-3560-4B7D-B002-B0A3F8A1BE88}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{DD718A40-EB37-4C6E-BA23-E511F95E1997}">
       <text>
         <r>
           <rPr>
@@ -474,11 +474,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-DDZ alleen 1x6 bakken</t>
+zazo</t>
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{6BECAE74-5D00-4BB6-B0D6-6D39894B72B1}">
+    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{6BECAE74-5D00-4BB6-B0D6-6D39894B72B1}">
       <text>
         <r>
           <rPr>
@@ -503,7 +503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{77AFD862-B4EA-429F-BB66-A98C2B8B3480}">
+    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{77AFD862-B4EA-429F-BB66-A98C2B8B3480}">
       <text>
         <r>
           <rPr>
@@ -527,7 +527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A50" authorId="0" shapeId="0" xr:uid="{DD718A40-EB37-4C6E-BA23-E511F95E1997}">
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{428C447F-3560-4B7D-B002-B0A3F8A1BE88}">
       <text>
         <r>
           <rPr>
@@ -547,7 +547,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-zazo</t>
+DDZ alleen 1x6 bakken</t>
         </r>
       </text>
     </comment>
@@ -10628,8 +10628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D33F517-9C34-403A-A4F3-107C3F8D830D}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10663,883 +10663,883 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="42">
-        <v>100</v>
+        <v>17800</v>
       </c>
       <c r="B2" t="s">
-        <v>539</v>
-      </c>
-      <c r="D2" t="s">
-        <v>586</v>
+        <v>643</v>
+      </c>
+      <c r="C2" t="s">
+        <v>575</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="42">
-        <v>120</v>
+      <c r="A3">
+        <v>30400</v>
       </c>
       <c r="B3" t="s">
-        <v>539</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>586</v>
+        <v>644</v>
+      </c>
+      <c r="C3" t="s">
+        <v>576</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>583</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="42">
-        <v>140</v>
+        <v>30900</v>
       </c>
       <c r="B4" t="s">
-        <v>808</v>
-      </c>
-      <c r="D4" t="s">
-        <v>578</v>
+        <v>643</v>
+      </c>
+      <c r="C4" t="s">
+        <v>575</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="42">
-        <v>150</v>
+        <v>31100</v>
       </c>
       <c r="B5" t="s">
-        <v>539</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>586</v>
+        <v>644</v>
+      </c>
+      <c r="C5" t="s">
+        <v>576</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>583</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="42">
-        <v>240</v>
+        <v>20000</v>
       </c>
       <c r="B6" t="s">
-        <v>808</v>
-      </c>
-      <c r="D6" t="s">
-        <v>578</v>
+        <v>601</v>
+      </c>
+      <c r="C6" t="s">
+        <v>575</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="42">
-        <v>250</v>
+        <v>30700</v>
       </c>
       <c r="B7" t="s">
-        <v>539</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>586</v>
+        <v>602</v>
+      </c>
+      <c r="C7" t="s">
+        <v>575</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="42">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>809</v>
-      </c>
-      <c r="D8" t="s">
+        <v>539</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="42">
-        <v>420</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>809</v>
-      </c>
-      <c r="D9" t="s">
+        <v>539</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" s="42" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="42">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>563</v>
+        <v>539</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
-        <v>556</v>
-      </c>
-      <c r="E10">
-        <v>190</v>
+      <c r="D10" s="42" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="42">
-        <v>600</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>563</v>
+        <v>539</v>
       </c>
       <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>556</v>
-      </c>
-      <c r="E11">
-        <v>290</v>
+        <v>7</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="42">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="B12" t="s">
-        <v>563</v>
-      </c>
-      <c r="C12">
-        <v>9</v>
+        <v>809</v>
       </c>
       <c r="D12" t="s">
-        <v>556</v>
-      </c>
-      <c r="E12">
-        <v>250</v>
+        <v>586</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="42">
-        <v>800</v>
+        <v>420</v>
       </c>
       <c r="B13" t="s">
-        <v>549</v>
-      </c>
-      <c r="C13">
-        <v>8</v>
+        <v>809</v>
       </c>
       <c r="D13" t="s">
-        <v>557</v>
-      </c>
-      <c r="E13">
-        <v>230</v>
+        <v>586</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="42">
-        <v>1500</v>
+        <v>32200</v>
       </c>
       <c r="B14" t="s">
-        <v>563</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>556</v>
-      </c>
-      <c r="E14">
-        <v>190</v>
+        <v>603</v>
+      </c>
+      <c r="C14" t="s">
+        <v>575</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="42">
-        <v>1600</v>
+        <v>31300</v>
       </c>
       <c r="B15" t="s">
-        <v>825</v>
-      </c>
-      <c r="C15" t="s">
-        <v>810</v>
-      </c>
-      <c r="D15" t="s">
-        <v>611</v>
-      </c>
-      <c r="E15">
-        <v>250</v>
-      </c>
-      <c r="F15" t="s">
-        <v>811</v>
+        <v>820</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="42">
-        <v>1700</v>
+        <v>31400</v>
       </c>
       <c r="B16" t="s">
-        <v>825</v>
-      </c>
-      <c r="C16" t="s">
-        <v>812</v>
-      </c>
-      <c r="D16" t="s">
-        <v>611</v>
-      </c>
-      <c r="F16" t="s">
-        <v>813</v>
+        <v>820</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="42">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="B17" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="C17">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>556</v>
+        <v>12</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="42">
-        <v>2800</v>
+        <v>5500</v>
       </c>
       <c r="B18" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="C18">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>556</v>
+        <v>6</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>606</v>
       </c>
       <c r="E18">
-        <v>220</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="42">
-        <v>2900</v>
+        <v>5700</v>
       </c>
       <c r="B19" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="C19">
         <v>10</v>
       </c>
-      <c r="D19" t="s">
-        <v>557</v>
+      <c r="D19" s="42" t="s">
+        <v>606</v>
       </c>
       <c r="E19">
-        <v>280</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="42">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="B20" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
-      <c r="D20" t="s">
-        <v>557</v>
+      <c r="D20" s="42" t="s">
+        <v>606</v>
       </c>
       <c r="E20">
-        <v>280</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="42">
-        <v>3100</v>
+        <v>6900</v>
       </c>
       <c r="B21" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="C21">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>557</v>
-      </c>
-      <c r="E21">
-        <v>230</v>
+        <v>12</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="51">
-        <v>3200</v>
+      <c r="A22" s="42">
+        <v>8800</v>
       </c>
       <c r="B22" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="C22">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>557</v>
+        <v>10</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E22">
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="42">
-        <v>3500</v>
+        <v>8900</v>
       </c>
       <c r="B23" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="C23">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>557</v>
+        <v>10</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E23">
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="42">
-        <v>3600</v>
+        <v>14900</v>
       </c>
       <c r="B24" t="s">
-        <v>814</v>
+        <v>567</v>
       </c>
       <c r="C24">
         <v>6</v>
       </c>
-      <c r="D24" t="s">
-        <v>824</v>
+      <c r="D24" s="42" t="s">
+        <v>606</v>
       </c>
       <c r="E24">
-        <v>170</v>
-      </c>
-      <c r="F24" t="s">
-        <v>815</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="52">
-        <v>3700</v>
+      <c r="A25" s="42">
+        <v>15600</v>
       </c>
       <c r="B25" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>557</v>
+        <v>4</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>606</v>
       </c>
       <c r="E25">
-        <v>170</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="42">
-        <v>3900</v>
+        <v>28300</v>
       </c>
       <c r="B26" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="C26">
-        <v>6</v>
-      </c>
-      <c r="D26" t="s">
-        <v>557</v>
+        <v>4</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>606</v>
       </c>
       <c r="E26">
-        <v>170</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="42">
-        <v>4000</v>
+        <v>7300</v>
       </c>
       <c r="B27" t="s">
-        <v>567</v>
+        <v>818</v>
       </c>
       <c r="C27">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>606</v>
+        <v>6</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>822</v>
+      </c>
+      <c r="E27">
+        <v>110</v>
+      </c>
+      <c r="F27" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="42">
-        <v>4900</v>
+        <v>7400</v>
       </c>
       <c r="B28" t="s">
-        <v>550</v>
+        <v>818</v>
       </c>
       <c r="C28">
-        <v>7</v>
-      </c>
-      <c r="D28" t="s">
-        <v>609</v>
-      </c>
-      <c r="E28">
-        <v>150</v>
+        <v>11</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>822</v>
+      </c>
+      <c r="F28" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="42">
-        <v>5500</v>
+        <v>800</v>
       </c>
       <c r="B29" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
       <c r="C29">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>606</v>
+        <v>8</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>557</v>
       </c>
       <c r="E29">
-        <v>110</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="42">
-        <v>5600</v>
+        <v>2900</v>
       </c>
       <c r="B30" t="s">
-        <v>568</v>
+        <v>549</v>
       </c>
       <c r="C30">
         <v>10</v>
       </c>
-      <c r="D30" t="s">
-        <v>558</v>
+      <c r="D30" s="42" t="s">
+        <v>557</v>
       </c>
       <c r="E30">
-        <v>210</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="42">
-        <v>5700</v>
+        <v>3000</v>
       </c>
       <c r="B31" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
       <c r="C31">
         <v>10</v>
       </c>
-      <c r="D31" t="s">
-        <v>606</v>
+      <c r="D31" s="42" t="s">
+        <v>557</v>
       </c>
       <c r="E31">
-        <v>180</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="42">
-        <v>6000</v>
+        <v>3100</v>
       </c>
       <c r="B32" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
       <c r="C32">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>606</v>
+        <v>8</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>557</v>
       </c>
       <c r="E32">
-        <v>180</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="42">
-        <v>6600</v>
+      <c r="A33" s="51">
+        <v>3200</v>
       </c>
       <c r="B33" t="s">
-        <v>572</v>
-      </c>
-      <c r="C33" t="s">
-        <v>817</v>
-      </c>
-      <c r="D33" t="s">
-        <v>821</v>
-      </c>
-      <c r="F33" t="s">
-        <v>816</v>
+        <v>549</v>
+      </c>
+      <c r="C33">
+        <v>12</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="42">
-        <v>6900</v>
+        <v>3500</v>
       </c>
       <c r="B34" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
       <c r="C34">
         <v>12</v>
       </c>
-      <c r="D34" t="s">
-        <v>606</v>
+      <c r="D34" s="42" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="42">
-        <v>7000</v>
+      <c r="A35" s="52">
+        <v>3700</v>
       </c>
       <c r="B35" t="s">
-        <v>568</v>
+        <v>549</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
-      <c r="D35" t="s">
-        <v>558</v>
+      <c r="D35" s="42" t="s">
+        <v>557</v>
       </c>
       <c r="E35">
-        <v>130</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="42">
-        <v>7300</v>
+        <v>3900</v>
       </c>
       <c r="B36" t="s">
-        <v>818</v>
+        <v>549</v>
       </c>
       <c r="C36">
         <v>6</v>
       </c>
-      <c r="D36" t="s">
-        <v>822</v>
+      <c r="D36" s="42" t="s">
+        <v>557</v>
       </c>
       <c r="E36">
-        <v>110</v>
-      </c>
-      <c r="F36" t="s">
-        <v>595</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="42">
-        <v>7400</v>
+        <v>3600</v>
       </c>
       <c r="B37" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="C37">
-        <v>11</v>
-      </c>
-      <c r="D37" t="s">
-        <v>822</v>
+        <v>6</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>824</v>
+      </c>
+      <c r="E37">
+        <v>170</v>
       </c>
       <c r="F37" t="s">
-        <v>595</v>
+        <v>815</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="42">
-        <v>7500</v>
+        <v>500</v>
       </c>
       <c r="B38" t="s">
-        <v>819</v>
+        <v>563</v>
       </c>
       <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
-        <v>823</v>
+        <v>7</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>556</v>
       </c>
       <c r="E38">
-        <v>80</v>
-      </c>
-      <c r="F38" t="s">
-        <v>595</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="42">
-        <v>7600</v>
+        <v>600</v>
       </c>
       <c r="B39" t="s">
-        <v>550</v>
+        <v>563</v>
       </c>
       <c r="C39">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>609</v>
+        <v>10</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>556</v>
       </c>
       <c r="E39">
-        <v>140</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="42">
-        <v>8800</v>
+        <v>700</v>
       </c>
       <c r="B40" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C40">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>606</v>
+        <v>9</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>556</v>
       </c>
       <c r="E40">
-        <v>180</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="42">
-        <v>8900</v>
+        <v>1500</v>
       </c>
       <c r="B41" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C41">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>606</v>
+        <v>7</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>556</v>
       </c>
       <c r="E41">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="42">
-        <v>11600</v>
+        <v>2000</v>
       </c>
       <c r="B42" t="s">
-        <v>825</v>
+        <v>563</v>
       </c>
       <c r="C42">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>611</v>
-      </c>
-      <c r="E42">
-        <v>170</v>
-      </c>
-      <c r="F42" t="s">
-        <v>594</v>
+        <v>11</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="42">
-        <v>11700</v>
+        <v>2800</v>
       </c>
       <c r="B43" t="s">
-        <v>825</v>
-      </c>
-      <c r="C43" t="s">
-        <v>571</v>
-      </c>
-      <c r="D43" t="s">
-        <v>611</v>
+        <v>563</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>556</v>
       </c>
       <c r="E43">
-        <v>290</v>
-      </c>
-      <c r="F43" t="s">
-        <v>816</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="42">
-        <v>14900</v>
+        <v>1600</v>
       </c>
       <c r="B44" t="s">
-        <v>567</v>
-      </c>
-      <c r="C44">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>606</v>
+        <v>825</v>
+      </c>
+      <c r="C44" t="s">
+        <v>810</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>611</v>
       </c>
       <c r="E44">
-        <v>110</v>
+        <v>250</v>
+      </c>
+      <c r="F44" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="42">
-        <v>15600</v>
+        <v>1700</v>
       </c>
       <c r="B45" t="s">
-        <v>567</v>
-      </c>
-      <c r="C45">
-        <v>4</v>
-      </c>
-      <c r="D45" t="s">
-        <v>606</v>
-      </c>
-      <c r="E45">
-        <v>80</v>
+        <v>825</v>
+      </c>
+      <c r="C45" t="s">
+        <v>812</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>611</v>
+      </c>
+      <c r="F45" t="s">
+        <v>813</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="42">
-        <v>15800</v>
+        <v>11600</v>
       </c>
       <c r="B46" t="s">
-        <v>568</v>
+        <v>825</v>
       </c>
       <c r="C46">
-        <v>8</v>
-      </c>
-      <c r="D46" t="s">
-        <v>558</v>
+        <v>6</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>611</v>
       </c>
       <c r="E46">
-        <v>160</v>
+        <v>170</v>
+      </c>
+      <c r="F46" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="42">
-        <v>17800</v>
+        <v>11700</v>
       </c>
       <c r="B47" t="s">
-        <v>643</v>
+        <v>825</v>
       </c>
       <c r="C47" t="s">
-        <v>575</v>
-      </c>
-      <c r="D47" t="s">
-        <v>583</v>
+        <v>571</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>611</v>
+      </c>
+      <c r="E47">
+        <v>290</v>
+      </c>
+      <c r="F47" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="42">
-        <v>20000</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
-        <v>601</v>
-      </c>
-      <c r="C48" t="s">
-        <v>575</v>
-      </c>
-      <c r="D48" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+        <v>808</v>
+      </c>
+      <c r="D48" s="42" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="42">
-        <v>28300</v>
+        <v>240</v>
       </c>
       <c r="B49" t="s">
-        <v>567</v>
-      </c>
-      <c r="C49">
+        <v>808</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="42">
+        <v>5600</v>
+      </c>
+      <c r="B50" t="s">
+        <v>568</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>558</v>
+      </c>
+      <c r="E50">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="42">
+        <v>7000</v>
+      </c>
+      <c r="B51" t="s">
+        <v>568</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>558</v>
+      </c>
+      <c r="E51">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="42">
+        <v>15800</v>
+      </c>
+      <c r="B52" t="s">
+        <v>568</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="D52" s="42" t="s">
+        <v>558</v>
+      </c>
+      <c r="E52">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="42">
+        <v>7500</v>
+      </c>
+      <c r="B53" t="s">
+        <v>819</v>
+      </c>
+      <c r="C53">
         <v>4</v>
       </c>
-      <c r="D49" t="s">
-        <v>606</v>
-      </c>
-      <c r="E49">
+      <c r="D53" s="42" t="s">
+        <v>823</v>
+      </c>
+      <c r="E53">
         <v>80</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A50">
-        <v>30400</v>
-      </c>
-      <c r="B50" t="s">
-        <v>644</v>
-      </c>
-      <c r="C50" t="s">
-        <v>576</v>
-      </c>
-      <c r="D50" t="s">
-        <v>583</v>
-      </c>
-      <c r="E50">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51" s="42">
-        <v>30700</v>
-      </c>
-      <c r="B51" t="s">
-        <v>602</v>
-      </c>
-      <c r="C51" t="s">
-        <v>575</v>
-      </c>
-      <c r="D51" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52" s="42">
-        <v>30900</v>
-      </c>
-      <c r="B52" t="s">
-        <v>643</v>
-      </c>
-      <c r="C52" t="s">
-        <v>575</v>
-      </c>
-      <c r="D52" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53" s="42">
-        <v>31100</v>
-      </c>
-      <c r="B53" t="s">
-        <v>644</v>
-      </c>
-      <c r="C53" t="s">
-        <v>576</v>
-      </c>
-      <c r="D53" t="s">
-        <v>583</v>
-      </c>
-      <c r="E53">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F53" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="42">
-        <v>31300</v>
+        <v>4900</v>
       </c>
       <c r="B54" t="s">
-        <v>820</v>
+        <v>550</v>
       </c>
       <c r="C54">
-        <v>3</v>
-      </c>
-      <c r="D54" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>609</v>
+      </c>
+      <c r="E54">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="42">
-        <v>31400</v>
+        <v>7600</v>
       </c>
       <c r="B55" t="s">
-        <v>820</v>
+        <v>550</v>
       </c>
       <c r="C55">
-        <v>3</v>
-      </c>
-      <c r="D55" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>609</v>
+      </c>
+      <c r="E55">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="42">
-        <v>32200</v>
+        <v>6600</v>
       </c>
       <c r="B56" t="s">
-        <v>603</v>
+        <v>572</v>
       </c>
       <c r="C56" t="s">
-        <v>575</v>
-      </c>
-      <c r="D56" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+        <v>817</v>
+      </c>
+      <c r="D56" s="42" t="s">
+        <v>821</v>
+      </c>
+      <c r="F56" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="42">
         <v>32300</v>
       </c>
@@ -11550,7 +11550,7 @@
   </sheetData>
   <autoFilter ref="A1:F122" xr:uid="{4CD7727A-D3C7-4DD7-AD54-8F6EE120CBB6}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F57">
-      <sortCondition ref="A1:A122"/>
+      <sortCondition ref="D1:D122"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A29">

</xml_diff>

<commit_message>
[2200] Finish AI all the way to Vs
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC6ED6D-B04E-45DE-BC3C-FF5A49285BD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE198FA-EFDA-4615-9EC6-16952DA62219}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7140" yWindow="2107" windowWidth="14400" windowHeight="7486" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3405,13 +3405,6 @@
 - cRbSloe25 Rsd-Bgn</t>
   </si>
   <si>
-    <t>- IJsm/Rtst
-- Kfh
-- Ddr
-- Zlw
-- Rsd</t>
-  </si>
-  <si>
     <t>Ddr-Rsd:
 - cDdrZwd10
 - cDdzdDdr10
@@ -3432,7 +3425,19 @@
 - cGsBzl25 Rb-Bgn
 - 2201 Kbd
 - cGsBzl25 Krg
-- 2201 Gs</t>
+- 2201 Gs
+Gs-Vs:
+- cGsBzl25 Lwd-Ha
+- 2001 Mdb</t>
+  </si>
+  <si>
+    <t>- IJsm/Rtst
+- Kfh
+- Ddr
+- Zlw
+- Rsd
+- Gs (QD 1100 + MarcD sik)
+- Vs</t>
   </si>
 </sst>
 </file>
@@ -11579,7 +11584,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12041,7 +12046,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12425,24 +12430,26 @@
       <c r="F13" s="40" t="s">
         <v>802</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="40" t="s">
         <v>803</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="40" t="s">
         <v>824</v>
       </c>
-      <c r="I13" s="46" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="I13" s="40" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="342" x14ac:dyDescent="0.45">
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
-      <c r="G14" s="41" t="s">
-        <v>826</v>
-      </c>
+      <c r="G14" s="40" t="s">
+        <v>825</v>
+      </c>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
ERROR [3101] research. Somda not up to date yet.
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE198FA-EFDA-4615-9EC6-16952DA62219}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD4220-538F-438C-9384-CE031535309A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7140" yWindow="2107" windowWidth="14400" windowHeight="7486" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
     <sheet name="Goederentreinen" sheetId="9" r:id="rId2"/>
     <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId3"/>
-    <sheet name="HvN-Treinseries 2022" sheetId="18" r:id="rId4"/>
-    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId5"/>
+    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId4"/>
+    <sheet name="HvN-Treinseries 2022" sheetId="18" r:id="rId5"/>
     <sheet name="Scenarios" sheetId="14" r:id="rId6"/>
     <sheet name="Vervoerders" sheetId="7" r:id="rId7"/>
     <sheet name="ICRm" sheetId="17" r:id="rId8"/>
@@ -26,8 +26,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'HvN-Treinseries 2022'!$A$1:$F$122</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HvN-Treinseries 2022'!$A$1:$F$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -454,7 +454,41 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{DD718A40-EB37-4C6E-BA23-E511F95E1997}">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+10 Rtd-Rsd, 6 Rsd-Vs</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{428C447F-3560-4B7D-B002-B0A3F8A1BE88}">
       <text>
         <r>
           <rPr>
@@ -474,11 +508,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-zazo</t>
+DDZ alleen 1x6 bakken</t>
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{6BECAE74-5D00-4BB6-B0D6-6D39894B72B1}">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{6BECAE74-5D00-4BB6-B0D6-6D39894B72B1}">
       <text>
         <r>
           <rPr>
@@ -503,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{77AFD862-B4EA-429F-BB66-A98C2B8B3480}">
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{77AFD862-B4EA-429F-BB66-A98C2B8B3480}">
       <text>
         <r>
           <rPr>
@@ -527,7 +561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{428C447F-3560-4B7D-B002-B0A3F8A1BE88}">
+    <comment ref="A50" authorId="0" shapeId="0" xr:uid="{DD718A40-EB37-4C6E-BA23-E511F95E1997}">
       <text>
         <r>
           <rPr>
@@ -547,41 +581,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-DDZ alleen 1x6 bakken</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Tom</author>
-  </authors>
-  <commentList>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{02553BA0-0343-4B61-AEAC-7BE617765AB4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-10 Rtd-Rsd, 6 Rsd-Vs</t>
+zazo</t>
         </r>
       </text>
     </comment>
@@ -619,12 +619,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{C65A4037-B9CE-4ECD-A63A-FE0C8574D8C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+somda drgl klopt niet :(
+my bad, zie https://www.somda.nl/forum/24550/invoeren-aanpassen-van-dienstregeling-2022/</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="831">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3438,6 +3463,53 @@
 - Rsd
 - Gs (QD 1100 + MarcD sik)
 - Vs</t>
+  </si>
+  <si>
+    <t>3101 Ut-Db-Ah</t>
+  </si>
+  <si>
+    <t>- Ut19
+- Db
+- Ed</t>
+  </si>
+  <si>
+    <t>Ut:
+- 2000 Ut8
+- 3000 Ut5
+- 3500 Ut7
+- 4901/5700 Ut1
+- 5600/5601 Ut4
+- 6001/8801 Ut21
+- 6900 Ut20
+- cUtoBlw13 Ut9
+Ut-Ah:
+- 7300 Bnk-Ut14
+- 3100 Bnk
+- cKlpHar04 (FG) Bnk(2)
+- 7400 Db
+- 3200 Db(2)
+- 100/120/400 Mrg
+- 401 Mrg?
+- 3000 Har-Mrn
+- 7300 Har
+- 3100 Klp
+- 3200 Ed-Klp
+- cKlpHar09 Ed
+- 7500 Wf-Ed
+- 100/120/c Wf-Ed(2)
+- 3000 Wf-Ed(3)
+- 31100 Ahwa
+- 7600 Ah7</t>
+  </si>
+  <si>
+    <t>Ah:
+- 3100 Ah11
+- 3200/3201 Ah9
+- 6600/6601 Ah4a
+- 7500/7501 Ah10
+- 20000/20001 Ah6a
+- 30700/30701 Ah6b
+- cAhAhb15 Ah7</t>
   </si>
 </sst>
 </file>
@@ -3589,7 +3661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3696,6 +3768,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10643,943 +10718,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D33F517-9C34-403A-A4F3-107C3F8D830D}">
-  <dimension ref="A1:F57"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="13.53125" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.9296875" customWidth="1"/>
-    <col min="5" max="5" width="13.59765625" customWidth="1"/>
-    <col min="6" max="6" width="16.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>553</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="42">
-        <v>17800</v>
-      </c>
-      <c r="B2" t="s">
-        <v>643</v>
-      </c>
-      <c r="C2" t="s">
-        <v>575</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>30400</v>
-      </c>
-      <c r="B3" t="s">
-        <v>644</v>
-      </c>
-      <c r="C3" t="s">
-        <v>576</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>583</v>
-      </c>
-      <c r="E3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="42">
-        <v>30900</v>
-      </c>
-      <c r="B4" t="s">
-        <v>643</v>
-      </c>
-      <c r="C4" t="s">
-        <v>575</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="42">
-        <v>31100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>644</v>
-      </c>
-      <c r="C5" t="s">
-        <v>576</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>583</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="42">
-        <v>20000</v>
-      </c>
-      <c r="B6" t="s">
-        <v>601</v>
-      </c>
-      <c r="C6" t="s">
-        <v>575</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="42">
-        <v>30700</v>
-      </c>
-      <c r="B7" t="s">
-        <v>602</v>
-      </c>
-      <c r="C7" t="s">
-        <v>575</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="42">
-        <v>100</v>
-      </c>
-      <c r="B8" t="s">
-        <v>539</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="42">
-        <v>120</v>
-      </c>
-      <c r="B9" t="s">
-        <v>539</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="42">
-        <v>150</v>
-      </c>
-      <c r="B10" t="s">
-        <v>539</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="42">
-        <v>250</v>
-      </c>
-      <c r="B11" t="s">
-        <v>539</v>
-      </c>
-      <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="42">
-        <v>400</v>
-      </c>
-      <c r="B12" t="s">
-        <v>806</v>
-      </c>
-      <c r="D12" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="42">
-        <v>420</v>
-      </c>
-      <c r="B13" t="s">
-        <v>806</v>
-      </c>
-      <c r="D13" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="42">
-        <v>32200</v>
-      </c>
-      <c r="B14" t="s">
-        <v>603</v>
-      </c>
-      <c r="C14" t="s">
-        <v>575</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="42">
-        <v>31300</v>
-      </c>
-      <c r="B15" t="s">
-        <v>817</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="42">
-        <v>31400</v>
-      </c>
-      <c r="B16" t="s">
-        <v>817</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="42">
-        <v>4000</v>
-      </c>
-      <c r="B17" t="s">
-        <v>567</v>
-      </c>
-      <c r="C17">
-        <v>12</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="42">
-        <v>5500</v>
-      </c>
-      <c r="B18" t="s">
-        <v>567</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="E18">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="42">
-        <v>5700</v>
-      </c>
-      <c r="B19" t="s">
-        <v>567</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="E19">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="42">
-        <v>6000</v>
-      </c>
-      <c r="B20" t="s">
-        <v>567</v>
-      </c>
-      <c r="C20">
-        <v>10</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="E20">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="42">
-        <v>6900</v>
-      </c>
-      <c r="B21" t="s">
-        <v>567</v>
-      </c>
-      <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="42">
-        <v>8800</v>
-      </c>
-      <c r="B22" t="s">
-        <v>567</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="E22">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="42">
-        <v>8900</v>
-      </c>
-      <c r="B23" t="s">
-        <v>567</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="E23">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="42">
-        <v>14900</v>
-      </c>
-      <c r="B24" t="s">
-        <v>567</v>
-      </c>
-      <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="E24">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="42">
-        <v>15600</v>
-      </c>
-      <c r="B25" t="s">
-        <v>567</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="E25">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="42">
-        <v>28300</v>
-      </c>
-      <c r="B26" t="s">
-        <v>567</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="E26">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="42">
-        <v>7300</v>
-      </c>
-      <c r="B27" t="s">
-        <v>815</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>819</v>
-      </c>
-      <c r="E27">
-        <v>110</v>
-      </c>
-      <c r="F27" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="42">
-        <v>7400</v>
-      </c>
-      <c r="B28" t="s">
-        <v>815</v>
-      </c>
-      <c r="C28">
-        <v>11</v>
-      </c>
-      <c r="D28" s="42" t="s">
-        <v>819</v>
-      </c>
-      <c r="F28" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="42">
-        <v>800</v>
-      </c>
-      <c r="B29" t="s">
-        <v>549</v>
-      </c>
-      <c r="C29">
-        <v>8</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>557</v>
-      </c>
-      <c r="E29">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="42">
-        <v>2900</v>
-      </c>
-      <c r="B30" t="s">
-        <v>549</v>
-      </c>
-      <c r="C30">
-        <v>10</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>557</v>
-      </c>
-      <c r="E30">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="42">
-        <v>3000</v>
-      </c>
-      <c r="B31" t="s">
-        <v>549</v>
-      </c>
-      <c r="C31">
-        <v>10</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>557</v>
-      </c>
-      <c r="E31">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="42">
-        <v>3100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>549</v>
-      </c>
-      <c r="C32">
-        <v>8</v>
-      </c>
-      <c r="D32" s="42" t="s">
-        <v>557</v>
-      </c>
-      <c r="E32">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="50">
-        <v>3200</v>
-      </c>
-      <c r="B33" t="s">
-        <v>549</v>
-      </c>
-      <c r="C33">
-        <v>12</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="42">
-        <v>3500</v>
-      </c>
-      <c r="B34" t="s">
-        <v>549</v>
-      </c>
-      <c r="C34">
-        <v>12</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="51">
-        <v>3700</v>
-      </c>
-      <c r="B35" t="s">
-        <v>549</v>
-      </c>
-      <c r="C35">
-        <v>6</v>
-      </c>
-      <c r="D35" s="42" t="s">
-        <v>557</v>
-      </c>
-      <c r="E35">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="42">
-        <v>3900</v>
-      </c>
-      <c r="B36" t="s">
-        <v>549</v>
-      </c>
-      <c r="C36">
-        <v>6</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>557</v>
-      </c>
-      <c r="E36">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="42">
-        <v>3600</v>
-      </c>
-      <c r="B37" t="s">
-        <v>811</v>
-      </c>
-      <c r="C37">
-        <v>6</v>
-      </c>
-      <c r="D37" s="42" t="s">
-        <v>821</v>
-      </c>
-      <c r="E37">
-        <v>170</v>
-      </c>
-      <c r="F37" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="42">
-        <v>500</v>
-      </c>
-      <c r="B38" t="s">
-        <v>563</v>
-      </c>
-      <c r="C38">
-        <v>7</v>
-      </c>
-      <c r="D38" s="42" t="s">
-        <v>556</v>
-      </c>
-      <c r="E38">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="42">
-        <v>600</v>
-      </c>
-      <c r="B39" t="s">
-        <v>563</v>
-      </c>
-      <c r="C39">
-        <v>10</v>
-      </c>
-      <c r="D39" s="42" t="s">
-        <v>556</v>
-      </c>
-      <c r="E39">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="42">
-        <v>700</v>
-      </c>
-      <c r="B40" t="s">
-        <v>563</v>
-      </c>
-      <c r="C40">
-        <v>9</v>
-      </c>
-      <c r="D40" s="42" t="s">
-        <v>556</v>
-      </c>
-      <c r="E40">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="42">
-        <v>1500</v>
-      </c>
-      <c r="B41" t="s">
-        <v>563</v>
-      </c>
-      <c r="C41">
-        <v>7</v>
-      </c>
-      <c r="D41" s="42" t="s">
-        <v>556</v>
-      </c>
-      <c r="E41">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="42">
-        <v>2000</v>
-      </c>
-      <c r="B42" t="s">
-        <v>563</v>
-      </c>
-      <c r="C42">
-        <v>11</v>
-      </c>
-      <c r="D42" s="42" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="42">
-        <v>2800</v>
-      </c>
-      <c r="B43" t="s">
-        <v>563</v>
-      </c>
-      <c r="C43">
-        <v>8</v>
-      </c>
-      <c r="D43" s="42" t="s">
-        <v>556</v>
-      </c>
-      <c r="E43">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="42">
-        <v>1600</v>
-      </c>
-      <c r="B44" t="s">
-        <v>822</v>
-      </c>
-      <c r="C44" t="s">
-        <v>807</v>
-      </c>
-      <c r="D44" s="42" t="s">
-        <v>611</v>
-      </c>
-      <c r="E44">
-        <v>250</v>
-      </c>
-      <c r="F44" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="42">
-        <v>1700</v>
-      </c>
-      <c r="B45" t="s">
-        <v>822</v>
-      </c>
-      <c r="C45" t="s">
-        <v>809</v>
-      </c>
-      <c r="D45" s="42" t="s">
-        <v>611</v>
-      </c>
-      <c r="F45" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="42">
-        <v>11600</v>
-      </c>
-      <c r="B46" t="s">
-        <v>822</v>
-      </c>
-      <c r="C46">
-        <v>6</v>
-      </c>
-      <c r="D46" s="42" t="s">
-        <v>611</v>
-      </c>
-      <c r="E46">
-        <v>170</v>
-      </c>
-      <c r="F46" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="42">
-        <v>11700</v>
-      </c>
-      <c r="B47" t="s">
-        <v>822</v>
-      </c>
-      <c r="C47" t="s">
-        <v>571</v>
-      </c>
-      <c r="D47" s="42" t="s">
-        <v>611</v>
-      </c>
-      <c r="E47">
-        <v>290</v>
-      </c>
-      <c r="F47" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="42">
-        <v>140</v>
-      </c>
-      <c r="B48" t="s">
-        <v>805</v>
-      </c>
-      <c r="D48" s="42" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="42">
-        <v>240</v>
-      </c>
-      <c r="B49" t="s">
-        <v>805</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="42">
-        <v>5600</v>
-      </c>
-      <c r="B50" t="s">
-        <v>568</v>
-      </c>
-      <c r="C50">
-        <v>10</v>
-      </c>
-      <c r="D50" s="42" t="s">
-        <v>558</v>
-      </c>
-      <c r="E50">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="42">
-        <v>7000</v>
-      </c>
-      <c r="B51" t="s">
-        <v>568</v>
-      </c>
-      <c r="C51">
-        <v>6</v>
-      </c>
-      <c r="D51" s="42" t="s">
-        <v>558</v>
-      </c>
-      <c r="E51">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="42">
-        <v>15800</v>
-      </c>
-      <c r="B52" t="s">
-        <v>568</v>
-      </c>
-      <c r="C52">
-        <v>8</v>
-      </c>
-      <c r="D52" s="42" t="s">
-        <v>558</v>
-      </c>
-      <c r="E52">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53" s="42">
-        <v>7500</v>
-      </c>
-      <c r="B53" t="s">
-        <v>816</v>
-      </c>
-      <c r="C53">
-        <v>4</v>
-      </c>
-      <c r="D53" s="42" t="s">
-        <v>820</v>
-      </c>
-      <c r="E53">
-        <v>80</v>
-      </c>
-      <c r="F53" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" s="42">
-        <v>4900</v>
-      </c>
-      <c r="B54" t="s">
-        <v>550</v>
-      </c>
-      <c r="C54">
-        <v>7</v>
-      </c>
-      <c r="D54" s="42" t="s">
-        <v>609</v>
-      </c>
-      <c r="E54">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A55" s="42">
-        <v>7600</v>
-      </c>
-      <c r="B55" t="s">
-        <v>550</v>
-      </c>
-      <c r="C55">
-        <v>6</v>
-      </c>
-      <c r="D55" s="42" t="s">
-        <v>609</v>
-      </c>
-      <c r="E55">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A56" s="42">
-        <v>6600</v>
-      </c>
-      <c r="B56" t="s">
-        <v>572</v>
-      </c>
-      <c r="C56" t="s">
-        <v>814</v>
-      </c>
-      <c r="D56" s="42" t="s">
-        <v>818</v>
-      </c>
-      <c r="F56" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="42">
-        <v>32300</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>823</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F122" xr:uid="{4CD7727A-D3C7-4DD7-AD54-8F6EE120CBB6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F57">
-      <sortCondition ref="D1:D122"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A29">
-    <sortCondition ref="A2:A29"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -12040,13 +11178,950 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D33F517-9C34-403A-A4F3-107C3F8D830D}">
+  <dimension ref="A1:F57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.53125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.9296875" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" customWidth="1"/>
+    <col min="6" max="6" width="16.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="42">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="42">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="42">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>805</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="42">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="42">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>805</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="42">
+        <v>250</v>
+      </c>
+      <c r="B7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="42">
+        <v>400</v>
+      </c>
+      <c r="B8" t="s">
+        <v>806</v>
+      </c>
+      <c r="D8" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="42">
+        <v>420</v>
+      </c>
+      <c r="B9" t="s">
+        <v>806</v>
+      </c>
+      <c r="D9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="42">
+        <v>500</v>
+      </c>
+      <c r="B10" t="s">
+        <v>563</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>556</v>
+      </c>
+      <c r="E10">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="42">
+        <v>600</v>
+      </c>
+      <c r="B11" t="s">
+        <v>563</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>556</v>
+      </c>
+      <c r="E11">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="42">
+        <v>700</v>
+      </c>
+      <c r="B12" t="s">
+        <v>563</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>556</v>
+      </c>
+      <c r="E12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="42">
+        <v>800</v>
+      </c>
+      <c r="B13" t="s">
+        <v>549</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E13">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="42">
+        <v>1500</v>
+      </c>
+      <c r="B14" t="s">
+        <v>563</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>556</v>
+      </c>
+      <c r="E14">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="42">
+        <v>1600</v>
+      </c>
+      <c r="B15" t="s">
+        <v>822</v>
+      </c>
+      <c r="C15" t="s">
+        <v>807</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>611</v>
+      </c>
+      <c r="E15">
+        <v>250</v>
+      </c>
+      <c r="F15" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="42">
+        <v>1700</v>
+      </c>
+      <c r="B16" t="s">
+        <v>822</v>
+      </c>
+      <c r="C16" t="s">
+        <v>809</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>611</v>
+      </c>
+      <c r="F16" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="42">
+        <v>2000</v>
+      </c>
+      <c r="B17" t="s">
+        <v>563</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="42">
+        <v>2800</v>
+      </c>
+      <c r="B18" t="s">
+        <v>563</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>556</v>
+      </c>
+      <c r="E18">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="42">
+        <v>2900</v>
+      </c>
+      <c r="B19" t="s">
+        <v>549</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E19">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="42">
+        <v>3000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>549</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E20">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="42">
+        <v>3100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>549</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E21">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="50">
+        <v>3200</v>
+      </c>
+      <c r="B22" t="s">
+        <v>549</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="42">
+        <v>3500</v>
+      </c>
+      <c r="B23" t="s">
+        <v>549</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="42">
+        <v>3600</v>
+      </c>
+      <c r="B24" t="s">
+        <v>811</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>821</v>
+      </c>
+      <c r="E24">
+        <v>170</v>
+      </c>
+      <c r="F24" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="51">
+        <v>3700</v>
+      </c>
+      <c r="B25" t="s">
+        <v>549</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="42">
+        <v>3900</v>
+      </c>
+      <c r="B26" t="s">
+        <v>549</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E26">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="42">
+        <v>4000</v>
+      </c>
+      <c r="B27" t="s">
+        <v>567</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="42">
+        <v>4900</v>
+      </c>
+      <c r="B28" t="s">
+        <v>550</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>609</v>
+      </c>
+      <c r="E28">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="42">
+        <v>5500</v>
+      </c>
+      <c r="B29" t="s">
+        <v>567</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E29">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="42">
+        <v>5600</v>
+      </c>
+      <c r="B30" t="s">
+        <v>568</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>558</v>
+      </c>
+      <c r="E30">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="42">
+        <v>5700</v>
+      </c>
+      <c r="B31" t="s">
+        <v>567</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E31">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="42">
+        <v>6000</v>
+      </c>
+      <c r="B32" t="s">
+        <v>567</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E32">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="42">
+        <v>6600</v>
+      </c>
+      <c r="B33" t="s">
+        <v>572</v>
+      </c>
+      <c r="C33" t="s">
+        <v>814</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>818</v>
+      </c>
+      <c r="F33" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="42">
+        <v>6900</v>
+      </c>
+      <c r="B34" t="s">
+        <v>567</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="42">
+        <v>7000</v>
+      </c>
+      <c r="B35" t="s">
+        <v>568</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>558</v>
+      </c>
+      <c r="E35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="42">
+        <v>7300</v>
+      </c>
+      <c r="B36" t="s">
+        <v>815</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>819</v>
+      </c>
+      <c r="E36">
+        <v>110</v>
+      </c>
+      <c r="F36" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="42">
+        <v>7400</v>
+      </c>
+      <c r="B37" t="s">
+        <v>815</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>819</v>
+      </c>
+      <c r="F37" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="42">
+        <v>7500</v>
+      </c>
+      <c r="B38" t="s">
+        <v>816</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>820</v>
+      </c>
+      <c r="E38">
+        <v>80</v>
+      </c>
+      <c r="F38" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="42">
+        <v>7600</v>
+      </c>
+      <c r="B39" t="s">
+        <v>550</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>609</v>
+      </c>
+      <c r="E39">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="42">
+        <v>8800</v>
+      </c>
+      <c r="B40" t="s">
+        <v>567</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E40">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="42">
+        <v>8900</v>
+      </c>
+      <c r="B41" t="s">
+        <v>567</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E41">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="42">
+        <v>11600</v>
+      </c>
+      <c r="B42" t="s">
+        <v>822</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>611</v>
+      </c>
+      <c r="E42">
+        <v>170</v>
+      </c>
+      <c r="F42" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="42">
+        <v>11700</v>
+      </c>
+      <c r="B43" t="s">
+        <v>822</v>
+      </c>
+      <c r="C43" t="s">
+        <v>571</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>611</v>
+      </c>
+      <c r="E43">
+        <v>290</v>
+      </c>
+      <c r="F43" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="42">
+        <v>14900</v>
+      </c>
+      <c r="B44" t="s">
+        <v>567</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E44">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="42">
+        <v>15600</v>
+      </c>
+      <c r="B45" t="s">
+        <v>567</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="42">
+        <v>15800</v>
+      </c>
+      <c r="B46" t="s">
+        <v>568</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>558</v>
+      </c>
+      <c r="E46">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="42">
+        <v>17800</v>
+      </c>
+      <c r="B47" t="s">
+        <v>643</v>
+      </c>
+      <c r="C47" t="s">
+        <v>575</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="42">
+        <v>20000</v>
+      </c>
+      <c r="B48" t="s">
+        <v>601</v>
+      </c>
+      <c r="C48" t="s">
+        <v>575</v>
+      </c>
+      <c r="D48" s="42" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49" s="42">
+        <v>28300</v>
+      </c>
+      <c r="B49" t="s">
+        <v>567</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E49">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>30400</v>
+      </c>
+      <c r="B50" t="s">
+        <v>644</v>
+      </c>
+      <c r="C50" t="s">
+        <v>576</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>583</v>
+      </c>
+      <c r="E50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" s="42">
+        <v>30700</v>
+      </c>
+      <c r="B51" t="s">
+        <v>602</v>
+      </c>
+      <c r="C51" t="s">
+        <v>575</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" s="42">
+        <v>30900</v>
+      </c>
+      <c r="B52" t="s">
+        <v>643</v>
+      </c>
+      <c r="C52" t="s">
+        <v>575</v>
+      </c>
+      <c r="D52" s="42" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53" s="42">
+        <v>31100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>644</v>
+      </c>
+      <c r="C53" t="s">
+        <v>576</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>583</v>
+      </c>
+      <c r="E53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" s="42">
+        <v>31300</v>
+      </c>
+      <c r="B54" t="s">
+        <v>817</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" s="42">
+        <v>31400</v>
+      </c>
+      <c r="B55" t="s">
+        <v>817</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" s="42">
+        <v>32200</v>
+      </c>
+      <c r="B56" t="s">
+        <v>603</v>
+      </c>
+      <c r="C56" t="s">
+        <v>575</v>
+      </c>
+      <c r="D56" s="42" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57" s="42">
+        <v>32300</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>823</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F122" xr:uid="{4CD7727A-D3C7-4DD7-AD54-8F6EE120CBB6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F57">
+      <sortCondition ref="A1:A122"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A29">
+    <sortCondition ref="A2:A29"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12450,6 +12525,31 @@
       </c>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
+    </row>
+    <row r="15" spans="1:11" ht="384.75" x14ac:dyDescent="0.45">
+      <c r="A15" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>827</v>
+      </c>
+      <c r="E15" s="52">
+        <v>3022</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>828</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="114" x14ac:dyDescent="0.45">
+      <c r="B16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="38" t="s">
+        <v>830</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add 3101, 7300 to version control
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD4220-538F-438C-9384-CE031535309A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479D96D2-1F13-4DB9-8DCF-0FC07186C08E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8115" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
     <sheet name="Goederentreinen" sheetId="9" r:id="rId2"/>
-    <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId3"/>
-    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId4"/>
-    <sheet name="HvN-Treinseries 2022" sheetId="18" r:id="rId5"/>
+    <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId3"/>
+    <sheet name="HvN-Treinseries 2022" sheetId="18" r:id="rId4"/>
+    <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId5"/>
     <sheet name="Scenarios" sheetId="14" r:id="rId6"/>
     <sheet name="Vervoerders" sheetId="7" r:id="rId7"/>
     <sheet name="ICRm" sheetId="17" r:id="rId8"/>
@@ -25,9 +25,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goederentreinen!$A$2:$R$156</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HvN-Treinseries 2022'!$A$1:$F$122</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'HvN-Treinseries 2022'!$A$1:$F$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -649,7 +649,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="836">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3510,6 +3510,38 @@
 - 20000/20001 Ah6a
 - 30700/30701 Ah6b
 - cAhAhb15 Ah7</t>
+  </si>
+  <si>
+    <t>7300 Rhn-Ut-Bkl</t>
+  </si>
+  <si>
+    <t>Rhn-Ut: https://www.youtube.com/watch?v=VA-6EAtctSA, https://www.youtube.com/watch?v=WFtqaRxnfQs
+Ut-Bkl: https://www.youtube.com/watch?v=FZLvehiQuZo</t>
+  </si>
+  <si>
+    <t>- Rhn
+- Vndc
+- Db
+- Ut</t>
+  </si>
+  <si>
+    <t>- 3000 Har-Utvr</t>
+  </si>
+  <si>
+    <t>Rhn-Ut:
+- 7301 Vndc
+- 7401 Har-Vndw
+- 3101 Har
+- 7301 Mrn
+- 3001 Db-Mrg
+- 7401 Db
+- 101/121/221/421/c Bnk
+- 3101 Utza-Bnk
+- 7301 Utza
+- 6001 Utvr
+- 3901 Utvr
+- 6000 Utln-Ut20
+- TODO cUtUto18</t>
   </si>
 </sst>
 </file>
@@ -3661,7 +3693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3769,6 +3801,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -9756,968 +9794,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
-  <dimension ref="A1:F61"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="21.53125" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="27.46484375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>553</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>539</v>
-      </c>
-      <c r="D2" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>120</v>
-      </c>
-      <c r="B3" t="s">
-        <v>539</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>140</v>
-      </c>
-      <c r="B4" t="s">
-        <v>605</v>
-      </c>
-      <c r="D4" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>220</v>
-      </c>
-      <c r="B5" t="s">
-        <v>539</v>
-      </c>
-      <c r="D5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>240</v>
-      </c>
-      <c r="B6" t="s">
-        <v>605</v>
-      </c>
-      <c r="D6" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>400</v>
-      </c>
-      <c r="B7" t="s">
-        <v>627</v>
-      </c>
-      <c r="D7" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>500</v>
-      </c>
-      <c r="B8" t="s">
-        <v>563</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>600</v>
-      </c>
-      <c r="B9" t="s">
-        <v>563</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>556</v>
-      </c>
-      <c r="E9">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>700</v>
-      </c>
-      <c r="B10" t="s">
-        <v>563</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>800</v>
-      </c>
-      <c r="B11" t="s">
-        <v>549</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>557</v>
-      </c>
-      <c r="E11">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>1500</v>
-      </c>
-      <c r="B12" t="s">
-        <v>566</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>612</v>
-      </c>
-      <c r="E12">
-        <v>200</v>
-      </c>
-      <c r="F12" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>1600</v>
-      </c>
-      <c r="B13" t="s">
-        <v>561</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>608</v>
-      </c>
-      <c r="E13">
-        <v>170</v>
-      </c>
-      <c r="F13" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>1700</v>
-      </c>
-      <c r="B14" t="s">
-        <v>561</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>608</v>
-      </c>
-      <c r="E14">
-        <v>200</v>
-      </c>
-      <c r="F14" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>1800</v>
-      </c>
-      <c r="B15" t="s">
-        <v>563</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>2000</v>
-      </c>
-      <c r="B16" t="s">
-        <v>563</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>556</v>
-      </c>
-      <c r="E16">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>2400</v>
-      </c>
-      <c r="B17" t="s">
-        <v>549</v>
-      </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>557</v>
-      </c>
-      <c r="E17">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>2600</v>
-      </c>
-      <c r="B18" t="s">
-        <v>566</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>612</v>
-      </c>
-      <c r="E18">
-        <v>200</v>
-      </c>
-      <c r="F18" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>2800</v>
-      </c>
-      <c r="B19" t="s">
-        <v>563</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>556</v>
-      </c>
-      <c r="E19">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>2900</v>
-      </c>
-      <c r="B20" t="s">
-        <v>549</v>
-      </c>
-      <c r="C20">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>557</v>
-      </c>
-      <c r="E20">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>3000</v>
-      </c>
-      <c r="B21" t="s">
-        <v>549</v>
-      </c>
-      <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>3100</v>
-      </c>
-      <c r="B22" t="s">
-        <v>549</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>557</v>
-      </c>
-      <c r="E22">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>3500</v>
-      </c>
-      <c r="B23" t="s">
-        <v>549</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>557</v>
-      </c>
-      <c r="E23">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>3600</v>
-      </c>
-      <c r="B24" t="s">
-        <v>549</v>
-      </c>
-      <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>557</v>
-      </c>
-      <c r="E24">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>3900</v>
-      </c>
-      <c r="B25" t="s">
-        <v>549</v>
-      </c>
-      <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>557</v>
-      </c>
-      <c r="E25">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>4000</v>
-      </c>
-      <c r="B26" t="s">
-        <v>567</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>4300</v>
-      </c>
-      <c r="B27" t="s">
-        <v>567</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>606</v>
-      </c>
-      <c r="E27">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>4900</v>
-      </c>
-      <c r="B28" t="s">
-        <v>567</v>
-      </c>
-      <c r="C28">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>606</v>
-      </c>
-      <c r="E28">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>5500</v>
-      </c>
-      <c r="B29" t="s">
-        <v>570</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>580</v>
-      </c>
-      <c r="E29">
-        <v>80</v>
-      </c>
-      <c r="F29" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30">
-        <v>5600</v>
-      </c>
-      <c r="B30" t="s">
-        <v>568</v>
-      </c>
-      <c r="C30">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>558</v>
-      </c>
-      <c r="E30">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31">
-        <v>5700</v>
-      </c>
-      <c r="B31" t="s">
-        <v>567</v>
-      </c>
-      <c r="C31">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>606</v>
-      </c>
-      <c r="E31">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32">
-        <v>6000</v>
-      </c>
-      <c r="B32" t="s">
-        <v>567</v>
-      </c>
-      <c r="C32">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <v>6500</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <v>6600</v>
-      </c>
-      <c r="B34" t="s">
-        <v>550</v>
-      </c>
-      <c r="C34">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35">
-        <v>6900</v>
-      </c>
-      <c r="B35" t="s">
-        <v>567</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>7000</v>
-      </c>
-      <c r="B36" t="s">
-        <v>568</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>558</v>
-      </c>
-      <c r="E36">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37">
-        <v>7300</v>
-      </c>
-      <c r="B37" t="s">
-        <v>567</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>606</v>
-      </c>
-      <c r="E37">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <v>7400</v>
-      </c>
-      <c r="B38" t="s">
-        <v>567</v>
-      </c>
-      <c r="C38">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>606</v>
-      </c>
-      <c r="E38">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39">
-        <v>7500</v>
-      </c>
-      <c r="B39" t="s">
-        <v>596</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>610</v>
-      </c>
-      <c r="E39">
-        <v>80</v>
-      </c>
-      <c r="F39" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40">
-        <v>7600</v>
-      </c>
-      <c r="B40" t="s">
-        <v>568</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>558</v>
-      </c>
-      <c r="E40">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>8800</v>
-      </c>
-      <c r="B41" t="s">
-        <v>597</v>
-      </c>
-      <c r="C41">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>607</v>
-      </c>
-      <c r="F41" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42">
-        <v>11600</v>
-      </c>
-      <c r="B42" t="s">
-        <v>598</v>
-      </c>
-      <c r="C42">
-        <v>5</v>
-      </c>
-      <c r="D42" t="s">
-        <v>611</v>
-      </c>
-      <c r="E42">
-        <v>140</v>
-      </c>
-      <c r="F42" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>11700</v>
-      </c>
-      <c r="B43" t="s">
-        <v>561</v>
-      </c>
-      <c r="C43">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
-        <v>608</v>
-      </c>
-      <c r="E43">
-        <v>200</v>
-      </c>
-      <c r="F43" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>14600</v>
-      </c>
-      <c r="B44" t="s">
-        <v>568</v>
-      </c>
-      <c r="C44">
-        <v>8</v>
-      </c>
-      <c r="D44" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45">
-        <v>14900</v>
-      </c>
-      <c r="B45" t="s">
-        <v>567</v>
-      </c>
-      <c r="C45">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
-        <v>606</v>
-      </c>
-      <c r="E45">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46">
-        <v>15600</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47">
-        <v>15800</v>
-      </c>
-      <c r="B47" t="s">
-        <v>568</v>
-      </c>
-      <c r="C47">
-        <v>8</v>
-      </c>
-      <c r="D47" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <v>17800</v>
-      </c>
-      <c r="B48" t="s">
-        <v>643</v>
-      </c>
-      <c r="C48" t="s">
-        <v>576</v>
-      </c>
-      <c r="D48" t="s">
-        <v>583</v>
-      </c>
-      <c r="E48">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A49">
-        <v>20000</v>
-      </c>
-      <c r="B49" t="s">
-        <v>601</v>
-      </c>
-      <c r="C49" t="s">
-        <v>576</v>
-      </c>
-      <c r="D49" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A50">
-        <v>28300</v>
-      </c>
-      <c r="B50" t="s">
-        <v>567</v>
-      </c>
-      <c r="C50">
-        <v>6</v>
-      </c>
-      <c r="D50" t="s">
-        <v>606</v>
-      </c>
-      <c r="E50">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <v>30700</v>
-      </c>
-      <c r="B51" t="s">
-        <v>602</v>
-      </c>
-      <c r="C51" t="s">
-        <v>576</v>
-      </c>
-      <c r="D51" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A52">
-        <v>30900</v>
-      </c>
-      <c r="B52" t="s">
-        <v>643</v>
-      </c>
-      <c r="C52" t="s">
-        <v>575</v>
-      </c>
-      <c r="D52" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A53">
-        <v>31100</v>
-      </c>
-      <c r="B53" t="s">
-        <v>644</v>
-      </c>
-      <c r="C53" t="s">
-        <v>576</v>
-      </c>
-      <c r="D53" t="s">
-        <v>583</v>
-      </c>
-      <c r="E53">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A54">
-        <v>31300</v>
-      </c>
-      <c r="B54" t="s">
-        <v>604</v>
-      </c>
-      <c r="D54" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A55">
-        <v>31400</v>
-      </c>
-      <c r="B55" t="s">
-        <v>604</v>
-      </c>
-      <c r="D55" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A56">
-        <v>32200</v>
-      </c>
-      <c r="B56" t="s">
-        <v>603</v>
-      </c>
-      <c r="C56" t="s">
-        <v>575</v>
-      </c>
-      <c r="D56" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A57">
-        <v>32300</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>629</v>
-      </c>
-      <c r="B58" t="s">
-        <v>643</v>
-      </c>
-      <c r="C58" t="s">
-        <v>576</v>
-      </c>
-      <c r="D58" t="s">
-        <v>583</v>
-      </c>
-      <c r="E58">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>628</v>
-      </c>
-      <c r="B59" t="s">
-        <v>549</v>
-      </c>
-      <c r="C59">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>557</v>
-      </c>
-      <c r="E59">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>559</v>
-      </c>
-      <c r="D60" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>559</v>
-      </c>
-      <c r="D61" t="s">
-        <v>592</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
-      <sortCondition ref="A1:A61"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
-    <sortCondition ref="A3:A60"/>
-  </sortState>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED858DC8-394D-4594-8BA9-4710557E3293}">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -11178,12 +10254,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D33F517-9C34-403A-A4F3-107C3F8D830D}">
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12115,13 +11191,975 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
+  <dimension ref="A1:F61"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="21.53125" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="27.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>605</v>
+      </c>
+      <c r="D4" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>220</v>
+      </c>
+      <c r="B5" t="s">
+        <v>539</v>
+      </c>
+      <c r="D5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>605</v>
+      </c>
+      <c r="D6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>400</v>
+      </c>
+      <c r="B7" t="s">
+        <v>627</v>
+      </c>
+      <c r="D7" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>500</v>
+      </c>
+      <c r="B8" t="s">
+        <v>563</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>600</v>
+      </c>
+      <c r="B9" t="s">
+        <v>563</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>556</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>700</v>
+      </c>
+      <c r="B10" t="s">
+        <v>563</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>800</v>
+      </c>
+      <c r="B11" t="s">
+        <v>549</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>557</v>
+      </c>
+      <c r="E11">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>1500</v>
+      </c>
+      <c r="B12" t="s">
+        <v>566</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>612</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>1600</v>
+      </c>
+      <c r="B13" t="s">
+        <v>561</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>608</v>
+      </c>
+      <c r="E13">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>1700</v>
+      </c>
+      <c r="B14" t="s">
+        <v>561</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>608</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>1800</v>
+      </c>
+      <c r="B15" t="s">
+        <v>563</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>2000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>563</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>556</v>
+      </c>
+      <c r="E16">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>2400</v>
+      </c>
+      <c r="B17" t="s">
+        <v>549</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>557</v>
+      </c>
+      <c r="E17">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>2600</v>
+      </c>
+      <c r="B18" t="s">
+        <v>566</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>612</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
+      <c r="F18" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2800</v>
+      </c>
+      <c r="B19" t="s">
+        <v>563</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>556</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>2900</v>
+      </c>
+      <c r="B20" t="s">
+        <v>549</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>557</v>
+      </c>
+      <c r="E20">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>3000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>549</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>3100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>549</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>557</v>
+      </c>
+      <c r="E22">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>3500</v>
+      </c>
+      <c r="B23" t="s">
+        <v>549</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>557</v>
+      </c>
+      <c r="E23">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>3600</v>
+      </c>
+      <c r="B24" t="s">
+        <v>549</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>557</v>
+      </c>
+      <c r="E24">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>3900</v>
+      </c>
+      <c r="B25" t="s">
+        <v>549</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>557</v>
+      </c>
+      <c r="E25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>4000</v>
+      </c>
+      <c r="B26" t="s">
+        <v>567</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>4300</v>
+      </c>
+      <c r="B27" t="s">
+        <v>567</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>606</v>
+      </c>
+      <c r="E27">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>4900</v>
+      </c>
+      <c r="B28" t="s">
+        <v>567</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>606</v>
+      </c>
+      <c r="E28">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>5500</v>
+      </c>
+      <c r="B29" t="s">
+        <v>570</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>580</v>
+      </c>
+      <c r="E29">
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>5600</v>
+      </c>
+      <c r="B30" t="s">
+        <v>568</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>558</v>
+      </c>
+      <c r="E30">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>5700</v>
+      </c>
+      <c r="B31" t="s">
+        <v>567</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>606</v>
+      </c>
+      <c r="E31">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>6000</v>
+      </c>
+      <c r="B32" t="s">
+        <v>567</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>6500</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>6600</v>
+      </c>
+      <c r="B34" t="s">
+        <v>550</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>6900</v>
+      </c>
+      <c r="B35" t="s">
+        <v>567</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>7000</v>
+      </c>
+      <c r="B36" t="s">
+        <v>568</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>558</v>
+      </c>
+      <c r="E36">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>7300</v>
+      </c>
+      <c r="B37" t="s">
+        <v>567</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>606</v>
+      </c>
+      <c r="E37">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>7400</v>
+      </c>
+      <c r="B38" t="s">
+        <v>567</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>606</v>
+      </c>
+      <c r="E38">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>7500</v>
+      </c>
+      <c r="B39" t="s">
+        <v>596</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>610</v>
+      </c>
+      <c r="E39">
+        <v>80</v>
+      </c>
+      <c r="F39" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>7600</v>
+      </c>
+      <c r="B40" t="s">
+        <v>568</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>558</v>
+      </c>
+      <c r="E40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>8800</v>
+      </c>
+      <c r="B41" t="s">
+        <v>597</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>607</v>
+      </c>
+      <c r="F41" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>11600</v>
+      </c>
+      <c r="B42" t="s">
+        <v>598</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>611</v>
+      </c>
+      <c r="E42">
+        <v>140</v>
+      </c>
+      <c r="F42" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>11700</v>
+      </c>
+      <c r="B43" t="s">
+        <v>561</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>608</v>
+      </c>
+      <c r="E43">
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>14600</v>
+      </c>
+      <c r="B44" t="s">
+        <v>568</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>14900</v>
+      </c>
+      <c r="B45" t="s">
+        <v>567</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>606</v>
+      </c>
+      <c r="E45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>15600</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>15800</v>
+      </c>
+      <c r="B47" t="s">
+        <v>568</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>17800</v>
+      </c>
+      <c r="B48" t="s">
+        <v>643</v>
+      </c>
+      <c r="C48" t="s">
+        <v>576</v>
+      </c>
+      <c r="D48" t="s">
+        <v>583</v>
+      </c>
+      <c r="E48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>20000</v>
+      </c>
+      <c r="B49" t="s">
+        <v>601</v>
+      </c>
+      <c r="C49" t="s">
+        <v>576</v>
+      </c>
+      <c r="D49" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>28300</v>
+      </c>
+      <c r="B50" t="s">
+        <v>567</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>606</v>
+      </c>
+      <c r="E50">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>30700</v>
+      </c>
+      <c r="B51" t="s">
+        <v>602</v>
+      </c>
+      <c r="C51" t="s">
+        <v>576</v>
+      </c>
+      <c r="D51" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>30900</v>
+      </c>
+      <c r="B52" t="s">
+        <v>643</v>
+      </c>
+      <c r="C52" t="s">
+        <v>575</v>
+      </c>
+      <c r="D52" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>31100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>644</v>
+      </c>
+      <c r="C53" t="s">
+        <v>576</v>
+      </c>
+      <c r="D53" t="s">
+        <v>583</v>
+      </c>
+      <c r="E53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>31300</v>
+      </c>
+      <c r="B54" t="s">
+        <v>604</v>
+      </c>
+      <c r="D54" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>31400</v>
+      </c>
+      <c r="B55" t="s">
+        <v>604</v>
+      </c>
+      <c r="D55" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>32200</v>
+      </c>
+      <c r="B56" t="s">
+        <v>603</v>
+      </c>
+      <c r="C56" t="s">
+        <v>575</v>
+      </c>
+      <c r="D56" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>32300</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>629</v>
+      </c>
+      <c r="B58" t="s">
+        <v>643</v>
+      </c>
+      <c r="C58" t="s">
+        <v>576</v>
+      </c>
+      <c r="D58" t="s">
+        <v>583</v>
+      </c>
+      <c r="E58">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>628</v>
+      </c>
+      <c r="B59" t="s">
+        <v>549</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>557</v>
+      </c>
+      <c r="E59">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>559</v>
+      </c>
+      <c r="D60" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>559</v>
+      </c>
+      <c r="D61" t="s">
+        <v>592</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F61" xr:uid="{5A1DA6AB-23E9-4D76-A1A2-206FECFD3B18}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
+      <sortCondition ref="A1:A61"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
+    <sortCondition ref="A3:A60"/>
+  </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12549,6 +12587,29 @@
       <c r="F16" s="33"/>
       <c r="G16" s="38" t="s">
         <v>830</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="199.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>831</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>832</v>
+      </c>
+      <c r="E17" s="33">
+        <v>3021</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>833</v>
+      </c>
+      <c r="G17" s="53" t="s">
+        <v>835</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[7300] Add AI Ut, Bkl
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479D96D2-1F13-4DB9-8DCF-0FC07186C08E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782CAC66-424C-4A94-99E7-7E8ECA5A11E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8115" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -649,7 +649,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="837">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3541,7 +3541,25 @@
 - 6001 Utvr
 - 3901 Utvr
 - 6000 Utln-Ut20
-- TODO cUtUto18</t>
+- cUtUto18 Utza-Amf
+Ut:
+- 2001/8800/8801? Ut12
+- 3501 Ut18
+- 4900/5701 Ut1
+- 5600/5601 Ut4
+- 6901 Ut21
+- 28300/28301 Ut2</t>
+  </si>
+  <si>
+    <t>Ut-Bkl:
+- 3101 Ut19
+- 7401 Ut15
+- 421/c Utzl-Ut*
+- 801 Mas-Utzl*
+- 101/121/221 Mas
+- 3101 Bkl-Mas
+- 7301 Bkla-Mas
+- 3901 Bkl</t>
   </si>
 </sst>
 </file>
@@ -3693,7 +3711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3801,12 +3819,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -11195,8 +11207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D537A-268C-4038-9C7F-D98434B08E7D}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12155,11 +12167,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12571,6 +12583,9 @@
       <c r="B15" s="52" t="s">
         <v>827</v>
       </c>
+      <c r="D15" s="33" t="s">
+        <v>710</v>
+      </c>
       <c r="E15" s="52">
         <v>3022</v>
       </c>
@@ -12583,21 +12598,25 @@
     </row>
     <row r="16" spans="1:11" ht="114" x14ac:dyDescent="0.45">
       <c r="B16" s="52"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="52"/>
       <c r="F16" s="33"/>
       <c r="G16" s="38" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A17" s="32" t="s">
         <v>636</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>831</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="38" t="s">
         <v>832</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>710</v>
       </c>
       <c r="E17" s="33">
         <v>3021</v>
@@ -12605,12 +12624,26 @@
       <c r="F17" s="40" t="s">
         <v>833</v>
       </c>
-      <c r="G17" s="53" t="s">
+      <c r="G17" s="38" t="s">
         <v>835</v>
       </c>
-      <c r="H17" s="54" t="s">
+      <c r="H17" s="39" t="s">
         <v>834</v>
       </c>
+      <c r="I17" s="39" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
['96/'97] Creatieve oplossing 600/601 Rsd...
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A3F363-7483-47E2-94EE-1AA776D0FA42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92119AD2-BEB5-4F59-9348-5B1CFC024D30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6645" yWindow="4260" windowWidth="14400" windowHeight="7485" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="874">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3738,9 +3738,6 @@
     <t>Spits</t>
   </si>
   <si>
-    <t>IRM, Mat 54(?)</t>
-  </si>
-  <si>
     <t>Mat 64</t>
   </si>
   <si>
@@ -3781,6 +3778,12 @@
   </si>
   <si>
     <t>4x als spitstrein 'SpitsPendel', onregelmatig!</t>
+  </si>
+  <si>
+    <t>NMBS Varkensneus, Duikbril</t>
+  </si>
+  <si>
+    <t>IRM</t>
   </si>
 </sst>
 </file>
@@ -13743,14 +13746,14 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="6.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.73046875" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.19921875" customWidth="1"/>
     <col min="6" max="6" width="19.3984375" customWidth="1"/>
     <col min="7" max="7" width="13.59765625" customWidth="1"/>
   </cols>
@@ -13800,7 +13803,7 @@
         <v>855</v>
       </c>
       <c r="C3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -13821,6 +13824,9 @@
       <c r="C5" t="s">
         <v>852</v>
       </c>
+      <c r="D5" t="s">
+        <v>872</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="54">
@@ -13830,7 +13836,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -13909,7 +13915,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>858</v>
+        <v>873</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -13952,7 +13958,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -13963,7 +13969,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -13974,7 +13980,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
@@ -13985,10 +13991,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>860</v>
+      </c>
+      <c r="D22" t="s">
         <v>861</v>
-      </c>
-      <c r="D22" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -13996,7 +14002,7 @@
         <v>9300</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C23" t="s">
         <v>551</v>
@@ -14018,7 +14024,7 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
@@ -14029,7 +14035,7 @@
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D26" t="s">
         <v>690</v>
@@ -14056,7 +14062,7 @@
         <v>15400</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C29" t="s">
         <v>857</v>
@@ -14070,7 +14076,7 @@
         <v>855</v>
       </c>
       <c r="C30" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
@@ -14081,7 +14087,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
@@ -14092,7 +14098,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
['96/'97] eerste consists compleet ZWNL 1996/97
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8729375-3930-4C3C-903C-3921CC56C4BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B38194-29CB-4FBC-B0B7-76A4E33282D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13973,7 +13973,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14091,7 +14091,7 @@
       <c r="G5" t="s">
         <v>916</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="42" t="s">
         <v>928</v>
       </c>
     </row>
@@ -14137,7 +14137,7 @@
       <c r="F7" t="s">
         <v>871</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="42" t="s">
         <v>587</v>
       </c>
     </row>
@@ -14352,7 +14352,7 @@
       <c r="G17" t="s">
         <v>909</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="42" t="s">
         <v>926</v>
       </c>
     </row>
@@ -14478,7 +14478,7 @@
       <c r="F23" t="s">
         <v>919</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="42" t="s">
         <v>558</v>
       </c>
     </row>
@@ -14498,7 +14498,7 @@
       <c r="F24" t="s">
         <v>923</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="42" t="s">
         <v>609</v>
       </c>
     </row>
@@ -14512,6 +14512,7 @@
       <c r="E25" t="s">
         <v>862</v>
       </c>
+      <c r="I25" s="42"/>
     </row>
     <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" s="55">
@@ -14526,6 +14527,7 @@
       <c r="F26" t="s">
         <v>690</v>
       </c>
+      <c r="I26" s="42"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="54">
@@ -14543,7 +14545,7 @@
       <c r="F27" t="s">
         <v>924</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="42" t="s">
         <v>609</v>
       </c>
     </row>
@@ -14563,7 +14565,7 @@
       <c r="F28" t="s">
         <v>873</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="42" t="s">
         <v>609</v>
       </c>
     </row>
@@ -14577,6 +14579,7 @@
       <c r="E29" t="s">
         <v>857</v>
       </c>
+      <c r="I29" s="42"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="54">
@@ -14597,7 +14600,7 @@
       <c r="G30" t="s">
         <v>914</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="42" t="s">
         <v>609</v>
       </c>
     </row>

</xml_diff>

<commit_message>
['97/'97] drgl en consists
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B38194-29CB-4FBC-B0B7-76A4E33282D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA73373-5827-497B-9EC3-2DB1646CB815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consists" sheetId="6" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="ZWNL-Treinseries 2021" sheetId="11" r:id="rId3"/>
     <sheet name="HvN-Treinseries 2022" sheetId="18" r:id="rId4"/>
     <sheet name="HvN-Treinseries 2021" sheetId="10" r:id="rId5"/>
-    <sheet name="Scenarios" sheetId="14" r:id="rId6"/>
-    <sheet name="Vervoerders" sheetId="7" r:id="rId7"/>
-    <sheet name="ICRm" sheetId="17" r:id="rId8"/>
-    <sheet name="ZWNL-Treinseries 96-97" sheetId="19" r:id="rId9"/>
+    <sheet name="ZWNL-Treinseries 96-97" sheetId="19" r:id="rId6"/>
+    <sheet name="Scenarios" sheetId="14" r:id="rId7"/>
+    <sheet name="Vervoerders" sheetId="7" r:id="rId8"/>
+    <sheet name="ICRm" sheetId="17" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Consists!$A$3:$I$3</definedName>
@@ -29,7 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HvN-Treinseries 2021'!$A$1:$F$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'HvN-Treinseries 2022'!$A$1:$F$122</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL-Treinseries 2021'!$A$1:$F$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'ZWNL-Treinseries 96-97'!$A$1:$J$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'ZWNL-Treinseries 96-97'!$A$1:$J$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -597,6 +597,90 @@
     <author>Tom</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AA444BDC-CF0D-4F74-A5D0-58801DCFDFA6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Groen: in drgl
+Rood: niet voor quickdrive, mogelijk wel als los scenario!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{48E94B4C-53B9-4DD3-A577-B7B5E11AC5C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+geen ICR meer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{859BDA5C-2888-4004-9AB2-0092C0487D4C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+vrijwel gehele dienst
+geen ICR meer</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
     <comment ref="G2" authorId="0" shapeId="0" xr:uid="{73E91D31-354C-4F1A-913F-AA2C421A3352}">
       <text>
         <r>
@@ -650,92 +734,8 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Tom</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AA444BDC-CF0D-4F74-A5D0-58801DCFDFA6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Groen: in drgl
-Rood: niet voor quickdrive, mogelijk wel als los scenario!</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{859BDA5C-2888-4004-9AB2-0092C0487D4C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-vrijwel gehele dienst
-geen ICR meer</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{48E94B4C-53B9-4DD3-A577-B7B5E11AC5C2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-geen ICR meer</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2354" uniqueCount="932">
   <si>
     <t>Zuid-West Nederland</t>
   </si>
@@ -3998,6 +3998,41 @@
   </si>
   <si>
     <t>Custom 3, Passenger Regional</t>
+  </si>
+  <si>
+    <t>5400 Bd-Rtd</t>
+  </si>
+  <si>
+    <t>- Bd
+- Ddr</t>
+  </si>
+  <si>
+    <t>Bd:
+- cZlwBd105
+Bd - Ddr:
+- cZlwBd107 Bdpb
+- 1901 Zonzeel
+- cZwdZlw101 Zlw
+- 4601 Wld
+- cZwdZlw103 Ddzd-Wld
+- 5403 Ddr-Ddzd
+- 2101 Ddr
+Ddr:
+- 4699 Ddr42
+- 7101/7102 Ddr15
+Ddr - Rtd:
+- 1501 Zwd
+- 9300 Kfhn
+- 5401 Brd-Zwd
+- 2401 Rtz
+- 1901 Rtb
+- c in pad 15400 Rtd
+Rtd:
+- 2000/2001 Rtd13
+- 4000/4001 Rtd16
+- 4201/4202 Rtd2
+- 5100/5103 Rtd9
+- 5403 Rtd4</t>
   </si>
 </sst>
 </file>
@@ -12622,12 +12657,681 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
-  <dimension ref="A1:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCE6247-AFF8-4753-B6F2-6C865F6727C8}">
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="6.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.265625" style="56" customWidth="1"/>
+    <col min="4" max="4" width="16.265625" style="56" customWidth="1"/>
+    <col min="5" max="5" width="8.86328125" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" customWidth="1"/>
+    <col min="7" max="7" width="40.3984375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.06640625" customWidth="1"/>
+    <col min="9" max="9" width="36.3984375" customWidth="1"/>
+    <col min="10" max="10" width="13.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>851</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>880</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>878</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>879</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="55">
+        <v>280</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E2" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="55">
+        <v>362</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E3" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="54">
+        <v>500</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>881</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>883</v>
+      </c>
+      <c r="F4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G4" t="s">
+        <v>913</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="54">
+        <v>600</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>882</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>884</v>
+      </c>
+      <c r="E5" t="s">
+        <v>852</v>
+      </c>
+      <c r="F5" t="s">
+        <v>871</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="58">
+        <v>1500</v>
+      </c>
+      <c r="B6" s="59">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>881</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>885</v>
+      </c>
+      <c r="E6" t="s">
+        <v>867</v>
+      </c>
+      <c r="F6" t="s">
+        <v>918</v>
+      </c>
+      <c r="G6" t="s">
+        <v>912</v>
+      </c>
+      <c r="I6" s="42" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="54">
+        <v>1700</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>881</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>886</v>
+      </c>
+      <c r="F7" t="s">
+        <v>563</v>
+      </c>
+      <c r="G7" t="s">
+        <v>872</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="58">
+        <v>1900</v>
+      </c>
+      <c r="B8" s="59">
+        <v>1</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>882</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>887</v>
+      </c>
+      <c r="F8" t="s">
+        <v>921</v>
+      </c>
+      <c r="G8" t="s">
+        <v>915</v>
+      </c>
+      <c r="I8" s="42" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="54">
+        <v>2000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>882</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>888</v>
+      </c>
+      <c r="F9" t="s">
+        <v>872</v>
+      </c>
+      <c r="I9" s="42" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="58">
+        <v>2100</v>
+      </c>
+      <c r="B10" s="59">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>881</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>889</v>
+      </c>
+      <c r="E10" t="s">
+        <v>853</v>
+      </c>
+      <c r="F10" t="s">
+        <v>908</v>
+      </c>
+      <c r="G10" t="s">
+        <v>907</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="58">
+        <v>2400</v>
+      </c>
+      <c r="B11" s="59">
+        <v>1</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>881</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>890</v>
+      </c>
+      <c r="E11" t="s">
+        <v>854</v>
+      </c>
+      <c r="F11" t="s">
+        <v>875</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="54">
+        <v>3400</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>882</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>891</v>
+      </c>
+      <c r="F12" t="s">
+        <v>876</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="55">
+        <v>3500</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>857</v>
+      </c>
+      <c r="F13" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="58">
+        <v>3600</v>
+      </c>
+      <c r="B14" s="59">
+        <v>2</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>882</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="F14" t="s">
+        <v>917</v>
+      </c>
+      <c r="G14" t="s">
+        <v>909</v>
+      </c>
+      <c r="I14" s="42" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="54">
+        <v>4000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>893</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>894</v>
+      </c>
+      <c r="F15" t="s">
+        <v>919</v>
+      </c>
+      <c r="I15" s="42" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="54">
+        <v>4100</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>893</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>895</v>
+      </c>
+      <c r="F16" t="s">
+        <v>923</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="54">
+        <v>4200</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>893</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>896</v>
+      </c>
+      <c r="F17" t="s">
+        <v>924</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="58">
+        <v>4600</v>
+      </c>
+      <c r="B18" s="59">
+        <v>1</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>893</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>897</v>
+      </c>
+      <c r="F18" t="s">
+        <v>906</v>
+      </c>
+      <c r="G18" t="s">
+        <v>911</v>
+      </c>
+      <c r="I18" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="54">
+        <v>5100</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>893</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>898</v>
+      </c>
+      <c r="F19" t="s">
+        <v>873</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="58">
+        <v>5400</v>
+      </c>
+      <c r="B20" s="59">
+        <v>2</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>882</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>743</v>
+      </c>
+      <c r="E20" t="s">
+        <v>868</v>
+      </c>
+      <c r="F20" t="s">
+        <v>920</v>
+      </c>
+      <c r="G20" t="s">
+        <v>916</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="54">
+        <v>7100</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>893</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>899</v>
+      </c>
+      <c r="E21" t="s">
+        <v>858</v>
+      </c>
+      <c r="F21" s="57" t="s">
+        <v>922</v>
+      </c>
+      <c r="G21" t="s">
+        <v>922</v>
+      </c>
+      <c r="I21" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="55">
+        <v>7500</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>859</v>
+      </c>
+      <c r="F22" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="58">
+        <v>9300</v>
+      </c>
+      <c r="B23" s="59" t="s">
+        <v>861</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>900</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>901</v>
+      </c>
+      <c r="E23" t="s">
+        <v>551</v>
+      </c>
+      <c r="F23" t="s">
+        <v>551</v>
+      </c>
+      <c r="I23" s="42" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="54">
+        <v>9800</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>893</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>902</v>
+      </c>
+      <c r="F24" t="s">
+        <v>874</v>
+      </c>
+      <c r="I24" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="55">
+        <v>10500</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>862</v>
+      </c>
+      <c r="I25" s="42"/>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="55">
+        <v>13600</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>869</v>
+      </c>
+      <c r="F26" t="s">
+        <v>690</v>
+      </c>
+      <c r="I26" s="42"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="54">
+        <v>14000</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>893</v>
+      </c>
+      <c r="D27" s="56" t="s">
+        <v>903</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>914</v>
+      </c>
+      <c r="G27" t="s">
+        <v>914</v>
+      </c>
+      <c r="I27" s="42" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="58">
+        <v>14600</v>
+      </c>
+      <c r="B28" s="59">
+        <v>1</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>893</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>904</v>
+      </c>
+      <c r="F28" t="s">
+        <v>906</v>
+      </c>
+      <c r="G28" t="s">
+        <v>910</v>
+      </c>
+      <c r="I28" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="55">
+        <v>15400</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="E29" t="s">
+        <v>857</v>
+      </c>
+      <c r="I29" s="42"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="54">
+        <v>31000</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="D30" s="56" t="s">
+        <v>905</v>
+      </c>
+      <c r="E30" t="s">
+        <v>864</v>
+      </c>
+      <c r="F30" t="s">
+        <v>872</v>
+      </c>
+      <c r="I30" s="42" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="55">
+        <v>31200</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="55">
+        <v>31800</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>865</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J13" xr:uid="{12137E18-5C8A-4092-B20B-35DFE2ACBAA4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J30">
+      <sortCondition ref="A1:A13"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD62907E-A64D-455B-B56E-7C77875AE798}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13164,6 +13868,23 @@
         <v>847</v>
       </c>
     </row>
+    <row r="21" spans="1:10" ht="370.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="32" t="s">
+        <v>747</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>929</v>
+      </c>
+      <c r="E21" s="33">
+        <v>2096</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>930</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>931</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{943F34A2-1BA5-4D1C-81A8-62EE384FF261}"/>
@@ -13174,7 +13895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FB34A4-CC11-43B7-A0E1-7E36604CB0F9}">
   <dimension ref="A1:D36"/>
   <sheetViews>
@@ -13666,7 +14387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8629E7C5-043E-4A29-9B03-D70DB32336F4}">
   <dimension ref="A1:I23"/>
   <sheetViews>
@@ -13966,673 +14687,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCE6247-AFF8-4753-B6F2-6C865F6727C8}">
-  <dimension ref="A1:J32"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="6.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.265625" style="56" customWidth="1"/>
-    <col min="4" max="4" width="16.265625" style="56" customWidth="1"/>
-    <col min="5" max="5" width="25.73046875" customWidth="1"/>
-    <col min="6" max="6" width="24.19921875" customWidth="1"/>
-    <col min="7" max="7" width="40.3984375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.06640625" customWidth="1"/>
-    <col min="9" max="9" width="36.3984375" customWidth="1"/>
-    <col min="10" max="10" width="13.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="B1" s="53" t="s">
-        <v>851</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>880</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>877</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>849</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>878</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>879</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="55">
-        <v>280</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="E2" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55">
-        <v>362</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="E3" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="58">
-        <v>1500</v>
-      </c>
-      <c r="B4" s="59">
-        <v>1</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>881</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>885</v>
-      </c>
-      <c r="E4" t="s">
-        <v>867</v>
-      </c>
-      <c r="F4" t="s">
-        <v>918</v>
-      </c>
-      <c r="G4" t="s">
-        <v>912</v>
-      </c>
-      <c r="I4" s="42" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="58">
-        <v>5400</v>
-      </c>
-      <c r="B5" s="59">
-        <v>2</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>882</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>743</v>
-      </c>
-      <c r="E5" t="s">
-        <v>868</v>
-      </c>
-      <c r="F5" t="s">
-        <v>920</v>
-      </c>
-      <c r="G5" t="s">
-        <v>916</v>
-      </c>
-      <c r="I5" s="42" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="58">
-        <v>9300</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>861</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>900</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>901</v>
-      </c>
-      <c r="E6" t="s">
-        <v>551</v>
-      </c>
-      <c r="F6" t="s">
-        <v>551</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="54">
-        <v>600</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>882</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>884</v>
-      </c>
-      <c r="E7" t="s">
-        <v>852</v>
-      </c>
-      <c r="F7" t="s">
-        <v>871</v>
-      </c>
-      <c r="I7" s="42" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="54">
-        <v>3400</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="56" t="s">
-        <v>882</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>891</v>
-      </c>
-      <c r="F8" t="s">
-        <v>876</v>
-      </c>
-      <c r="I8" s="42" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="58">
-        <v>4600</v>
-      </c>
-      <c r="B9" s="59">
-        <v>1</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>893</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>897</v>
-      </c>
-      <c r="F9" t="s">
-        <v>906</v>
-      </c>
-      <c r="G9" t="s">
-        <v>911</v>
-      </c>
-      <c r="I9" s="42" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="54">
-        <v>7100</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="56" t="s">
-        <v>893</v>
-      </c>
-      <c r="D10" s="56" t="s">
-        <v>899</v>
-      </c>
-      <c r="E10" t="s">
-        <v>858</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>922</v>
-      </c>
-      <c r="G10" t="s">
-        <v>922</v>
-      </c>
-      <c r="I10" s="42" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="54">
-        <v>9800</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="56" t="s">
-        <v>893</v>
-      </c>
-      <c r="D11" s="56" t="s">
-        <v>902</v>
-      </c>
-      <c r="F11" t="s">
-        <v>874</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="58">
-        <v>14600</v>
-      </c>
-      <c r="B12" s="59">
-        <v>1</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>893</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>904</v>
-      </c>
-      <c r="F12" t="s">
-        <v>906</v>
-      </c>
-      <c r="G12" t="s">
-        <v>910</v>
-      </c>
-      <c r="I12" s="42" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="55">
-        <v>3500</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>857</v>
-      </c>
-      <c r="F13" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="54">
-        <v>2000</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>882</v>
-      </c>
-      <c r="D14" s="56" t="s">
-        <v>888</v>
-      </c>
-      <c r="F14" t="s">
-        <v>872</v>
-      </c>
-      <c r="I14" s="42" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="58">
-        <v>2100</v>
-      </c>
-      <c r="B15" s="59">
-        <v>1</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>881</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>889</v>
-      </c>
-      <c r="E15" t="s">
-        <v>853</v>
-      </c>
-      <c r="F15" t="s">
-        <v>908</v>
-      </c>
-      <c r="G15" t="s">
-        <v>907</v>
-      </c>
-      <c r="I15" s="42" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="54">
-        <v>31000</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="D16" s="56" t="s">
-        <v>905</v>
-      </c>
-      <c r="E16" t="s">
-        <v>864</v>
-      </c>
-      <c r="F16" t="s">
-        <v>872</v>
-      </c>
-      <c r="I16" s="42" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="58">
-        <v>3600</v>
-      </c>
-      <c r="B17" s="59">
-        <v>2</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>882</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>892</v>
-      </c>
-      <c r="F17" t="s">
-        <v>917</v>
-      </c>
-      <c r="G17" t="s">
-        <v>909</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="54">
-        <v>500</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="56" t="s">
-        <v>881</v>
-      </c>
-      <c r="D18" s="56" t="s">
-        <v>883</v>
-      </c>
-      <c r="F18" t="s">
-        <v>563</v>
-      </c>
-      <c r="G18" t="s">
-        <v>913</v>
-      </c>
-      <c r="I18" s="42" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A19" s="54">
-        <v>1700</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="56" t="s">
-        <v>881</v>
-      </c>
-      <c r="D19" s="56" t="s">
-        <v>886</v>
-      </c>
-      <c r="F19" t="s">
-        <v>563</v>
-      </c>
-      <c r="G19" t="s">
-        <v>872</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A20" s="58">
-        <v>1900</v>
-      </c>
-      <c r="B20" s="59">
-        <v>1</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>882</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>887</v>
-      </c>
-      <c r="F20" t="s">
-        <v>921</v>
-      </c>
-      <c r="G20" t="s">
-        <v>915</v>
-      </c>
-      <c r="I20" s="42" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A21" s="58">
-        <v>2400</v>
-      </c>
-      <c r="B21" s="59">
-        <v>1</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>881</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>890</v>
-      </c>
-      <c r="E21" t="s">
-        <v>854</v>
-      </c>
-      <c r="F21" t="s">
-        <v>875</v>
-      </c>
-      <c r="I21" s="42" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="55">
-        <v>7500</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>859</v>
-      </c>
-      <c r="F22" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A23" s="54">
-        <v>4000</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="56" t="s">
-        <v>893</v>
-      </c>
-      <c r="D23" s="56" t="s">
-        <v>894</v>
-      </c>
-      <c r="F23" t="s">
-        <v>919</v>
-      </c>
-      <c r="I23" s="42" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A24" s="54">
-        <v>4100</v>
-      </c>
-      <c r="B24" s="1">
-        <v>2</v>
-      </c>
-      <c r="C24" s="56" t="s">
-        <v>893</v>
-      </c>
-      <c r="D24" s="56" t="s">
-        <v>895</v>
-      </c>
-      <c r="F24" t="s">
-        <v>923</v>
-      </c>
-      <c r="I24" s="42" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="55">
-        <v>10500</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>862</v>
-      </c>
-      <c r="I25" s="42"/>
-    </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="55">
-        <v>13600</v>
-      </c>
-      <c r="B26" s="1">
-        <v>2</v>
-      </c>
-      <c r="E26" t="s">
-        <v>869</v>
-      </c>
-      <c r="F26" t="s">
-        <v>690</v>
-      </c>
-      <c r="I26" s="42"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="54">
-        <v>4200</v>
-      </c>
-      <c r="B27" s="1">
-        <v>2</v>
-      </c>
-      <c r="C27" s="56" t="s">
-        <v>893</v>
-      </c>
-      <c r="D27" s="56" t="s">
-        <v>896</v>
-      </c>
-      <c r="F27" t="s">
-        <v>924</v>
-      </c>
-      <c r="I27" s="42" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" s="54">
-        <v>5100</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2</v>
-      </c>
-      <c r="C28" s="56" t="s">
-        <v>893</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>898</v>
-      </c>
-      <c r="F28" t="s">
-        <v>873</v>
-      </c>
-      <c r="I28" s="42" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="55">
-        <v>15400</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>863</v>
-      </c>
-      <c r="E29" t="s">
-        <v>857</v>
-      </c>
-      <c r="I29" s="42"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A30" s="54">
-        <v>14000</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="56" t="s">
-        <v>893</v>
-      </c>
-      <c r="D30" s="56" t="s">
-        <v>903</v>
-      </c>
-      <c r="F30" s="57" t="s">
-        <v>914</v>
-      </c>
-      <c r="G30" t="s">
-        <v>914</v>
-      </c>
-      <c r="I30" s="42" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="55">
-        <v>31200</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="55">
-        <v>31800</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>865</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:J13" xr:uid="{12137E18-5C8A-4092-B20B-35DFE2ACBAA4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J30">
-      <sortCondition ref="I1:I13"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>